<commit_message>
Anatest point enable for az comp added
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab2\Documents\projects\IVM6311\IVM6311ATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab2\Documents\projects\IVM6311\IVM6311ATE-flavio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01D72CD-9890-4434-B747-10D58A7AAF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408706AE-8FAC-4227-B198-CE393BEFDF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="435">
   <si>
     <t>Revision</t>
   </si>
@@ -40323,15 +40323,6 @@
     <t>4-10</t>
   </si>
   <si>
-    <t xml:space="preserve">2nd STG Current </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st STG Current </t>
-  </si>
-  <si>
-    <t>Ground AZCOMP</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="16"/>
@@ -40932,7 +40923,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Run_startup </t>
+      <t xml:space="preserve">Run__startup </t>
     </r>
     <r>
       <rPr>
@@ -40951,7 +40942,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0xFE_0x01</t>
+      <t xml:space="preserve">0xFE_0x01 </t>
     </r>
     <r>
       <rPr>
@@ -40960,8 +40951,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> "Select page 1"  
-</t>
+      <t>"Select page 1"</t>
     </r>
     <r>
       <rPr>
@@ -40970,7 +40960,8 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">0x17_0x02 </t>
+      <t xml:space="preserve">  
+0x17_0x02 </t>
     </r>
     <r>
       <rPr>
@@ -41027,7 +41018,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">0x10_0x08  </t>
+      <t xml:space="preserve">0x10_0x08 </t>
     </r>
     <r>
       <rPr>
@@ -41036,7 +41027,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">"Force ref_sdwn_b_dis_m"
+      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
 </t>
     </r>
     <r>
@@ -41065,7 +41056,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">0x1A_0x00 </t>
+      <t xml:space="preserve">0x1A_0x0D </t>
     </r>
     <r>
       <rPr>
@@ -41074,7 +41065,8 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"3rd STG Current analog test point</t>
+      <t xml:space="preserve">"OUTN_INT_PRT analog test point"
+</t>
     </r>
     <r>
       <rPr>
@@ -41083,8 +41075,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">"
-0xFE_0x00 </t>
+      <t xml:space="preserve">0xFE_0x00 </t>
     </r>
     <r>
       <rPr>
@@ -41094,26 +41085,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">"Return page 0"
- "Measure current between VBAT and SDWN pin"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Current__SDWN  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                                                                                                        </t>
+</t>
     </r>
   </si>
   <si>
@@ -41124,7 +41096,16 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Run_startup                                                                  
+      <t xml:space="preserve">Run__startup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                 
 </t>
     </r>
     <r>
@@ -41134,7 +41115,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0xFE_0x01</t>
+      <t xml:space="preserve">0xFE_0x01 </t>
     </r>
     <r>
       <rPr>
@@ -41143,8 +41124,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> "Select page 1"  
-</t>
+      <t>"Select page 1"</t>
     </r>
     <r>
       <rPr>
@@ -41153,7 +41133,8 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">0x17_0x02 </t>
+      <t xml:space="preserve">  
+0x17_0x02 </t>
     </r>
     <r>
       <rPr>
@@ -41172,7 +41153,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0x18_0x02</t>
+      <t xml:space="preserve">0x18_0x02 </t>
     </r>
     <r>
       <rPr>
@@ -41181,7 +41162,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> "dig_azcomp_en"
+      <t xml:space="preserve">"dig_azcomp_en"
 </t>
     </r>
     <r>
@@ -41191,7 +41172,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0x0F_0xC8</t>
+      <t xml:space="preserve">0x0F_0xC8 </t>
     </r>
     <r>
       <rPr>
@@ -41200,7 +41181,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> " force otp and mod clock on"
+      <t xml:space="preserve">" force otp and mod clock on"
 </t>
     </r>
     <r>
@@ -41210,7 +41191,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0x10_0x08</t>
+      <t xml:space="preserve">0x10_0x08 </t>
     </r>
     <r>
       <rPr>
@@ -41219,7 +41200,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  "Force ref_sdwn_b_dis_m"
+      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
 </t>
     </r>
     <r>
@@ -41229,7 +41210,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0x19_0x88</t>
+      <t xml:space="preserve">0x19_0x88  </t>
     </r>
     <r>
       <rPr>
@@ -41238,7 +41219,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">  "test analog azcomp enable"
+      <t xml:space="preserve">"test analog azcomp enable"
 </t>
     </r>
     <r>
@@ -41248,7 +41229,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0x1A_0x01</t>
+      <t xml:space="preserve">0x1A_0x0E </t>
     </r>
     <r>
       <rPr>
@@ -41257,7 +41238,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> "2rd STG Current analog test point"
+      <t xml:space="preserve">"OUTP_EXT_PRT analog test point"
 </t>
     </r>
     <r>
@@ -41267,7 +41248,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0xFE_0x00</t>
+      <t xml:space="preserve">0xFE_0x00 </t>
     </r>
     <r>
       <rPr>
@@ -41276,1328 +41257,8 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> "Return page 0"
- "Measure current between VBAT and SDWN pin"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Current__SDWN  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run_startup
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 1"  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"1rd STG Current analog test point"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">"Return page 0"
- "Measure current between VBAT and SDWN pin"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Current__SDWN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run__startup </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Select page 1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  
-0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x03 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"GND analog test point"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Return page 0"
- "Measure Voltage between SDWN pin and GND"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run__startup </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Select page 1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  
-0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x0B </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"OUTN_EXT_PRT analog test point"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Return page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Force__OUTP__2V   
-Force__OUTN__2V   
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Measure Voltage between SDWN pin and GND, it should be 2V"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run__startup </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Select page 1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  
-0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x0C </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"OUTP_EXT_PRT analog test point"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Return page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Force__OUTP__2V   
-Force__OUTN__2V   
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Measure Voltage between SDWN pin and GND, it should be 2V"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run__startup </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Select page 1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  
-0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x0D </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"OUTN_INT_PRT analog test point"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Return page 0"
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run__startup </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Select page 1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  
-0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x0E </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"OUTP_EXT_PRT analog test point"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Return page 0"
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run__startup </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Select page 1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  
-0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x0F </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"VCM_AVDD analog test point"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Return page 0"
- "Measure Voltage between SDWN pin and GND, you should measure VBAT/2"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
+</t>
     </r>
   </si>
   <si>
@@ -42614,9 +41275,6 @@
   </si>
   <si>
     <t>Startup</t>
-  </si>
-  <si>
-    <t>DACPA_tourn_on_wo_calibration</t>
   </si>
   <si>
     <t>Procedura_Maurizio</t>
@@ -42647,46 +41305,6 @@
   </si>
   <si>
     <t>BOOST_FORCE_VBSO19V</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00 "Select page 0"
-0x13[4]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Disable authomatic calibration at power up"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Play, speaker enable"</t>
-    </r>
   </si>
   <si>
     <t>Procedura per consentire la misura dell'offset in ANALOG_IN, visto che i DAC non sono abilitati di default  per applicare la parola di correzione</t>
@@ -43618,6 +42236,1432 @@
   </si>
   <si>
     <t>OUT_TEST_FRO_VVCO</t>
+  </si>
+  <si>
+    <t>3rd_STG_Current</t>
+  </si>
+  <si>
+    <t>2nd_STG_Current</t>
+  </si>
+  <si>
+    <t>Ground_AZCOMP</t>
+  </si>
+  <si>
+    <t>1st_STG_Current</t>
+  </si>
+  <si>
+    <t>2V</t>
+  </si>
+  <si>
+    <t>Enable_Ana_Testpoint_AZ_comp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8
+0x10_0x08
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">FORCE__SDWN__OPEN
+0x19_0x88 "Enable reference analog test"
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run__startup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  
+0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x0B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"OUTN_EXT_PRT analog test point"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Force__OUTP__2V   
+Force__OUTN__2V   
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Measure Voltage between SDWN pin and GND, it should be 2V"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run__startup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  
+0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x0C </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"OUTP_EXT_PRT analog test point"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Force__OUTP__2V   
+Force__OUTN__2V   
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Measure Voltage between SDWN pin and GND, it should be 2V"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run__startup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  
+0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x0F </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"VCM_AVDD analog test point"
+ "Measure Voltage between SDWN pin and GND, you should measure VBAT/2"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run_startup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"3rd STG Current analog test point</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Measure current between VBAT and SDWN pin"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Current__SDWN  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                                                        </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run_startup                                                                  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x18_0x02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x0F_0xC8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> " force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x10_0x08</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19_0x88</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1A_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "2rd STG Current analog test point"
+"Measure current between VBAT and SDWN pin"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Current__SDWN  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run_startup
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Select page 1"  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"1rd STG Current analog test point"
+"Measure current between VBAT and SDWN pin"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Current__SDWN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run__startup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  
+0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x03 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"GND analog test point"
+"Measure Voltage between SDWN pin and GND"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -45309,6 +45353,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -45335,9 +45382,6 @@
     </xf>
     <xf numFmtId="3" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -45752,177 +45796,177 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="K6" s="58" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="58" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="23" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>401</v>
+        <v>389</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -46831,10 +46875,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="230" t="s">
-        <v>423</v>
-      </c>
-      <c r="B1" s="230"/>
+      <c r="A1" s="231" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" s="231"/>
       <c r="C1" s="9" t="s">
         <v>142</v>
       </c>
@@ -46865,10 +46909,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="231" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="230"/>
+      <c r="B3" s="231"/>
       <c r="C3" s="15" t="s">
         <v>60</v>
       </c>
@@ -46883,10 +46927,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="231" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="230"/>
+      <c r="B4" s="231"/>
       <c r="C4" s="9" t="s">
         <v>142</v>
       </c>
@@ -46901,23 +46945,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="231"/>
-      <c r="B5" s="232"/>
+      <c r="A5" s="232"/>
+      <c r="B5" s="233"/>
       <c r="C5" s="220" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="D5" s="207" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="E5" s="207" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="F5" s="223" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="233" t="s">
+      <c r="A6" s="234" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -46928,12 +46972,12 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="F6" s="67"/>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="233"/>
+      <c r="A7" s="234"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -46945,7 +46989,7 @@
       <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="233"/>
+      <c r="A8" s="234"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -46961,7 +47005,7 @@
       <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="233"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -46975,7 +47019,7 @@
       <c r="F9" s="71"/>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="233"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -47900,10 +47944,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="230" t="s">
+      <c r="A1" s="231" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="230"/>
+      <c r="B1" s="231"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -47934,10 +47978,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="231" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="230"/>
+      <c r="B3" s="231"/>
       <c r="C3" s="15" t="s">
         <v>79</v>
       </c>
@@ -47952,10 +47996,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="231" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="230"/>
+      <c r="B4" s="231"/>
       <c r="C4" s="9" t="s">
         <v>202</v>
       </c>
@@ -47970,8 +48014,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="273" x14ac:dyDescent="0.25">
-      <c r="A5" s="231"/>
-      <c r="B5" s="232"/>
+      <c r="A5" s="232"/>
+      <c r="B5" s="233"/>
       <c r="C5" s="37" t="s">
         <v>206</v>
       </c>
@@ -47986,7 +48030,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="233" t="s">
+      <c r="A6" s="234" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48004,7 +48048,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="233"/>
+      <c r="A7" s="234"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48020,7 +48064,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="233"/>
+      <c r="A8" s="234"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -48038,7 +48082,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="233"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -48054,7 +48098,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="233"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -48814,8 +48858,8 @@
   </sheetPr>
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48827,17 +48871,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="230" t="s">
+      <c r="A1" s="231" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="230"/>
+      <c r="B1" s="231"/>
       <c r="C1" s="104" t="s">
         <v>213</v>
       </c>
       <c r="D1" s="117" t="s">
-        <v>432</v>
-      </c>
-      <c r="E1" s="239" t="s">
+        <v>420</v>
+      </c>
+      <c r="E1" s="230" t="s">
         <v>214</v>
       </c>
       <c r="F1" s="129" t="s">
@@ -48859,10 +48903,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="231" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="230"/>
+      <c r="B3" s="231"/>
       <c r="C3" s="103" t="s">
         <v>20</v>
       </c>
@@ -48877,15 +48921,15 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="231" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="230"/>
+      <c r="B4" s="231"/>
       <c r="C4" s="104" t="s">
         <v>213</v>
       </c>
       <c r="D4" s="117" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="E4" s="104" t="s">
         <v>214</v>
@@ -48895,23 +48939,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="231"/>
-      <c r="B5" s="232"/>
+      <c r="A5" s="232"/>
+      <c r="B5" s="233"/>
       <c r="C5" s="210" t="s">
         <v>216</v>
       </c>
       <c r="D5" s="219" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="E5" s="210" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="F5" s="222" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="233" t="s">
+      <c r="A6" s="234" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48925,7 +48969,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="233"/>
+      <c r="A7" s="234"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48935,12 +48979,12 @@
       <c r="F7" s="131"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="233"/>
+      <c r="A8" s="234"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
       <c r="C8" s="107" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D8" s="120" t="s">
         <v>218</v>
@@ -48953,7 +48997,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="233"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -48965,7 +49009,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="233"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -49868,7 +49912,7 @@
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49885,10 +49929,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="234" t="s">
+      <c r="A1" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="234"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="17" t="s">
         <v>222</v>
       </c>
@@ -50055,10 +50099,10 @@
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="234" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="234"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="185" t="s">
         <v>20</v>
       </c>
@@ -50142,10 +50186,10 @@
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="234" t="s">
+      <c r="A4" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="234"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="65" t="s">
         <v>19</v>
       </c>
@@ -50229,8 +50273,8 @@
       </c>
     </row>
     <row r="5" spans="1:29" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="235"/>
-      <c r="B5" s="235"/>
+      <c r="A5" s="236"/>
+      <c r="B5" s="236"/>
       <c r="C5" s="226" t="s">
         <v>234</v>
       </c>
@@ -50314,7 +50358,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -50393,7 +50437,7 @@
       <c r="AC6" s="67"/>
     </row>
     <row r="7" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="236"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -50428,7 +50472,7 @@
       <c r="AC7" s="68"/>
     </row>
     <row r="8" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="236"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -50481,7 +50525,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="236"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -50560,7 +50604,7 @@
       <c r="AC9" s="71"/>
     </row>
     <row r="10" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="236"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -54102,10 +54146,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="234" t="s">
+      <c r="A1" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="234"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -54200,10 +54244,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="234" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="234"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="15" t="s">
         <v>99</v>
       </c>
@@ -54251,10 +54295,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="234" t="s">
+      <c r="A4" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="234"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="65" t="s">
         <v>278</v>
       </c>
@@ -54302,8 +54346,8 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="237"/>
-      <c r="B5" s="238"/>
+      <c r="A5" s="238"/>
+      <c r="B5" s="239"/>
       <c r="C5" s="224" t="s">
         <v>293</v>
       </c>
@@ -54351,7 +54395,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -54374,7 +54418,7 @@
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="236"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -54395,7 +54439,7 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="236"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -54440,7 +54484,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="236"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -54465,7 +54509,7 @@
       <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="236"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -56616,8 +56660,8 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56636,24 +56680,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="234" t="s">
+      <c r="A1" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="234"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="65" t="s">
         <v>64</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>68</v>
+        <v>421</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>337</v>
+        <v>422</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>338</v>
+        <v>424</v>
       </c>
       <c r="G1" s="65" t="s">
-        <v>339</v>
+        <v>423</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>114</v>
@@ -56662,16 +56706,16 @@
         <v>118</v>
       </c>
       <c r="J1" s="65" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="K1" s="65" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="L1" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M1" s="95" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
@@ -56710,10 +56754,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="234" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="234"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="64" t="s">
         <v>65</v>
       </c>
@@ -56749,24 +56793,24 @@
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A4" s="234" t="s">
+      <c r="A4" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="234"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="65" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>68</v>
+        <v>421</v>
       </c>
       <c r="E4" s="65" t="s">
-        <v>337</v>
+        <v>422</v>
       </c>
       <c r="F4" s="65" t="s">
-        <v>338</v>
+        <v>424</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>339</v>
+        <v>423</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>114</v>
@@ -56775,55 +56819,55 @@
         <v>118</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="K4" s="65" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="L4" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M4" s="95" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="238"/>
+      <c r="B5" s="238"/>
+      <c r="C5" s="211" t="s">
+        <v>340</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>431</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>432</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>433</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>434</v>
+      </c>
+      <c r="H5" s="56" t="s">
+        <v>428</v>
+      </c>
+      <c r="I5" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="J5" s="56" t="s">
+        <v>341</v>
+      </c>
+      <c r="K5" s="56" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="237"/>
-      <c r="B5" s="237"/>
-      <c r="C5" s="211" t="s">
-        <v>343</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>344</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>345</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>346</v>
-      </c>
-      <c r="G5" s="56" t="s">
-        <v>347</v>
-      </c>
-      <c r="H5" s="56" t="s">
-        <v>348</v>
-      </c>
-      <c r="I5" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="J5" s="56" t="s">
-        <v>350</v>
-      </c>
-      <c r="K5" s="56" t="s">
-        <v>351</v>
-      </c>
       <c r="L5" s="56" t="s">
-        <v>352</v>
+        <v>430</v>
       </c>
       <c r="M5" s="56"/>
     </row>
     <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -56842,7 +56886,7 @@
       <c r="M6" s="67"/>
     </row>
     <row r="7" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="236"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -56859,7 +56903,7 @@
       <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="236"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -56867,36 +56911,36 @@
         <v>262</v>
       </c>
       <c r="D8" s="69" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="E8" s="69" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="69" t="s">
-        <v>355</v>
+        <v>425</v>
       </c>
       <c r="I8" s="69" t="s">
-        <v>355</v>
+        <v>425</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="L8" s="69" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="236"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -56913,7 +56957,7 @@
       <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="236"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -58575,13 +58619,12 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="37.28515625" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+    <col min="1" max="3" width="37.28515625" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" customWidth="1"/>
     <col min="6" max="6" width="39.85546875" bestFit="1" customWidth="1"/>
@@ -58593,84 +58636,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>358</v>
+        <v>426</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="E1" s="57" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="F1" s="57" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="G1" s="57" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="I1" s="57" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="J1" s="57" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="K1" s="57" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="L1" s="57" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="M1" s="57" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="229" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="B2" s="177" t="s">
-        <v>422</v>
-      </c>
-      <c r="C2" s="83" t="s">
-        <v>369</v>
+        <v>410</v>
+      </c>
+      <c r="C2" s="177" t="s">
+        <v>427</v>
       </c>
       <c r="D2" s="83" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="E2" s="83" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="F2" s="83" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="G2" s="83" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="H2" s="83" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="I2" s="83" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="J2" s="83" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="K2" s="83" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="L2" s="83" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="M2" s="83" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test 1,2,3 AZ_comp now are working
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab2\Documents\projects\IVM6311\IVM6311ATE-flavio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408706AE-8FAC-4227-B198-CE393BEFDF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830F3E68-BB23-4F02-A478-C3F24C1BF072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="434">
   <si>
     <t>Revision</t>
   </si>
@@ -42248,9 +42248,6 @@
   </si>
   <si>
     <t>1st_STG_Current</t>
-  </si>
-  <si>
-    <t>2V</t>
   </si>
   <si>
     <t>Enable_Ana_Testpoint_AZ_comp</t>
@@ -46862,8 +46859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A58BE6-10B8-478E-A3FE-3CA6A691AC11}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48859,7 +48856,7 @@
   <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56660,8 +56657,8 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56838,22 +56835,22 @@
         <v>340</v>
       </c>
       <c r="D5" s="37" t="s">
+        <v>430</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>431</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="F5" s="37" t="s">
         <v>432</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="G5" s="37" t="s">
         <v>433</v>
       </c>
-      <c r="G5" s="37" t="s">
-        <v>434</v>
-      </c>
       <c r="H5" s="56" t="s">
+        <v>427</v>
+      </c>
+      <c r="I5" s="56" t="s">
         <v>428</v>
-      </c>
-      <c r="I5" s="56" t="s">
-        <v>429</v>
       </c>
       <c r="J5" s="56" t="s">
         <v>341</v>
@@ -56862,7 +56859,7 @@
         <v>342</v>
       </c>
       <c r="L5" s="56" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M5" s="56"/>
     </row>
@@ -56923,10 +56920,10 @@
         <v>20</v>
       </c>
       <c r="H8" s="69" t="s">
-        <v>425</v>
+        <v>75</v>
       </c>
       <c r="I8" s="69" t="s">
-        <v>425</v>
+        <v>75</v>
       </c>
       <c r="J8" s="69" t="s">
         <v>345</v>
@@ -58642,7 +58639,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D1" s="57" t="s">
         <v>348</v>
@@ -58683,7 +58680,7 @@
         <v>410</v>
       </c>
       <c r="C2" s="177" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D2" s="83" t="s">
         <v>358</v>
@@ -58723,6 +58720,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
@@ -58731,15 +58737,6 @@
     <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58960,20 +58957,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
     <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added force parser instruction
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab2\Documents\projects\IVM6311\IVM6311ATE-flavio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830F3E68-BB23-4F02-A478-C3F24C1BF072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9600FF7-EA7C-4B94-9EF0-E7DF1F8978A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="433">
   <si>
     <t>Revision</t>
   </si>
@@ -41269,9 +41269,6 @@
   </si>
   <si>
     <t>&lt;6.6</t>
-  </si>
-  <si>
-    <t>VBAT/2</t>
   </si>
   <si>
     <t>Startup</t>
@@ -44773,7 +44770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -45380,6 +45377,9 @@
     <xf numFmtId="3" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -45793,177 +45793,177 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>368</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
+        <v>369</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>370</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="G6" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="24" t="s">
         <v>379</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="J6" s="25" t="s">
         <v>380</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="K6" s="58" t="s">
         <v>381</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="58" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="23" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>387</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>388</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="J9" s="25" t="s">
         <v>389</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="J10" s="25" t="s">
         <v>391</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="J11" s="25" t="s">
         <v>393</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>395</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="J13" s="25" t="s">
         <v>397</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="J14" s="25" t="s">
         <v>399</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="J15" s="25" t="s">
         <v>401</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="J16" s="25" t="s">
         <v>403</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="J17" s="25" t="s">
         <v>405</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="J18" s="25" t="s">
         <v>407</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -46873,7 +46873,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="231" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B1" s="231"/>
       <c r="C1" s="9" t="s">
@@ -46945,16 +46945,16 @@
       <c r="A5" s="232"/>
       <c r="B5" s="233"/>
       <c r="C5" s="220" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D5" s="207" t="s">
+        <v>411</v>
+      </c>
+      <c r="E5" s="207" t="s">
+        <v>415</v>
+      </c>
+      <c r="F5" s="223" t="s">
         <v>412</v>
-      </c>
-      <c r="E5" s="207" t="s">
-        <v>416</v>
-      </c>
-      <c r="F5" s="223" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
@@ -46969,7 +46969,7 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F6" s="67"/>
     </row>
@@ -48876,7 +48876,7 @@
         <v>213</v>
       </c>
       <c r="D1" s="117" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E1" s="230" t="s">
         <v>214</v>
@@ -48926,7 +48926,7 @@
         <v>213</v>
       </c>
       <c r="D4" s="117" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E4" s="104" t="s">
         <v>214</v>
@@ -48942,10 +48942,10 @@
         <v>216</v>
       </c>
       <c r="D5" s="219" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E5" s="210" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F5" s="222" t="s">
         <v>217</v>
@@ -48981,7 +48981,7 @@
         <v>149</v>
       </c>
       <c r="C8" s="107" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D8" s="120" t="s">
         <v>218</v>
@@ -56657,8 +56657,8 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56685,16 +56685,16 @@
         <v>64</v>
       </c>
       <c r="D1" s="65" t="s">
+        <v>420</v>
+      </c>
+      <c r="E1" s="65" t="s">
         <v>421</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="F1" s="65" t="s">
+        <v>423</v>
+      </c>
+      <c r="G1" s="65" t="s">
         <v>422</v>
-      </c>
-      <c r="F1" s="65" t="s">
-        <v>424</v>
-      </c>
-      <c r="G1" s="65" t="s">
-        <v>423</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>114</v>
@@ -56798,16 +56798,16 @@
         <v>64</v>
       </c>
       <c r="D4" s="65" t="s">
+        <v>420</v>
+      </c>
+      <c r="E4" s="65" t="s">
         <v>421</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="F4" s="65" t="s">
+        <v>423</v>
+      </c>
+      <c r="G4" s="65" t="s">
         <v>422</v>
-      </c>
-      <c r="F4" s="65" t="s">
-        <v>424</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>423</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>114</v>
@@ -56835,22 +56835,22 @@
         <v>340</v>
       </c>
       <c r="D5" s="37" t="s">
+        <v>429</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>430</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="F5" s="37" t="s">
         <v>431</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="G5" s="37" t="s">
         <v>432</v>
       </c>
-      <c r="G5" s="37" t="s">
-        <v>433</v>
-      </c>
       <c r="H5" s="56" t="s">
+        <v>426</v>
+      </c>
+      <c r="I5" s="37" t="s">
         <v>427</v>
-      </c>
-      <c r="I5" s="56" t="s">
-        <v>428</v>
       </c>
       <c r="J5" s="56" t="s">
         <v>341</v>
@@ -56859,7 +56859,7 @@
         <v>342</v>
       </c>
       <c r="L5" s="56" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M5" s="56"/>
     </row>
@@ -56919,11 +56919,11 @@
       <c r="G8" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="69" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="69" t="s">
-        <v>75</v>
+      <c r="H8" s="240">
+        <v>2</v>
+      </c>
+      <c r="I8" s="240">
+        <v>2</v>
       </c>
       <c r="J8" s="69" t="s">
         <v>345</v>
@@ -56931,8 +56931,8 @@
       <c r="K8" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="L8" s="69" t="s">
-        <v>346</v>
+      <c r="L8" s="240">
+        <v>2</v>
       </c>
       <c r="M8" s="69"/>
     </row>
@@ -58633,84 +58633,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D1" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="F1" s="57" t="s">
         <v>349</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="G1" s="57" t="s">
         <v>350</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="H1" s="57" t="s">
         <v>351</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="I1" s="57" t="s">
         <v>352</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="J1" s="57" t="s">
         <v>353</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>354</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="L1" s="57" t="s">
         <v>355</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="M1" s="57" t="s">
         <v>356</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="229" t="s">
+        <v>408</v>
+      </c>
+      <c r="B2" s="177" t="s">
         <v>409</v>
       </c>
-      <c r="B2" s="177" t="s">
-        <v>410</v>
-      </c>
       <c r="C2" s="177" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D2" s="83" t="s">
+        <v>357</v>
+      </c>
+      <c r="E2" s="83" t="s">
         <v>358</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="F2" s="83" t="s">
         <v>359</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="G2" s="83" t="s">
         <v>360</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="H2" s="83" t="s">
         <v>361</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="I2" s="83" t="s">
         <v>362</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="J2" s="83" t="s">
         <v>363</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="K2" s="83" t="s">
         <v>364</v>
       </c>
-      <c r="K2" s="83" t="s">
+      <c r="L2" s="83" t="s">
         <v>365</v>
       </c>
-      <c r="L2" s="83" t="s">
+      <c r="M2" s="83" t="s">
         <v>366</v>
-      </c>
-      <c r="M2" s="83" t="s">
-        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -58720,15 +58720,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
@@ -58737,6 +58728,15 @@
     <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58957,20 +58957,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
     <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update the script AZ_comp_ATE now it is working
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab2\Documents\projects\IVM6311\IVM6311ATE-flavio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9600FF7-EA7C-4B94-9EF0-E7DF1F8978A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9018998E-A1C9-43C8-B2CB-F5EAFBEAFE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="434">
   <si>
     <t>Revision</t>
   </si>
@@ -42310,7 +42310,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Run__startup </t>
+      <t xml:space="preserve">Run_startup </t>
     </r>
     <r>
       <rPr>
@@ -42329,7 +42329,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
+      <t>0xFE_0x01</t>
     </r>
     <r>
       <rPr>
@@ -42338,7 +42338,8 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"Select page 1"</t>
+      <t xml:space="preserve"> "Select page 1"  
+</t>
     </r>
     <r>
       <rPr>
@@ -42347,6 +42348,584 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"3rd STG Current analog test point</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Measure current between VBAT and SDWN pin"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Current__SDWN  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                                                        </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run_startup                                                                  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x18_0x02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x0F_0xC8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> " force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x10_0x08</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19_0x88</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1A_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "2rd STG Current analog test point"
+"Measure current between VBAT and SDWN pin"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Current__SDWN  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run_startup
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Select page 1"  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"1rd STG Current analog test point"
+"Measure current between VBAT and SDWN pin"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Current__SDWN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run__startup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">  
 0x17_0x02 </t>
     </r>
@@ -42444,7 +43023,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Enable_Ana_Testpoint_AZ_comp</t>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
     </r>
     <r>
       <rPr>
@@ -42463,7 +43042,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">0x1A_0x0B </t>
+      <t xml:space="preserve">0x1A_0x03 </t>
     </r>
     <r>
       <rPr>
@@ -42472,7 +43051,155 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">"OUTN_EXT_PRT analog test point"
+      <t xml:space="preserve">"GND analog test point"
+"Measure Voltage between SDWN pin and GND"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
+    </r>
+  </si>
+  <si>
+    <t>2v</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run__startup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  
+0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
 </t>
     </r>
     <r>
@@ -42480,6 +43207,45 @@
         <sz val="16"/>
         <color rgb="FFFF33CC"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x0B </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"OUTN_EXT_PRT analog test point"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Force__OUTP__2V   
@@ -42648,7 +43414,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Enable_Ana_Testpoint_AZ_comp</t>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
     </r>
     <r>
       <rPr>
@@ -42852,7 +43618,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Enable_Ana_Testpoint_AZ_comp</t>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
     </r>
     <r>
       <rPr>
@@ -42882,769 +43648,6 @@
       </rPr>
       <t xml:space="preserve">"VCM_AVDD analog test point"
  "Measure Voltage between SDWN pin and GND, you should measure VBAT/2"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run_startup </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"3rd STG Current analog test point</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Measure current between VBAT and SDWN pin"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Current__SDWN  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                                                                                                        </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run_startup                                                                  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x18_0x02</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x0F_0xC8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> " force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x10_0x08</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  "Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19_0x88</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  "test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1A_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "2rd STG Current analog test point"
-"Measure current between VBAT and SDWN pin"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Current__SDWN  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run_startup
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 1"  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"1rd STG Current analog test point"
-"Measure current between VBAT and SDWN pin"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Current__SDWN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run__startup </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Select page 1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  
-0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x03 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"GND analog test point"
-"Measure Voltage between SDWN pin and GND"
 </t>
     </r>
     <r>
@@ -45350,6 +45353,9 @@
     <xf numFmtId="49" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -45376,9 +45382,6 @@
     </xf>
     <xf numFmtId="3" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -46872,10 +46875,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="232" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="231"/>
+      <c r="B1" s="232"/>
       <c r="C1" s="9" t="s">
         <v>142</v>
       </c>
@@ -46906,10 +46909,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="231" t="s">
+      <c r="A3" s="232" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="231"/>
+      <c r="B3" s="232"/>
       <c r="C3" s="15" t="s">
         <v>60</v>
       </c>
@@ -46924,10 +46927,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="232" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="231"/>
+      <c r="B4" s="232"/>
       <c r="C4" s="9" t="s">
         <v>142</v>
       </c>
@@ -46942,8 +46945,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="232"/>
-      <c r="B5" s="233"/>
+      <c r="A5" s="233"/>
+      <c r="B5" s="234"/>
       <c r="C5" s="220" t="s">
         <v>413</v>
       </c>
@@ -46958,7 +46961,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="234" t="s">
+      <c r="A6" s="235" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -46974,7 +46977,7 @@
       <c r="F6" s="67"/>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="234"/>
+      <c r="A7" s="235"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -46986,7 +46989,7 @@
       <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="234"/>
+      <c r="A8" s="235"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -47002,7 +47005,7 @@
       <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="234"/>
+      <c r="A9" s="235"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -47016,7 +47019,7 @@
       <c r="F9" s="71"/>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="234"/>
+      <c r="A10" s="235"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -47941,10 +47944,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="232" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="231"/>
+      <c r="B1" s="232"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -47975,10 +47978,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="231" t="s">
+      <c r="A3" s="232" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="231"/>
+      <c r="B3" s="232"/>
       <c r="C3" s="15" t="s">
         <v>79</v>
       </c>
@@ -47993,10 +47996,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="232" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="231"/>
+      <c r="B4" s="232"/>
       <c r="C4" s="9" t="s">
         <v>202</v>
       </c>
@@ -48011,8 +48014,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="273" x14ac:dyDescent="0.25">
-      <c r="A5" s="232"/>
-      <c r="B5" s="233"/>
+      <c r="A5" s="233"/>
+      <c r="B5" s="234"/>
       <c r="C5" s="37" t="s">
         <v>206</v>
       </c>
@@ -48027,7 +48030,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="234" t="s">
+      <c r="A6" s="235" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48045,7 +48048,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="234"/>
+      <c r="A7" s="235"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48061,7 +48064,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="234"/>
+      <c r="A8" s="235"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -48079,7 +48082,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="234"/>
+      <c r="A9" s="235"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -48095,7 +48098,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="234"/>
+      <c r="A10" s="235"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -48868,10 +48871,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="232" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="231"/>
+      <c r="B1" s="232"/>
       <c r="C1" s="104" t="s">
         <v>213</v>
       </c>
@@ -48900,10 +48903,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="231" t="s">
+      <c r="A3" s="232" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="231"/>
+      <c r="B3" s="232"/>
       <c r="C3" s="103" t="s">
         <v>20</v>
       </c>
@@ -48918,10 +48921,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="232" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="231"/>
+      <c r="B4" s="232"/>
       <c r="C4" s="104" t="s">
         <v>213</v>
       </c>
@@ -48936,8 +48939,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="232"/>
-      <c r="B5" s="233"/>
+      <c r="A5" s="233"/>
+      <c r="B5" s="234"/>
       <c r="C5" s="210" t="s">
         <v>216</v>
       </c>
@@ -48952,7 +48955,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="234" t="s">
+      <c r="A6" s="235" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48966,7 +48969,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="234"/>
+      <c r="A7" s="235"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48976,7 +48979,7 @@
       <c r="F7" s="131"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="234"/>
+      <c r="A8" s="235"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -48994,7 +48997,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="234"/>
+      <c r="A9" s="235"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -49006,7 +49009,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="234"/>
+      <c r="A10" s="235"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -49926,10 +49929,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="236" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="235"/>
+      <c r="B1" s="236"/>
       <c r="C1" s="17" t="s">
         <v>222</v>
       </c>
@@ -50096,10 +50099,10 @@
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="236" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="235"/>
+      <c r="B3" s="236"/>
       <c r="C3" s="185" t="s">
         <v>20</v>
       </c>
@@ -50183,10 +50186,10 @@
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="235" t="s">
+      <c r="A4" s="236" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="235"/>
+      <c r="B4" s="236"/>
       <c r="C4" s="65" t="s">
         <v>19</v>
       </c>
@@ -50270,8 +50273,8 @@
       </c>
     </row>
     <row r="5" spans="1:29" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="236"/>
-      <c r="B5" s="236"/>
+      <c r="A5" s="237"/>
+      <c r="B5" s="237"/>
       <c r="C5" s="226" t="s">
         <v>234</v>
       </c>
@@ -50355,7 +50358,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="238" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -50434,7 +50437,7 @@
       <c r="AC6" s="67"/>
     </row>
     <row r="7" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="237"/>
+      <c r="A7" s="238"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -50469,7 +50472,7 @@
       <c r="AC7" s="68"/>
     </row>
     <row r="8" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="237"/>
+      <c r="A8" s="238"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -50522,7 +50525,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="237"/>
+      <c r="A9" s="238"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -50601,7 +50604,7 @@
       <c r="AC9" s="71"/>
     </row>
     <row r="10" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="237"/>
+      <c r="A10" s="238"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -54143,10 +54146,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="236" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="235"/>
+      <c r="B1" s="236"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -54241,10 +54244,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="236" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="235"/>
+      <c r="B3" s="236"/>
       <c r="C3" s="15" t="s">
         <v>99</v>
       </c>
@@ -54292,10 +54295,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="235" t="s">
+      <c r="A4" s="236" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="235"/>
+      <c r="B4" s="236"/>
       <c r="C4" s="65" t="s">
         <v>278</v>
       </c>
@@ -54343,8 +54346,8 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="238"/>
-      <c r="B5" s="239"/>
+      <c r="A5" s="239"/>
+      <c r="B5" s="240"/>
       <c r="C5" s="224" t="s">
         <v>293</v>
       </c>
@@ -54392,7 +54395,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="238" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -54415,7 +54418,7 @@
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="237"/>
+      <c r="A7" s="238"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -54436,7 +54439,7 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="237"/>
+      <c r="A8" s="238"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -54481,7 +54484,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="237"/>
+      <c r="A9" s="238"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -54506,7 +54509,7 @@
       <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="237"/>
+      <c r="A10" s="238"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -56657,7 +56660,7 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -56677,10 +56680,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="236" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="235"/>
+      <c r="B1" s="236"/>
       <c r="C1" s="65" t="s">
         <v>64</v>
       </c>
@@ -56751,10 +56754,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="236" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="235"/>
+      <c r="B3" s="236"/>
       <c r="C3" s="64" t="s">
         <v>65</v>
       </c>
@@ -56790,10 +56793,10 @@
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A4" s="235" t="s">
+      <c r="A4" s="236" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="235"/>
+      <c r="B4" s="236"/>
       <c r="C4" s="65" t="s">
         <v>64</v>
       </c>
@@ -56829,28 +56832,28 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="238"/>
-      <c r="B5" s="238"/>
+      <c r="A5" s="239"/>
+      <c r="B5" s="239"/>
       <c r="C5" s="211" t="s">
         <v>340</v>
       </c>
       <c r="D5" s="37" t="s">
+        <v>426</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>427</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>428</v>
+      </c>
+      <c r="G5" s="37" t="s">
         <v>429</v>
       </c>
-      <c r="E5" s="37" t="s">
-        <v>430</v>
-      </c>
-      <c r="F5" s="37" t="s">
+      <c r="H5" s="37" t="s">
         <v>431</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="I5" s="37" t="s">
         <v>432</v>
-      </c>
-      <c r="H5" s="56" t="s">
-        <v>426</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>427</v>
       </c>
       <c r="J5" s="56" t="s">
         <v>341</v>
@@ -56858,13 +56861,13 @@
       <c r="K5" s="56" t="s">
         <v>342</v>
       </c>
-      <c r="L5" s="56" t="s">
-        <v>428</v>
+      <c r="L5" s="37" t="s">
+        <v>433</v>
       </c>
       <c r="M5" s="56"/>
     </row>
     <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="238" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -56883,7 +56886,7 @@
       <c r="M6" s="67"/>
     </row>
     <row r="7" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="237"/>
+      <c r="A7" s="238"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -56900,7 +56903,7 @@
       <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="237"/>
+      <c r="A8" s="238"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -56919,11 +56922,11 @@
       <c r="G8" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="240">
-        <v>2</v>
-      </c>
-      <c r="I8" s="240">
-        <v>2</v>
+      <c r="H8" s="231" t="s">
+        <v>430</v>
+      </c>
+      <c r="I8" s="231" t="s">
+        <v>430</v>
       </c>
       <c r="J8" s="69" t="s">
         <v>345</v>
@@ -56931,13 +56934,13 @@
       <c r="K8" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="L8" s="240">
-        <v>2</v>
+      <c r="L8" s="231" t="s">
+        <v>430</v>
       </c>
       <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="237"/>
+      <c r="A9" s="238"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -56954,7 +56957,7 @@
       <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="237"/>
+      <c r="A10" s="238"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -58720,6 +58723,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
@@ -58728,15 +58740,6 @@
     <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58957,20 +58960,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
     <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
shift the typical_value_clean function in dft_syntaxparser.py
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab2\Documents\projects\IVM6311\IVM6311ATE-flavio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9018998E-A1C9-43C8-B2CB-F5EAFBEAFE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53380B30-CF65-48EE-81F0-AE8B9DC14754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="3" r:id="rId1"/>
@@ -42000,68 +42000,6 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Run__Startup
-Run__Enable_Ana_Testpoint
-0xFE_0x01 "Select page 1"
-0x1A_0x04 "TSDN"
-Measure__Voltage__SDWN
-TrimSweep -  0xB3[7:5] "Select code which sets ATEST voltage as close as possible to target"
-Calculate__MinError
-0xFE_0x00 "Return page 0"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run__startup
-Run__Boost_test_default
-Wait__delay__0.1ms
-0xFE_0x00 "Select page 0"
-0xB0[1]_0x01 "ocp en
-0xB2[1]_0x01 "ls_sel on"
-0xC0[2:0]_0x01 "OCP threshold set to 200mA"
-0xFE_0x01 "Select page 1"
-0x1A_0x10 "TSW to OCP Sense"
-Wait__delay__0.1ms
-0xFE_0x00 "Select page 0"
-0xB2[0]_0x01 "Power Force en"
-0xFE_0x01 "Select page 1"
-Wait__delay__0.1ms
-0x15[2]_0x01 "Force ocp"
-0x19[1]_0x01 "bst_test en"
-Wait__delay__0.1ms
-Measure__Voltage__SDWN
-TrimSweep - 0xB2[5]_0xB1[3:0] "trim in 2 different registers, what is the correct command"
-Calculate__MinError
-0x1A_0x00
-0x19_0x00
-</t>
-  </si>
-  <si>
-    <t>Run__Startup
-Run__Enable_Ana_Testpoint
-0xFE_0x01 "Select page 1"
-0x1A_0x01 "Bandgap"
-0xB0_0x0E
-Measure__Voltage__SDWN
-TrimSweep - 0xB0[7:4] "Select code which sets ATEST voltage as close as possible to target"
-Calculate__MinError
-0xFE_0x00 "Return page 0"</t>
-  </si>
-  <si>
-    <t>0xFE_0x01</t>
-  </si>
-  <si>
-    <t>Run__Startup
-0xFE_0x00
-0x00_0x0D
-0xFE_0x01 "Select page 1"
-0x03_0x04 "Enable digital test FSYN"
-0x04_0x20 "Enable digital test ana_ref_fro_clk_13m"
-0x0F_0x80
-Measure__Frequency__FSYN
-TrimSweep -  0xEF[4:0] "Select code which sets ATEST frequency as close as possible to target"
-Calculate__MinError
-0xFE_0x00 "Return page 0"</t>
-  </si>
-  <si>
     <t>3,6</t>
   </si>
   <si>
@@ -43659,6 +43597,65 @@
       </rPr>
       <t xml:space="preserve">Measure__Voltage_SDWN  </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">"Run__startup
+Run__Boost_test_default
+Wait__delay__0.1ms
+0xFE_0x00 ""Select page 0""
+0xB0[1]_0x01 ""ocp en
+0xB2[1]_0x01 ""ls_sel on""
+0xC0[2:0]_0x01 ""OCP threshold set to 200mA""
+0xFE_0x01 ""Select page 1""
+0x1A_0x10 ""TSW to OCP Sense""
+Wait__delay__0.1ms
+0xFE_0x00 ""Select page 0""
+0xB2[0]_0x01 ""Power Force en""
+0xFE_0x01 ""Select page 1""
+Wait__delay__0.1ms
+0x15[2]_0x01 ""Force ocp""
+0x19[1]_0x01 ""bst_test en""
+Wait__delay__0.1ms
+Measure__Voltage__SDWN
+Trim__0xB2[5]_0xB1[3:0] ""trim in 2 different registers, what is the correct command""
+Calculate__MinError
+0x1A_0x00
+0x19_0x00
+"
+</t>
+  </si>
+  <si>
+    <t>Run__Startup
+0xFE_0x01 "Select page 1"
+0x03_0x04 "Enable digital test FSYN"
+0x04_0x32 "Enable digital test ana_ref_fro_clk_13m"
+Measure__Frequency__FSYN
+Trim__ 0xEF[4:0] "Select code which sets ATEST frequency as close as possible to target"
+Calculate__MinError
+0xFE_0x00 "Return page 0"</t>
+  </si>
+  <si>
+    <t>12,5</t>
+  </si>
+  <si>
+    <t>Run__Startup
+Run__Enable_Ana_Testpoint
+0xFE_0x01 "Select page 1"
+0x1A_0x04 "TSDN"
+Measure__Voltage__SDWN
+Trim__ 0xB3[7:5] "Select code which sets ATEST voltage as close as possible to target"
+Calculate__MinError
+0xFE_0x00 "Return page 0"</t>
+  </si>
+  <si>
+    <t>Run__Startup
+Run__Enable_Ana_Testpoint
+0xFE_0x01 "Select page 1"
+0x1A_0x01 "Bandgap"
+Measure__Voltage__SDWN
+Trim__0xB0[7:4] "Select code which sets ATEST voltage as close as possible to target"
+Calculate__MinError
+0xFE_0x00 "Return page 0"</t>
   </si>
 </sst>
 </file>
@@ -44773,7 +44770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="241">
+  <cellXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -45329,9 +45326,6 @@
     <xf numFmtId="49" fontId="14" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -46065,7 +46059,7 @@
       <c r="F3" s="151" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="227" t="s">
+      <c r="G3" s="226" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="213" t="s">
@@ -46091,7 +46085,7 @@
       <c r="F4" s="188" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="228" t="s">
+      <c r="G4" s="227" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="186" t="s">
@@ -46117,7 +46111,7 @@
       <c r="F5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="226" t="s">
+      <c r="G5" s="225" t="s">
         <v>29</v>
       </c>
       <c r="H5" s="186" t="s">
@@ -46143,7 +46137,7 @@
       <c r="F6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="226" t="s">
+      <c r="G6" s="225" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="186" t="s">
@@ -46169,10 +46163,10 @@
       <c r="F7" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="226" t="s">
+      <c r="G7" s="225" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="226" t="s">
+      <c r="H7" s="225" t="s">
         <v>38</v>
       </c>
     </row>
@@ -46247,7 +46241,7 @@
       <c r="F10" s="190" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="226" t="s">
+      <c r="G10" s="225" t="s">
         <v>49</v>
       </c>
       <c r="H10" s="186" t="s">
@@ -46429,7 +46423,7 @@
       <c r="F17" s="190" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="226" t="s">
+      <c r="G17" s="225" t="s">
         <v>76</v>
       </c>
       <c r="H17" s="186" t="s">
@@ -46844,7 +46838,7 @@
       <c r="F34" s="190" t="s">
         <v>134</v>
       </c>
-      <c r="G34" s="226" t="s">
+      <c r="G34" s="225" t="s">
         <v>135</v>
       </c>
       <c r="H34" s="186" t="s">
@@ -46862,8 +46856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A58BE6-10B8-478E-A3FE-3CA6A691AC11}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46875,10 +46869,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="231" t="s">
         <v>410</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="231"/>
       <c r="C1" s="9" t="s">
         <v>142</v>
       </c>
@@ -46909,10 +46903,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="231" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="232"/>
+      <c r="B3" s="231"/>
       <c r="C3" s="15" t="s">
         <v>60</v>
       </c>
@@ -46927,10 +46921,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="232" t="s">
+      <c r="A4" s="231" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="231"/>
       <c r="C4" s="9" t="s">
         <v>142</v>
       </c>
@@ -46945,23 +46939,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="233"/>
-      <c r="B5" s="234"/>
+      <c r="A5" s="232"/>
+      <c r="B5" s="233"/>
       <c r="C5" s="220" t="s">
-        <v>413</v>
+        <v>433</v>
       </c>
       <c r="D5" s="207" t="s">
-        <v>411</v>
+        <v>432</v>
       </c>
       <c r="E5" s="207" t="s">
-        <v>415</v>
-      </c>
-      <c r="F5" s="223" t="s">
-        <v>412</v>
+        <v>430</v>
+      </c>
+      <c r="F5" s="192" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="235" t="s">
+      <c r="A6" s="234" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -46972,12 +46966,12 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>414</v>
+        <v>431</v>
       </c>
       <c r="F6" s="67"/>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="235"/>
+      <c r="A7" s="234"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -46989,7 +46983,7 @@
       <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="235"/>
+      <c r="A8" s="234"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -47005,7 +46999,7 @@
       <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="235"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -47013,13 +47007,11 @@
         <v>1804</v>
       </c>
       <c r="D9" s="39"/>
-      <c r="E9" s="39" t="s">
-        <v>153</v>
-      </c>
+      <c r="E9" s="39"/>
       <c r="F9" s="71"/>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="235"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -47027,7 +47019,9 @@
         <v>155</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>153</v>
+      </c>
       <c r="F10" s="68"/>
     </row>
     <row r="11" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
@@ -47944,10 +47938,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="231" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="231"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -47978,10 +47972,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="231" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="232"/>
+      <c r="B3" s="231"/>
       <c r="C3" s="15" t="s">
         <v>79</v>
       </c>
@@ -47996,10 +47990,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="232" t="s">
+      <c r="A4" s="231" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="231"/>
       <c r="C4" s="9" t="s">
         <v>202</v>
       </c>
@@ -48014,8 +48008,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="273" x14ac:dyDescent="0.25">
-      <c r="A5" s="233"/>
-      <c r="B5" s="234"/>
+      <c r="A5" s="232"/>
+      <c r="B5" s="233"/>
       <c r="C5" s="37" t="s">
         <v>206</v>
       </c>
@@ -48030,7 +48024,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="235" t="s">
+      <c r="A6" s="234" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48048,7 +48042,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="235"/>
+      <c r="A7" s="234"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48064,7 +48058,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="235"/>
+      <c r="A8" s="234"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -48082,7 +48076,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="235"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -48098,7 +48092,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="235"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -48871,17 +48865,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="231" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="231"/>
       <c r="C1" s="104" t="s">
         <v>213</v>
       </c>
       <c r="D1" s="117" t="s">
-        <v>419</v>
-      </c>
-      <c r="E1" s="230" t="s">
+        <v>414</v>
+      </c>
+      <c r="E1" s="229" t="s">
         <v>214</v>
       </c>
       <c r="F1" s="129" t="s">
@@ -48903,10 +48897,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="231" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="232"/>
+      <c r="B3" s="231"/>
       <c r="C3" s="103" t="s">
         <v>20</v>
       </c>
@@ -48921,15 +48915,15 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="232" t="s">
+      <c r="A4" s="231" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="231"/>
       <c r="C4" s="104" t="s">
         <v>213</v>
       </c>
       <c r="D4" s="117" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="E4" s="104" t="s">
         <v>214</v>
@@ -48939,23 +48933,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="233"/>
-      <c r="B5" s="234"/>
+      <c r="A5" s="232"/>
+      <c r="B5" s="233"/>
       <c r="C5" s="210" t="s">
         <v>216</v>
       </c>
       <c r="D5" s="219" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E5" s="210" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="F5" s="222" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="235" t="s">
+      <c r="A6" s="234" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48969,7 +48963,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="235"/>
+      <c r="A7" s="234"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48979,12 +48973,12 @@
       <c r="F7" s="131"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="235"/>
+      <c r="A8" s="234"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
       <c r="C8" s="107" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="D8" s="120" t="s">
         <v>218</v>
@@ -48997,7 +48991,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="235"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -49009,7 +49003,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="235"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -49929,10 +49923,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="236" t="s">
+      <c r="A1" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="236"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="17" t="s">
         <v>222</v>
       </c>
@@ -50099,10 +50093,10 @@
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="236"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="185" t="s">
         <v>20</v>
       </c>
@@ -50186,10 +50180,10 @@
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="236" t="s">
+      <c r="A4" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="236"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="65" t="s">
         <v>19</v>
       </c>
@@ -50273,18 +50267,18 @@
       </c>
     </row>
     <row r="5" spans="1:29" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="237"/>
-      <c r="B5" s="237"/>
-      <c r="C5" s="226" t="s">
+      <c r="A5" s="236"/>
+      <c r="B5" s="236"/>
+      <c r="C5" s="225" t="s">
         <v>234</v>
       </c>
-      <c r="D5" s="226" t="s">
+      <c r="D5" s="225" t="s">
         <v>235</v>
       </c>
-      <c r="E5" s="226" t="s">
+      <c r="E5" s="225" t="s">
         <v>236</v>
       </c>
-      <c r="F5" s="226" t="s">
+      <c r="F5" s="225" t="s">
         <v>237</v>
       </c>
       <c r="G5" s="186" t="s">
@@ -50308,19 +50302,19 @@
       <c r="M5" s="186" t="s">
         <v>50</v>
       </c>
-      <c r="N5" s="226" t="s">
+      <c r="N5" s="225" t="s">
         <v>244</v>
       </c>
-      <c r="O5" s="226" t="s">
+      <c r="O5" s="225" t="s">
         <v>245</v>
       </c>
-      <c r="P5" s="226" t="s">
+      <c r="P5" s="225" t="s">
         <v>246</v>
       </c>
-      <c r="Q5" s="226" t="s">
+      <c r="Q5" s="225" t="s">
         <v>247</v>
       </c>
-      <c r="R5" s="226" t="s">
+      <c r="R5" s="225" t="s">
         <v>248</v>
       </c>
       <c r="S5" s="191" t="s">
@@ -50353,12 +50347,12 @@
       <c r="AB5" s="192" t="s">
         <v>258</v>
       </c>
-      <c r="AC5" s="226" t="s">
+      <c r="AC5" s="225" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="238" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -50437,7 +50431,7 @@
       <c r="AC6" s="67"/>
     </row>
     <row r="7" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="238"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -50472,7 +50466,7 @@
       <c r="AC7" s="68"/>
     </row>
     <row r="8" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="238"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -50525,7 +50519,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="238"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -50604,7 +50598,7 @@
       <c r="AC9" s="71"/>
     </row>
     <row r="10" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="238"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -54146,10 +54140,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="236" t="s">
+      <c r="A1" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="236"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -54244,10 +54238,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="236"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="15" t="s">
         <v>99</v>
       </c>
@@ -54295,10 +54289,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="236" t="s">
+      <c r="A4" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="236"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="65" t="s">
         <v>278</v>
       </c>
@@ -54346,12 +54340,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="239"/>
-      <c r="B5" s="240"/>
-      <c r="C5" s="224" t="s">
+      <c r="A5" s="238"/>
+      <c r="B5" s="239"/>
+      <c r="C5" s="223" t="s">
         <v>293</v>
       </c>
-      <c r="D5" s="225" t="s">
+      <c r="D5" s="224" t="s">
         <v>294</v>
       </c>
       <c r="E5" s="206" t="s">
@@ -54395,7 +54389,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="238" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -54418,7 +54412,7 @@
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="238"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -54439,7 +54433,7 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="238"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -54484,7 +54478,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="238"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -54509,7 +54503,7 @@
       <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="238"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -56660,7 +56654,7 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -56680,24 +56674,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="236" t="s">
+      <c r="A1" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="236"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="65" t="s">
         <v>64</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="G1" s="65" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>114</v>
@@ -56754,10 +56748,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="236"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="64" t="s">
         <v>65</v>
       </c>
@@ -56793,24 +56787,24 @@
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A4" s="236" t="s">
+      <c r="A4" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="236"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="65" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E4" s="65" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="F4" s="65" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>114</v>
@@ -56832,28 +56826,28 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="239"/>
-      <c r="B5" s="239"/>
+      <c r="A5" s="238"/>
+      <c r="B5" s="238"/>
       <c r="C5" s="211" t="s">
         <v>340</v>
       </c>
       <c r="D5" s="37" t="s">
+        <v>421</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>422</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>423</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>424</v>
+      </c>
+      <c r="H5" s="37" t="s">
         <v>426</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="I5" s="37" t="s">
         <v>427</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>428</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>429</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>431</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>432</v>
       </c>
       <c r="J5" s="56" t="s">
         <v>341</v>
@@ -56862,12 +56856,12 @@
         <v>342</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="M5" s="56"/>
     </row>
     <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="238" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -56886,7 +56880,7 @@
       <c r="M6" s="67"/>
     </row>
     <row r="7" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="238"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -56903,7 +56897,7 @@
       <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="238"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -56922,11 +56916,11 @@
       <c r="G8" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="231" t="s">
-        <v>430</v>
-      </c>
-      <c r="I8" s="231" t="s">
-        <v>430</v>
+      <c r="H8" s="230" t="s">
+        <v>425</v>
+      </c>
+      <c r="I8" s="230" t="s">
+        <v>425</v>
       </c>
       <c r="J8" s="69" t="s">
         <v>345</v>
@@ -56934,13 +56928,13 @@
       <c r="K8" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="L8" s="231" t="s">
-        <v>430</v>
+      <c r="L8" s="230" t="s">
+        <v>425</v>
       </c>
       <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="238"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -56957,7 +56951,7 @@
       <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="238"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -58642,7 +58636,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D1" s="57" t="s">
         <v>347</v>
@@ -58676,14 +58670,14 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="229" t="s">
+      <c r="A2" s="228" t="s">
         <v>408</v>
       </c>
       <c r="B2" s="177" t="s">
         <v>409</v>
       </c>
       <c r="C2" s="177" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D2" s="83" t="s">
         <v>357</v>
@@ -58723,15 +58717,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
@@ -58740,6 +58725,15 @@
     <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58960,20 +58954,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
     <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
value clean function edited im parser
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab2\Documents\projects\IVM6311\IVM6311ATE-flavio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53380B30-CF65-48EE-81F0-AE8B9DC14754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E027041B-21DF-48F1-AC32-F944B5AE7552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="433">
   <si>
     <t>Revision</t>
   </si>
@@ -40367,558 +40367,6 @@
     <r>
       <rPr>
         <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run_startup  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 1"   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                                                                                                         
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x03_0x05</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Enable digital test FSYN"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x04_0x72</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Enable digital test ana_azcomp_out"  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0x80  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force otp_clock_on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x10  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force pa_pd_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x14_0x04</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  "Force en_dac3_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x13_0x04</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  "Force en_dac3_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x18_0x02</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  "Force_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xE0_0x0C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Comparator measure time 600us"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xE1_0x1F</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"azcomp_isel 2.0uA"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">   
-Force__OUTP__2V   
-Force__OUTN__2V 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Follow this step:
-1. Increased OUTN 1 step millivolt
-2. Write 0xE4_0x01
-3. Check on the oscilloscope SDI and FSYN. In the SDI you should see a digital signal that goes high for 750us. On the FSYN you should see the output of the azcomp.  
-4. You have to increased OUTN until the output of the azcomp became stable after 1ms. In this way you have found the values for which the offset is eliminated "
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Force__OUTN__2.001V </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"(1.)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xE4_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"azcomp_isel 2.0uA (2.)"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                                       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__FSYN </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"(3.)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__SDI </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"(3.)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Repeat the steps written before  (4.)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Force__OUTP__2V   
-Force__OUTN__2V 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Follow this step:
-1. Decrease OUTN 1 step millivolt
-2. Write 0xE4_0x01
-3. Check on the oscilloscope SDI and FSYN. In the SDI you should see a digital signal that goes high for 750us. On the FSYN you should see the output of the azcomp.  
-4. You have to decreased OUTN until the output of the azcomp became stable after 1ms. In this way you have found the values for which the offset is eliminated "
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Force__OUTN__1.999V </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"(1.)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xE4_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  "azcomp_isel 2.0uA (2.)"                                                                                                                                     </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__FSYN </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"(3.)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__SDI </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"(3.)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Repeat the steps written before (4.)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
         <color rgb="FFFF3399"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
@@ -43004,9 +42452,6 @@
     </r>
   </si>
   <si>
-    <t>2v</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="16"/>
@@ -43656,6 +43101,552 @@
 Trim__0xB0[7:4] "Select code which sets ATEST voltage as close as possible to target"
 Calculate__MinError
 0xFE_0x00 "Return page 0"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run_startup  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Select page 1"   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                                                                         
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x03_0x05</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Enable digital test FSYN"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x04_0x72</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Enable digital test ana_azcomp_out"  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0x80  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force otp_clock_on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x10  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force pa_pd_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x14_0x04</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "Force en_dac3_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x13_0x04</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "Force en_dac3_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x18_0x02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "Force_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xE0_0x0C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Comparator measure time 600us"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xE1_0x1F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"azcomp_isel 2.0uA"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   
+Force__OUTP__2V   
+Force__OUTN__2V 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Follow this step:
+1. Increased OUTN 1 step millivolt
+2. Write 0xE4_0x01
+3. Check on the oscilloscope SDI and FSYN. In the SDI you should see a digital signal that goes high for 750us. On the FSYN you should see the output of the azcomp.  
+4. You have to increased OUTN until the output of the azcomp became stable after 1ms. In this way you have found the values for which the offset is eliminated "
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Force__OUTN__2.001V </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"(1.)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xE4_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"azcomp_isel 2.0uA (2.)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__FSYN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"(3.)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__SDI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"(3.)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Repeat the steps written before  (4.)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Force__OUTP__2V   
+Force__OUTN__2V 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Follow this step:
+1. Decrease OUTN 1 step millivolt
+2. Write 0xE4_0x01
+3. Check on the oscilloscope SDI and FSYN. In the SDI you should see a digital signal that goes high for 750us. On the FSYN you should see the output of the azcomp.  
+4. You have to decreased OUTN until the output of the azcomp became stable after 1ms. In this way you have found the values for which the offset is eliminated "
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Force__OUTN__1.999V </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"(1.)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xE4_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "azcomp_isel 2.0uA (2.)"                                                                                                                                     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__FSYN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"(3.)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__SDI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"(3.)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Repeat the steps written before (4.)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -44770,7 +44761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -45347,9 +45338,6 @@
     <xf numFmtId="49" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -45790,177 +45778,177 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>367</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>369</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="G6" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="24" t="s">
         <v>378</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="J6" s="25" t="s">
         <v>379</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="K6" s="58" t="s">
         <v>380</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="58" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="23" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>386</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>387</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
+        <v>387</v>
+      </c>
+      <c r="J9" s="25" t="s">
         <v>388</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="J10" s="25" t="s">
         <v>390</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="J11" s="25" t="s">
         <v>392</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>394</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="J13" s="25" t="s">
         <v>396</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="J14" s="25" t="s">
         <v>398</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="J15" s="25" t="s">
         <v>400</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="J16" s="25" t="s">
         <v>402</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="J17" s="25" t="s">
         <v>404</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
+        <v>405</v>
+      </c>
+      <c r="J18" s="25" t="s">
         <v>406</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -46856,7 +46844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A58BE6-10B8-478E-A3FE-3CA6A691AC11}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -46869,10 +46857,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="231" t="s">
-        <v>410</v>
-      </c>
-      <c r="B1" s="231"/>
+      <c r="A1" s="230" t="s">
+        <v>409</v>
+      </c>
+      <c r="B1" s="230"/>
       <c r="C1" s="9" t="s">
         <v>142</v>
       </c>
@@ -46903,10 +46891,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="231" t="s">
+      <c r="A3" s="230" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="231"/>
+      <c r="B3" s="230"/>
       <c r="C3" s="15" t="s">
         <v>60</v>
       </c>
@@ -46921,10 +46909,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="230" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="231"/>
+      <c r="B4" s="230"/>
       <c r="C4" s="9" t="s">
         <v>142</v>
       </c>
@@ -46939,23 +46927,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="232"/>
-      <c r="B5" s="233"/>
+      <c r="A5" s="231"/>
+      <c r="B5" s="232"/>
       <c r="C5" s="220" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D5" s="207" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E5" s="207" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F5" s="192" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="234" t="s">
+      <c r="A6" s="233" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -46966,12 +46954,12 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F6" s="67"/>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="234"/>
+      <c r="A7" s="233"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -46983,7 +46971,7 @@
       <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="234"/>
+      <c r="A8" s="233"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -46999,7 +46987,7 @@
       <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="234"/>
+      <c r="A9" s="233"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -47011,7 +46999,7 @@
       <c r="F9" s="71"/>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="234"/>
+      <c r="A10" s="233"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -47938,10 +47926,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="230" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="231"/>
+      <c r="B1" s="230"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -47972,10 +47960,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="231" t="s">
+      <c r="A3" s="230" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="231"/>
+      <c r="B3" s="230"/>
       <c r="C3" s="15" t="s">
         <v>79</v>
       </c>
@@ -47990,10 +47978,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="230" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="231"/>
+      <c r="B4" s="230"/>
       <c r="C4" s="9" t="s">
         <v>202</v>
       </c>
@@ -48008,8 +47996,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="273" x14ac:dyDescent="0.25">
-      <c r="A5" s="232"/>
-      <c r="B5" s="233"/>
+      <c r="A5" s="231"/>
+      <c r="B5" s="232"/>
       <c r="C5" s="37" t="s">
         <v>206</v>
       </c>
@@ -48024,7 +48012,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="234" t="s">
+      <c r="A6" s="233" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48042,7 +48030,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="234"/>
+      <c r="A7" s="233"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48058,7 +48046,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="234"/>
+      <c r="A8" s="233"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -48076,7 +48064,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="234"/>
+      <c r="A9" s="233"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -48092,7 +48080,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="234"/>
+      <c r="A10" s="233"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -48865,15 +48853,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="230" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="231"/>
+      <c r="B1" s="230"/>
       <c r="C1" s="104" t="s">
         <v>213</v>
       </c>
       <c r="D1" s="117" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E1" s="229" t="s">
         <v>214</v>
@@ -48897,10 +48885,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="231" t="s">
+      <c r="A3" s="230" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="231"/>
+      <c r="B3" s="230"/>
       <c r="C3" s="103" t="s">
         <v>20</v>
       </c>
@@ -48915,15 +48903,15 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="230" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="231"/>
+      <c r="B4" s="230"/>
       <c r="C4" s="104" t="s">
         <v>213</v>
       </c>
       <c r="D4" s="117" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E4" s="104" t="s">
         <v>214</v>
@@ -48933,23 +48921,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="232"/>
-      <c r="B5" s="233"/>
+      <c r="A5" s="231"/>
+      <c r="B5" s="232"/>
       <c r="C5" s="210" t="s">
         <v>216</v>
       </c>
       <c r="D5" s="219" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E5" s="210" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F5" s="222" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="234" t="s">
+      <c r="A6" s="233" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48963,7 +48951,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="234"/>
+      <c r="A7" s="233"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48973,12 +48961,12 @@
       <c r="F7" s="131"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="234"/>
+      <c r="A8" s="233"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
       <c r="C8" s="107" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D8" s="120" t="s">
         <v>218</v>
@@ -48991,7 +48979,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="234"/>
+      <c r="A9" s="233"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -49003,7 +48991,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="234"/>
+      <c r="A10" s="233"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -49923,10 +49911,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="234" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="235"/>
+      <c r="B1" s="234"/>
       <c r="C1" s="17" t="s">
         <v>222</v>
       </c>
@@ -50093,10 +50081,10 @@
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="234" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="235"/>
+      <c r="B3" s="234"/>
       <c r="C3" s="185" t="s">
         <v>20</v>
       </c>
@@ -50180,10 +50168,10 @@
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="235" t="s">
+      <c r="A4" s="234" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="235"/>
+      <c r="B4" s="234"/>
       <c r="C4" s="65" t="s">
         <v>19</v>
       </c>
@@ -50267,8 +50255,8 @@
       </c>
     </row>
     <row r="5" spans="1:29" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="236"/>
-      <c r="B5" s="236"/>
+      <c r="A5" s="235"/>
+      <c r="B5" s="235"/>
       <c r="C5" s="225" t="s">
         <v>234</v>
       </c>
@@ -50352,7 +50340,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="236" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -50431,7 +50419,7 @@
       <c r="AC6" s="67"/>
     </row>
     <row r="7" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="237"/>
+      <c r="A7" s="236"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -50466,7 +50454,7 @@
       <c r="AC7" s="68"/>
     </row>
     <row r="8" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="237"/>
+      <c r="A8" s="236"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -50519,7 +50507,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="237"/>
+      <c r="A9" s="236"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -50598,7 +50586,7 @@
       <c r="AC9" s="71"/>
     </row>
     <row r="10" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="237"/>
+      <c r="A10" s="236"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -54140,10 +54128,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="234" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="235"/>
+      <c r="B1" s="234"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -54238,10 +54226,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="234" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="235"/>
+      <c r="B3" s="234"/>
       <c r="C3" s="15" t="s">
         <v>99</v>
       </c>
@@ -54289,10 +54277,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="235" t="s">
+      <c r="A4" s="234" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="235"/>
+      <c r="B4" s="234"/>
       <c r="C4" s="65" t="s">
         <v>278</v>
       </c>
@@ -54340,8 +54328,8 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="238"/>
-      <c r="B5" s="239"/>
+      <c r="A5" s="237"/>
+      <c r="B5" s="238"/>
       <c r="C5" s="223" t="s">
         <v>293</v>
       </c>
@@ -54389,7 +54377,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="236" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -54412,7 +54400,7 @@
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="237"/>
+      <c r="A7" s="236"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -54433,7 +54421,7 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="237"/>
+      <c r="A8" s="236"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -54478,7 +54466,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="237"/>
+      <c r="A9" s="236"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -54503,7 +54491,7 @@
       <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="237"/>
+      <c r="A10" s="236"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -56654,8 +56642,8 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56674,24 +56662,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="235" t="s">
+      <c r="A1" s="234" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="235"/>
+      <c r="B1" s="234"/>
       <c r="C1" s="65" t="s">
         <v>64</v>
       </c>
       <c r="D1" s="65" t="s">
+        <v>414</v>
+      </c>
+      <c r="E1" s="65" t="s">
         <v>415</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="F1" s="65" t="s">
+        <v>417</v>
+      </c>
+      <c r="G1" s="65" t="s">
         <v>416</v>
-      </c>
-      <c r="F1" s="65" t="s">
-        <v>418</v>
-      </c>
-      <c r="G1" s="65" t="s">
-        <v>417</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>114</v>
@@ -56748,10 +56736,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="234" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="235"/>
+      <c r="B3" s="234"/>
       <c r="C3" s="64" t="s">
         <v>65</v>
       </c>
@@ -56787,24 +56775,24 @@
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A4" s="235" t="s">
+      <c r="A4" s="234" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="235"/>
+      <c r="B4" s="234"/>
       <c r="C4" s="65" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="65" t="s">
+        <v>414</v>
+      </c>
+      <c r="E4" s="65" t="s">
         <v>415</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="F4" s="65" t="s">
+        <v>417</v>
+      </c>
+      <c r="G4" s="65" t="s">
         <v>416</v>
-      </c>
-      <c r="F4" s="65" t="s">
-        <v>418</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>417</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>114</v>
@@ -56826,42 +56814,42 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="238"/>
-      <c r="B5" s="238"/>
+      <c r="A5" s="237"/>
+      <c r="B5" s="237"/>
       <c r="C5" s="211" t="s">
+        <v>432</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>420</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>421</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>422</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>423</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>424</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>425</v>
+      </c>
+      <c r="J5" s="56" t="s">
         <v>340</v>
       </c>
-      <c r="D5" s="37" t="s">
-        <v>421</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>422</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>423</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>424</v>
-      </c>
-      <c r="H5" s="37" t="s">
+      <c r="K5" s="56" t="s">
+        <v>341</v>
+      </c>
+      <c r="L5" s="37" t="s">
         <v>426</v>
       </c>
-      <c r="I5" s="37" t="s">
-        <v>427</v>
-      </c>
-      <c r="J5" s="56" t="s">
-        <v>341</v>
-      </c>
-      <c r="K5" s="56" t="s">
-        <v>342</v>
-      </c>
-      <c r="L5" s="37" t="s">
-        <v>428</v>
-      </c>
       <c r="M5" s="56"/>
     </row>
     <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="236" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -56880,7 +56868,7 @@
       <c r="M6" s="67"/>
     </row>
     <row r="7" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="237"/>
+      <c r="A7" s="236"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -56897,7 +56885,7 @@
       <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="237"/>
+      <c r="A8" s="236"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -56905,36 +56893,36 @@
         <v>262</v>
       </c>
       <c r="D8" s="69" t="s">
+        <v>342</v>
+      </c>
+      <c r="E8" s="69" t="s">
         <v>343</v>
       </c>
-      <c r="E8" s="69" t="s">
-        <v>344</v>
-      </c>
       <c r="F8" s="69" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="230" t="s">
-        <v>425</v>
-      </c>
-      <c r="I8" s="230" t="s">
-        <v>425</v>
+      <c r="H8" s="69">
+        <v>2</v>
+      </c>
+      <c r="I8" s="69" t="s">
+        <v>75</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="L8" s="230" t="s">
-        <v>425</v>
+        <v>344</v>
+      </c>
+      <c r="L8" s="69">
+        <v>2</v>
       </c>
       <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="237"/>
+      <c r="A9" s="236"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -56951,7 +56939,7 @@
       <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="237"/>
+      <c r="A10" s="236"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -58630,84 +58618,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D1" s="57" t="s">
+        <v>346</v>
+      </c>
+      <c r="E1" s="57" t="s">
         <v>347</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="F1" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="G1" s="57" t="s">
         <v>349</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="H1" s="57" t="s">
         <v>350</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="I1" s="57" t="s">
         <v>351</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="J1" s="57" t="s">
         <v>352</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>353</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="L1" s="57" t="s">
         <v>354</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="M1" s="57" t="s">
         <v>355</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="228" t="s">
+        <v>407</v>
+      </c>
+      <c r="B2" s="177" t="s">
         <v>408</v>
       </c>
-      <c r="B2" s="177" t="s">
-        <v>409</v>
-      </c>
       <c r="C2" s="177" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D2" s="83" t="s">
+        <v>356</v>
+      </c>
+      <c r="E2" s="83" t="s">
         <v>357</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="F2" s="83" t="s">
         <v>358</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="G2" s="83" t="s">
         <v>359</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="H2" s="83" t="s">
         <v>360</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="I2" s="83" t="s">
         <v>361</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="J2" s="83" t="s">
         <v>362</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="K2" s="83" t="s">
         <v>363</v>
       </c>
-      <c r="K2" s="83" t="s">
+      <c r="L2" s="83" t="s">
         <v>364</v>
       </c>
-      <c r="L2" s="83" t="s">
+      <c r="M2" s="83" t="s">
         <v>365</v>
-      </c>
-      <c r="M2" s="83" t="s">
-        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -58717,6 +58705,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
@@ -58725,15 +58722,6 @@
     <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58954,20 +58942,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
     <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
bandgap curve mesaurements and scripts added
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab2\Documents\projects\IVM6311\IVM6311ATE-flavio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E027041B-21DF-48F1-AC32-F944B5AE7552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F803152C-DD64-4908-8571-BBAB68885745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="3" r:id="rId1"/>
@@ -39621,9 +39621,6 @@
 Measure__current__VBAT</t>
   </si>
   <si>
-    <t>TO BE DONE</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="16"/>
@@ -43647,6 +43644,9 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -45778,177 +45778,177 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>366</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>368</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23" t="s">
+        <v>374</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>375</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="G6" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="24" t="s">
         <v>377</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="J6" s="25" t="s">
         <v>378</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="K6" s="58" t="s">
         <v>379</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="58" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="23" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>385</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>386</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="J9" s="25" t="s">
         <v>387</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="J10" s="25" t="s">
         <v>389</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="J11" s="25" t="s">
         <v>391</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>393</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="J13" s="25" t="s">
         <v>395</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="J14" s="25" t="s">
         <v>397</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="J15" s="25" t="s">
         <v>399</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="J16" s="25" t="s">
         <v>401</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="J17" s="25" t="s">
         <v>403</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="J18" s="25" t="s">
         <v>405</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -46858,7 +46858,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="230" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B1" s="230"/>
       <c r="C1" s="9" t="s">
@@ -46930,16 +46930,16 @@
       <c r="A5" s="231"/>
       <c r="B5" s="232"/>
       <c r="C5" s="220" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D5" s="207" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E5" s="207" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F5" s="192" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
@@ -46954,7 +46954,7 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F6" s="67"/>
     </row>
@@ -48861,7 +48861,7 @@
         <v>213</v>
       </c>
       <c r="D1" s="117" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E1" s="229" t="s">
         <v>214</v>
@@ -48911,7 +48911,7 @@
         <v>213</v>
       </c>
       <c r="D4" s="117" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E4" s="104" t="s">
         <v>214</v>
@@ -48927,10 +48927,10 @@
         <v>216</v>
       </c>
       <c r="D5" s="219" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E5" s="210" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F5" s="222" t="s">
         <v>217</v>
@@ -48966,7 +48966,7 @@
         <v>149</v>
       </c>
       <c r="C8" s="107" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D8" s="120" t="s">
         <v>218</v>
@@ -54107,8 +54107,8 @@
   </sheetPr>
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54358,22 +54358,22 @@
         <v>301</v>
       </c>
       <c r="L5" s="206" t="s">
+        <v>432</v>
+      </c>
+      <c r="M5" s="205" t="s">
         <v>302</v>
       </c>
-      <c r="M5" s="205" t="s">
+      <c r="N5" s="205" t="s">
         <v>303</v>
       </c>
-      <c r="N5" s="205" t="s">
+      <c r="O5" s="205" t="s">
         <v>304</v>
       </c>
-      <c r="O5" s="205" t="s">
+      <c r="P5" s="205" t="s">
         <v>305</v>
       </c>
-      <c r="P5" s="205" t="s">
+      <c r="Q5" s="205" t="s">
         <v>306</v>
-      </c>
-      <c r="Q5" s="205" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -54428,41 +54428,41 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="N8" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="O8" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>312</v>
-      </c>
-      <c r="Q8" s="11" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -54474,7 +54474,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E9" s="71"/>
       <c r="F9" s="71"/>
@@ -54517,47 +54517,47 @@
         <v>156</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>316</v>
-      </c>
       <c r="G11" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5" t="s">
         <v>267</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>157</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -54877,13 +54877,13 @@
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="50" t="s">
+        <v>318</v>
+      </c>
+      <c r="E20" s="50" t="s">
         <v>319</v>
       </c>
-      <c r="E20" s="50" t="s">
-        <v>320</v>
-      </c>
       <c r="F20" s="50" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G20" s="89"/>
       <c r="I20" s="76"/>
@@ -54904,29 +54904,29 @@
         <v>186</v>
       </c>
       <c r="C21" s="50" t="s">
+        <v>320</v>
+      </c>
+      <c r="D21" s="50" t="s">
         <v>321</v>
       </c>
-      <c r="D21" s="50" t="s">
+      <c r="E21" s="50" t="s">
         <v>322</v>
-      </c>
-      <c r="E21" s="50" t="s">
-        <v>323</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="50" t="s">
+        <v>323</v>
+      </c>
+      <c r="H21" s="50" t="s">
         <v>324</v>
       </c>
-      <c r="H21" s="50" t="s">
+      <c r="I21" s="76" t="s">
         <v>325</v>
       </c>
-      <c r="I21" s="76" t="s">
-        <v>326</v>
-      </c>
       <c r="J21" s="76" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K21" s="76" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L21" s="76"/>
       <c r="M21" s="50"/>
@@ -54943,31 +54943,31 @@
         <v>188</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D22" s="50" t="s">
+        <v>326</v>
+      </c>
+      <c r="E22" s="50" t="s">
         <v>327</v>
       </c>
-      <c r="E22" s="50" t="s">
+      <c r="F22" s="50" t="s">
+        <v>327</v>
+      </c>
+      <c r="G22" s="50" t="s">
         <v>328</v>
       </c>
-      <c r="F22" s="50" t="s">
-        <v>328</v>
-      </c>
-      <c r="G22" s="50" t="s">
+      <c r="H22" s="50" t="s">
         <v>329</v>
       </c>
-      <c r="H22" s="50" t="s">
+      <c r="I22" s="76" t="s">
         <v>330</v>
       </c>
-      <c r="I22" s="76" t="s">
+      <c r="J22" s="76" t="s">
         <v>331</v>
       </c>
-      <c r="J22" s="76" t="s">
+      <c r="K22" s="76" t="s">
         <v>332</v>
-      </c>
-      <c r="K22" s="76" t="s">
-        <v>333</v>
       </c>
       <c r="L22" s="76"/>
       <c r="M22" s="50"/>
@@ -55053,31 +55053,31 @@
         <v>197</v>
       </c>
       <c r="C26" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="E26" s="50" t="s">
         <v>334</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="F26" s="50" t="s">
         <v>334</v>
       </c>
-      <c r="E26" s="50" t="s">
-        <v>335</v>
-      </c>
-      <c r="F26" s="50" t="s">
-        <v>335</v>
-      </c>
       <c r="G26" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I26" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J26" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K26" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L26" s="50"/>
       <c r="M26" s="50"/>
@@ -55094,31 +55094,31 @@
         <v>199</v>
       </c>
       <c r="C27" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="E27" s="50" t="s">
         <v>334</v>
       </c>
-      <c r="D27" s="50" t="s">
+      <c r="F27" s="50" t="s">
         <v>334</v>
       </c>
-      <c r="E27" s="50" t="s">
-        <v>335</v>
-      </c>
-      <c r="F27" s="50" t="s">
-        <v>335</v>
-      </c>
       <c r="G27" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I27" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J27" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K27" s="50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L27" s="50"/>
       <c r="M27" s="50"/>
@@ -56642,7 +56642,7 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -56670,16 +56670,16 @@
         <v>64</v>
       </c>
       <c r="D1" s="65" t="s">
+        <v>413</v>
+      </c>
+      <c r="E1" s="65" t="s">
         <v>414</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="F1" s="65" t="s">
+        <v>416</v>
+      </c>
+      <c r="G1" s="65" t="s">
         <v>415</v>
-      </c>
-      <c r="F1" s="65" t="s">
-        <v>417</v>
-      </c>
-      <c r="G1" s="65" t="s">
-        <v>416</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>114</v>
@@ -56688,16 +56688,16 @@
         <v>118</v>
       </c>
       <c r="J1" s="65" t="s">
+        <v>336</v>
+      </c>
+      <c r="K1" s="65" t="s">
         <v>337</v>
-      </c>
-      <c r="K1" s="65" t="s">
-        <v>338</v>
       </c>
       <c r="L1" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M1" s="95" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
@@ -56771,7 +56771,7 @@
         <v>36</v>
       </c>
       <c r="M3" s="64" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
@@ -56783,16 +56783,16 @@
         <v>64</v>
       </c>
       <c r="D4" s="65" t="s">
+        <v>413</v>
+      </c>
+      <c r="E4" s="65" t="s">
         <v>414</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="F4" s="65" t="s">
+        <v>416</v>
+      </c>
+      <c r="G4" s="65" t="s">
         <v>415</v>
-      </c>
-      <c r="F4" s="65" t="s">
-        <v>417</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>416</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>114</v>
@@ -56801,50 +56801,50 @@
         <v>118</v>
       </c>
       <c r="J4" s="65" t="s">
+        <v>336</v>
+      </c>
+      <c r="K4" s="65" t="s">
         <v>337</v>
-      </c>
-      <c r="K4" s="65" t="s">
-        <v>338</v>
       </c>
       <c r="L4" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M4" s="95" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="237"/>
       <c r="B5" s="237"/>
       <c r="C5" s="211" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D5" s="37" t="s">
+        <v>419</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>420</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="F5" s="37" t="s">
         <v>421</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="G5" s="37" t="s">
         <v>422</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="H5" s="37" t="s">
         <v>423</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="I5" s="37" t="s">
         <v>424</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="J5" s="56" t="s">
+        <v>339</v>
+      </c>
+      <c r="K5" s="56" t="s">
+        <v>340</v>
+      </c>
+      <c r="L5" s="37" t="s">
         <v>425</v>
-      </c>
-      <c r="J5" s="56" t="s">
-        <v>340</v>
-      </c>
-      <c r="K5" s="56" t="s">
-        <v>341</v>
-      </c>
-      <c r="L5" s="37" t="s">
-        <v>426</v>
       </c>
       <c r="M5" s="56"/>
     </row>
@@ -56893,13 +56893,13 @@
         <v>262</v>
       </c>
       <c r="D8" s="69" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" s="69" t="s">
         <v>342</v>
       </c>
-      <c r="E8" s="69" t="s">
-        <v>343</v>
-      </c>
       <c r="F8" s="69" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>20</v>
@@ -56911,10 +56911,10 @@
         <v>75</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L8" s="69">
         <v>2</v>
@@ -58601,7 +58601,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58618,84 +58618,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D1" s="57" t="s">
+        <v>345</v>
+      </c>
+      <c r="E1" s="57" t="s">
         <v>346</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="F1" s="57" t="s">
         <v>347</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="G1" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="H1" s="57" t="s">
         <v>349</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="I1" s="57" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="J1" s="57" t="s">
         <v>351</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>352</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="L1" s="57" t="s">
         <v>353</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="M1" s="57" t="s">
         <v>354</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="228" t="s">
+        <v>406</v>
+      </c>
+      <c r="B2" s="177" t="s">
         <v>407</v>
       </c>
-      <c r="B2" s="177" t="s">
-        <v>408</v>
-      </c>
       <c r="C2" s="177" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D2" s="83" t="s">
+        <v>355</v>
+      </c>
+      <c r="E2" s="83" t="s">
         <v>356</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="F2" s="83" t="s">
         <v>357</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="G2" s="83" t="s">
         <v>358</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="H2" s="83" t="s">
         <v>359</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="I2" s="83" t="s">
         <v>360</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="J2" s="83" t="s">
         <v>361</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="K2" s="83" t="s">
         <v>362</v>
       </c>
-      <c r="K2" s="83" t="s">
+      <c r="L2" s="83" t="s">
         <v>363</v>
       </c>
-      <c r="L2" s="83" t="s">
+      <c r="M2" s="83" t="s">
         <v>364</v>
-      </c>
-      <c r="M2" s="83" t="s">
-        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -58705,15 +58705,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
@@ -58722,6 +58713,15 @@
     <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58942,20 +58942,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
     <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
update the AZ_comp class, now is working
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab2\Documents\projects\IVM6311\IVM6311ATE-flavio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F803152C-DD64-4908-8571-BBAB68885745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6470645E-0E7C-48F1-A723-79815405F839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="28770" windowHeight="15600" tabRatio="693" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="433">
   <si>
     <t>Revision</t>
   </si>
@@ -39460,92 +39460,6 @@
 </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Run__DAC-PA TDM_768_IN_and_Path_generator
-Measure__THD__OUTP__OUTN
-Measure__flatness__OUTP__OUTN
-Measure__PSRR__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "in test page"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1E_0xF8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "set enable and gain = -61dB (Gains from-1dB to -61dB step -6) anf freq=1kHz (available freq: 1-2-4-8-16kHz)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "in base page"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Measure__noise__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Run__DAC-PA ANALOG_IN_DC_COUPLED
 ForceANA__-6_1000
 Measure__THD__OUTP__OUTN
@@ -40511,179 +40425,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">"OUTN_INT_PRT analog test point"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Return page 0"
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run__startup </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Select page 1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  
-0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x0E </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"OUTP_EXT_PRT analog test point"
 </t>
     </r>
     <r>
@@ -42857,190 +42598,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run__startup </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                                                                 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Select page 1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  
-0x17_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force_dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x18_0x02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig_azcomp_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0xC8 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" force otp and mod clock on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x10_0x08 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19_0x88  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"test analog azcomp enable"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x0F </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"VCM_AVDD analog test point"
- "Measure Voltage between SDWN pin and GND, you should measure VBAT/2"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF92D050"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">"Run__startup
 Run__Boost_test_default
 Wait__delay__0.1ms
@@ -43648,6 +43205,529 @@
   <si>
     <t xml:space="preserve">    </t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run__startup </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  
+0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run__Enable_Ana_Testpoint_AZ_comp</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x0F </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"VCM_AVDD analog test point"
+ "Measure Voltage between SDWN pin and GND, you should measure VBAT/2"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage_SDWN  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run__startup </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  
+0x17_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force_dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x18_0x02 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig_azcomp_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0xC8 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" force otp and mod clock on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x10_0x08 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force ref_sdwn_b_dis_m"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19_0x88  </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"test analog azcomp enable"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x0E </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"OUTP_EXT_PRT analog test point"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Return page 0"
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run__DAC-PA TDM_768_IN_and_Path_generator
+Measure__THD__OUTP__OUTN
+Measure__flatness__OUTP__OUTN
+Measure__PSRR__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "in test page"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1E_0xF8</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "set enable and gain = -61dB (Gains from-1dB to -61dB step -6) anf freq=1kHz (available freq: 1-2-4-8-16kHz)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "in base page"</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Measure__noise__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -43657,7 +43737,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="111" x14ac:knownFonts="1">
+  <fonts count="117" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44356,6 +44436,53 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FFFF3399"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FFFF33CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -44761,7 +44888,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -45338,6 +45465,9 @@
     <xf numFmtId="49" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="111" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -45365,10 +45495,13 @@
     <xf numFmtId="3" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="114" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -45778,177 +45911,177 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23" t="s">
+        <v>372</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>374</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="H6" s="24" t="s">
         <v>375</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="J6" s="25" t="s">
         <v>376</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="K6" s="58" t="s">
         <v>377</v>
-      </c>
-      <c r="J6" s="25" t="s">
-        <v>378</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="58" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="23" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="G8" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>383</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>384</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>385</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -46857,10 +46990,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="230" t="s">
-        <v>408</v>
-      </c>
-      <c r="B1" s="230"/>
+      <c r="A1" s="231" t="s">
+        <v>406</v>
+      </c>
+      <c r="B1" s="231"/>
       <c r="C1" s="9" t="s">
         <v>142</v>
       </c>
@@ -46891,10 +47024,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="231" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="230"/>
+      <c r="B3" s="231"/>
       <c r="C3" s="15" t="s">
         <v>60</v>
       </c>
@@ -46909,10 +47042,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="231" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="230"/>
+      <c r="B4" s="231"/>
       <c r="C4" s="9" t="s">
         <v>142</v>
       </c>
@@ -46927,23 +47060,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="231"/>
-      <c r="B5" s="232"/>
+      <c r="A5" s="232"/>
+      <c r="B5" s="233"/>
       <c r="C5" s="220" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D5" s="207" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E5" s="207" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F5" s="192" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="233" t="s">
+      <c r="A6" s="234" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -46954,12 +47087,12 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F6" s="67"/>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="233"/>
+      <c r="A7" s="234"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -46971,7 +47104,7 @@
       <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="233"/>
+      <c r="A8" s="234"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -46987,7 +47120,7 @@
       <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="233"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -46999,7 +47132,7 @@
       <c r="F9" s="71"/>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="233"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -47926,10 +48059,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="230" t="s">
+      <c r="A1" s="231" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="230"/>
+      <c r="B1" s="231"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -47960,10 +48093,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="231" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="230"/>
+      <c r="B3" s="231"/>
       <c r="C3" s="15" t="s">
         <v>79</v>
       </c>
@@ -47978,10 +48111,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="231" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="230"/>
+      <c r="B4" s="231"/>
       <c r="C4" s="9" t="s">
         <v>202</v>
       </c>
@@ -47996,8 +48129,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="273" x14ac:dyDescent="0.25">
-      <c r="A5" s="231"/>
-      <c r="B5" s="232"/>
+      <c r="A5" s="232"/>
+      <c r="B5" s="233"/>
       <c r="C5" s="37" t="s">
         <v>206</v>
       </c>
@@ -48012,7 +48145,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="233" t="s">
+      <c r="A6" s="234" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48030,7 +48163,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="233"/>
+      <c r="A7" s="234"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48046,7 +48179,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="233"/>
+      <c r="A8" s="234"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -48064,7 +48197,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="233"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -48080,7 +48213,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="233"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -48853,15 +48986,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="230" t="s">
+      <c r="A1" s="231" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="230"/>
+      <c r="B1" s="231"/>
       <c r="C1" s="104" t="s">
         <v>213</v>
       </c>
       <c r="D1" s="117" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E1" s="229" t="s">
         <v>214</v>
@@ -48885,10 +49018,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="230" t="s">
+      <c r="A3" s="231" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="230"/>
+      <c r="B3" s="231"/>
       <c r="C3" s="103" t="s">
         <v>20</v>
       </c>
@@ -48903,15 +49036,15 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="230" t="s">
+      <c r="A4" s="231" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="230"/>
+      <c r="B4" s="231"/>
       <c r="C4" s="104" t="s">
         <v>213</v>
       </c>
       <c r="D4" s="117" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E4" s="104" t="s">
         <v>214</v>
@@ -48921,23 +49054,23 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="231"/>
-      <c r="B5" s="232"/>
+      <c r="A5" s="232"/>
+      <c r="B5" s="233"/>
       <c r="C5" s="210" t="s">
         <v>216</v>
       </c>
       <c r="D5" s="219" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E5" s="210" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F5" s="222" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="233" t="s">
+      <c r="A6" s="234" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48951,7 +49084,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="233"/>
+      <c r="A7" s="234"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48961,12 +49094,12 @@
       <c r="F7" s="131"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="233"/>
+      <c r="A8" s="234"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
       <c r="C8" s="107" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D8" s="120" t="s">
         <v>218</v>
@@ -48979,7 +49112,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="233"/>
+      <c r="A9" s="234"/>
       <c r="B9" s="12" t="s">
         <v>152</v>
       </c>
@@ -48991,7 +49124,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="233"/>
+      <c r="A10" s="234"/>
       <c r="B10" s="14" t="s">
         <v>154</v>
       </c>
@@ -49911,10 +50044,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="234" t="s">
+      <c r="A1" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="234"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="17" t="s">
         <v>222</v>
       </c>
@@ -50081,10 +50214,10 @@
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="234" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="234"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="185" t="s">
         <v>20</v>
       </c>
@@ -50168,10 +50301,10 @@
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="234" t="s">
+      <c r="A4" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="234"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="65" t="s">
         <v>19</v>
       </c>
@@ -50255,8 +50388,8 @@
       </c>
     </row>
     <row r="5" spans="1:29" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="235"/>
-      <c r="B5" s="235"/>
+      <c r="A5" s="236"/>
+      <c r="B5" s="236"/>
       <c r="C5" s="225" t="s">
         <v>234</v>
       </c>
@@ -50340,7 +50473,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -50419,7 +50552,7 @@
       <c r="AC6" s="67"/>
     </row>
     <row r="7" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="236"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -50454,7 +50587,7 @@
       <c r="AC7" s="68"/>
     </row>
     <row r="8" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="236"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -50507,7 +50640,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="236"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -50586,7 +50719,7 @@
       <c r="AC9" s="71"/>
     </row>
     <row r="10" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="236"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -54107,8 +54240,8 @@
   </sheetPr>
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54128,10 +54261,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="234" t="s">
+      <c r="A1" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="234"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -54226,10 +54359,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="234" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="234"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="15" t="s">
         <v>99</v>
       </c>
@@ -54277,10 +54410,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="234" t="s">
+      <c r="A4" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="234"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="65" t="s">
         <v>278</v>
       </c>
@@ -54328,8 +54461,8 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="237"/>
-      <c r="B5" s="238"/>
+      <c r="A5" s="238"/>
+      <c r="B5" s="239"/>
       <c r="C5" s="223" t="s">
         <v>293</v>
       </c>
@@ -54339,45 +54472,45 @@
       <c r="E5" s="206" t="s">
         <v>295</v>
       </c>
-      <c r="F5" s="206" t="s">
+      <c r="F5" s="240" t="s">
+        <v>432</v>
+      </c>
+      <c r="G5" s="206" t="s">
         <v>296</v>
       </c>
-      <c r="G5" s="206" t="s">
+      <c r="H5" s="206" t="s">
         <v>297</v>
       </c>
-      <c r="H5" s="206" t="s">
+      <c r="I5" s="206" t="s">
         <v>298</v>
       </c>
-      <c r="I5" s="206" t="s">
+      <c r="J5" s="206" t="s">
         <v>299</v>
       </c>
-      <c r="J5" s="206" t="s">
+      <c r="K5" s="206" t="s">
         <v>300</v>
       </c>
-      <c r="K5" s="206" t="s">
+      <c r="L5" s="206" t="s">
+        <v>429</v>
+      </c>
+      <c r="M5" s="205" t="s">
         <v>301</v>
       </c>
-      <c r="L5" s="206" t="s">
-        <v>432</v>
-      </c>
-      <c r="M5" s="205" t="s">
+      <c r="N5" s="205" t="s">
         <v>302</v>
       </c>
-      <c r="N5" s="205" t="s">
+      <c r="O5" s="205" t="s">
         <v>303</v>
       </c>
-      <c r="O5" s="205" t="s">
+      <c r="P5" s="205" t="s">
         <v>304</v>
       </c>
-      <c r="P5" s="205" t="s">
+      <c r="Q5" s="205" t="s">
         <v>305</v>
       </c>
-      <c r="Q5" s="205" t="s">
-        <v>306</v>
-      </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -54400,7 +54533,7 @@
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="236"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -54421,52 +54554,52 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="236"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="N8" s="11" t="s">
         <v>308</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="O8" s="11" t="s">
         <v>309</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="Q8" s="11" t="s">
-        <v>312</v>
-      </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="236"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -54474,7 +54607,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E9" s="71"/>
       <c r="F9" s="71"/>
@@ -54491,7 +54624,7 @@
       <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="236"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -54517,47 +54650,47 @@
         <v>156</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>315</v>
-      </c>
       <c r="G11" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5" t="s">
         <v>267</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>157</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -54877,13 +55010,13 @@
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="50" t="s">
+        <v>317</v>
+      </c>
+      <c r="E20" s="50" t="s">
         <v>318</v>
       </c>
-      <c r="E20" s="50" t="s">
-        <v>319</v>
-      </c>
       <c r="F20" s="50" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G20" s="89"/>
       <c r="I20" s="76"/>
@@ -54904,29 +55037,29 @@
         <v>186</v>
       </c>
       <c r="C21" s="50" t="s">
+        <v>319</v>
+      </c>
+      <c r="D21" s="50" t="s">
         <v>320</v>
       </c>
-      <c r="D21" s="50" t="s">
+      <c r="E21" s="50" t="s">
         <v>321</v>
-      </c>
-      <c r="E21" s="50" t="s">
-        <v>322</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="50" t="s">
+        <v>322</v>
+      </c>
+      <c r="H21" s="50" t="s">
         <v>323</v>
       </c>
-      <c r="H21" s="50" t="s">
+      <c r="I21" s="76" t="s">
         <v>324</v>
       </c>
-      <c r="I21" s="76" t="s">
-        <v>325</v>
-      </c>
       <c r="J21" s="76" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K21" s="76" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L21" s="76"/>
       <c r="M21" s="50"/>
@@ -54943,31 +55076,31 @@
         <v>188</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D22" s="50" t="s">
+        <v>325</v>
+      </c>
+      <c r="E22" s="50" t="s">
         <v>326</v>
       </c>
-      <c r="E22" s="50" t="s">
+      <c r="F22" s="50" t="s">
+        <v>326</v>
+      </c>
+      <c r="G22" s="50" t="s">
         <v>327</v>
       </c>
-      <c r="F22" s="50" t="s">
-        <v>327</v>
-      </c>
-      <c r="G22" s="50" t="s">
+      <c r="H22" s="50" t="s">
         <v>328</v>
       </c>
-      <c r="H22" s="50" t="s">
+      <c r="I22" s="76" t="s">
         <v>329</v>
       </c>
-      <c r="I22" s="76" t="s">
+      <c r="J22" s="76" t="s">
         <v>330</v>
       </c>
-      <c r="J22" s="76" t="s">
+      <c r="K22" s="76" t="s">
         <v>331</v>
-      </c>
-      <c r="K22" s="76" t="s">
-        <v>332</v>
       </c>
       <c r="L22" s="76"/>
       <c r="M22" s="50"/>
@@ -55053,31 +55186,31 @@
         <v>197</v>
       </c>
       <c r="C26" s="50" t="s">
+        <v>332</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>332</v>
+      </c>
+      <c r="E26" s="50" t="s">
         <v>333</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="F26" s="50" t="s">
         <v>333</v>
       </c>
-      <c r="E26" s="50" t="s">
-        <v>334</v>
-      </c>
-      <c r="F26" s="50" t="s">
-        <v>334</v>
-      </c>
       <c r="G26" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I26" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J26" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K26" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L26" s="50"/>
       <c r="M26" s="50"/>
@@ -55094,31 +55227,31 @@
         <v>199</v>
       </c>
       <c r="C27" s="50" t="s">
+        <v>332</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>332</v>
+      </c>
+      <c r="E27" s="50" t="s">
         <v>333</v>
       </c>
-      <c r="D27" s="50" t="s">
+      <c r="F27" s="50" t="s">
         <v>333</v>
       </c>
-      <c r="E27" s="50" t="s">
-        <v>334</v>
-      </c>
-      <c r="F27" s="50" t="s">
-        <v>334</v>
-      </c>
       <c r="G27" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I27" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J27" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K27" s="50" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L27" s="50"/>
       <c r="M27" s="50"/>
@@ -56642,8 +56775,8 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56662,24 +56795,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="234" t="s">
+      <c r="A1" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="234"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="65" t="s">
         <v>64</v>
       </c>
       <c r="D1" s="65" t="s">
+        <v>411</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>412</v>
+      </c>
+      <c r="F1" s="65" t="s">
+        <v>414</v>
+      </c>
+      <c r="G1" s="65" t="s">
         <v>413</v>
-      </c>
-      <c r="E1" s="65" t="s">
-        <v>414</v>
-      </c>
-      <c r="F1" s="65" t="s">
-        <v>416</v>
-      </c>
-      <c r="G1" s="65" t="s">
-        <v>415</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>114</v>
@@ -56688,16 +56821,16 @@
         <v>118</v>
       </c>
       <c r="J1" s="65" t="s">
+        <v>335</v>
+      </c>
+      <c r="K1" s="65" t="s">
         <v>336</v>
-      </c>
-      <c r="K1" s="65" t="s">
-        <v>337</v>
       </c>
       <c r="L1" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M1" s="95" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
@@ -56736,10 +56869,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="234" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="234"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="64" t="s">
         <v>65</v>
       </c>
@@ -56771,28 +56904,28 @@
         <v>36</v>
       </c>
       <c r="M3" s="64" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A4" s="234" t="s">
+      <c r="A4" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="234"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="65" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="65" t="s">
+        <v>411</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>412</v>
+      </c>
+      <c r="F4" s="65" t="s">
+        <v>414</v>
+      </c>
+      <c r="G4" s="65" t="s">
         <v>413</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>414</v>
-      </c>
-      <c r="F4" s="65" t="s">
-        <v>416</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>415</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>114</v>
@@ -56801,55 +56934,55 @@
         <v>118</v>
       </c>
       <c r="J4" s="65" t="s">
+        <v>335</v>
+      </c>
+      <c r="K4" s="65" t="s">
         <v>336</v>
-      </c>
-      <c r="K4" s="65" t="s">
-        <v>337</v>
       </c>
       <c r="L4" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M4" s="95" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="238"/>
+      <c r="B5" s="238"/>
+      <c r="C5" s="211" t="s">
+        <v>428</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>417</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>418</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>419</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>420</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>421</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>422</v>
+      </c>
+      <c r="J5" s="56" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="237"/>
-      <c r="B5" s="237"/>
-      <c r="C5" s="211" t="s">
+      <c r="K5" s="230" t="s">
         <v>431</v>
       </c>
-      <c r="D5" s="37" t="s">
-        <v>419</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>420</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>421</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>422</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>423</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>424</v>
-      </c>
-      <c r="J5" s="56" t="s">
-        <v>339</v>
-      </c>
-      <c r="K5" s="56" t="s">
-        <v>340</v>
-      </c>
-      <c r="L5" s="37" t="s">
-        <v>425</v>
+      <c r="L5" s="230" t="s">
+        <v>430</v>
       </c>
       <c r="M5" s="56"/>
     </row>
     <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -56868,7 +57001,7 @@
       <c r="M6" s="67"/>
     </row>
     <row r="7" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="236"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -56885,7 +57018,7 @@
       <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="236"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -56893,36 +57026,36 @@
         <v>262</v>
       </c>
       <c r="D8" s="69" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E8" s="69" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="69">
-        <v>2</v>
-      </c>
-      <c r="I8" s="69" t="s">
+      <c r="H8" s="11" t="s">
         <v>75</v>
       </c>
+      <c r="I8" s="11" t="s">
+        <v>75</v>
+      </c>
       <c r="J8" s="69" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="L8" s="69">
-        <v>2</v>
+        <v>341</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="236"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="62" t="s">
         <v>152</v>
       </c>
@@ -56939,7 +57072,7 @@
       <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="236"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="60" t="s">
         <v>154</v>
       </c>
@@ -58618,84 +58751,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D1" s="57" t="s">
+        <v>343</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>344</v>
+      </c>
+      <c r="F1" s="57" t="s">
         <v>345</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="G1" s="57" t="s">
         <v>346</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="H1" s="57" t="s">
         <v>347</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="I1" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="J1" s="57" t="s">
         <v>349</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>350</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="L1" s="57" t="s">
         <v>351</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="M1" s="57" t="s">
         <v>352</v>
-      </c>
-      <c r="L1" s="57" t="s">
-        <v>353</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="228" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B2" s="177" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C2" s="177" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D2" s="83" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" s="83" t="s">
+        <v>354</v>
+      </c>
+      <c r="F2" s="83" t="s">
         <v>355</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="G2" s="83" t="s">
         <v>356</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="H2" s="83" t="s">
         <v>357</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="I2" s="83" t="s">
         <v>358</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="J2" s="83" t="s">
         <v>359</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="K2" s="83" t="s">
         <v>360</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="L2" s="83" t="s">
         <v>361</v>
       </c>
-      <c r="K2" s="83" t="s">
+      <c r="M2" s="83" t="s">
         <v>362</v>
-      </c>
-      <c r="L2" s="83" t="s">
-        <v>363</v>
-      </c>
-      <c r="M2" s="83" t="s">
-        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added reference class, with trimm sweep and function that find the best value, bandgap working, others trimming not
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139D3FF0-9573-4C24-A428-03E42DF4A44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A226B56-6598-447A-8D89-197A59626DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42638,16 +42638,6 @@
 0xFE_0x00 "Return page 0"</t>
   </si>
   <si>
-    <t>Run__Startup
-Run__Enable_Ana_Testpoint
-0xFE_0x01 "Select page 1"
-0x1A_0x01 "Bandgap"
-Measure__Voltage__SDWN
-Trim__0xB0[7:4] "Select code which sets ATEST voltage as close as possible to target"
-Calculate__MinError
-0xFE_0x00 "Return page 0"</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Run_startup  
 </t>
@@ -43721,6 +43711,16 @@
   </si>
   <si>
     <t>0.542</t>
+  </si>
+  <si>
+    <t>Run__Startup
+Run__Enable_Ana_Testpoint
+0xFE_0x01 "Select page 1"
+0x1A_0x01 "Bandgap"
+0xB0__0x0E
+Trim__0xB0[7:4] "Select code which sets ATEST voltage as close as possible to target"
+Calculate__MinError
+0xFE_0x00 "Return page 0"</t>
   </si>
 </sst>
 </file>
@@ -44897,7 +44897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="246">
+  <cellXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -45444,9 +45444,6 @@
     <xf numFmtId="49" fontId="14" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -45480,6 +45477,18 @@
     <xf numFmtId="49" fontId="114" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="118" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -45487,6 +45496,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -45505,21 +45517,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="117" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="118" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -46204,7 +46201,7 @@
       <c r="F3" s="151" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="226" t="s">
+      <c r="G3" s="225" t="s">
         <v>21</v>
       </c>
       <c r="H3" s="213" t="s">
@@ -46230,7 +46227,7 @@
       <c r="F4" s="188" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="227" t="s">
+      <c r="G4" s="226" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="186" t="s">
@@ -46256,7 +46253,7 @@
       <c r="F5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="225" t="s">
+      <c r="G5" s="224" t="s">
         <v>29</v>
       </c>
       <c r="H5" s="186" t="s">
@@ -46282,7 +46279,7 @@
       <c r="F6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="225" t="s">
+      <c r="G6" s="224" t="s">
         <v>33</v>
       </c>
       <c r="H6" s="186" t="s">
@@ -46308,10 +46305,10 @@
       <c r="F7" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="225" t="s">
+      <c r="G7" s="224" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="225" t="s">
+      <c r="H7" s="224" t="s">
         <v>38</v>
       </c>
     </row>
@@ -46386,7 +46383,7 @@
       <c r="F10" s="190" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="225" t="s">
+      <c r="G10" s="224" t="s">
         <v>49</v>
       </c>
       <c r="H10" s="186" t="s">
@@ -46568,7 +46565,7 @@
       <c r="F17" s="190" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="225" t="s">
+      <c r="G17" s="224" t="s">
         <v>76</v>
       </c>
       <c r="H17" s="186" t="s">
@@ -46983,7 +46980,7 @@
       <c r="F34" s="190" t="s">
         <v>134</v>
       </c>
-      <c r="G34" s="225" t="s">
+      <c r="G34" s="224" t="s">
         <v>135</v>
       </c>
       <c r="H34" s="186" t="s">
@@ -47001,8 +46998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A58BE6-10B8-478E-A3FE-3CA6A691AC11}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47014,10 +47011,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="235" t="s">
         <v>404</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="9" t="s">
         <v>142</v>
       </c>
@@ -47048,10 +47045,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="232"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="15" t="s">
         <v>60</v>
       </c>
@@ -47066,10 +47063,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="232" t="s">
+      <c r="A4" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="9" t="s">
         <v>142</v>
       </c>
@@ -47084,15 +47081,15 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="233"/>
-      <c r="B5" s="234"/>
-      <c r="C5" s="220" t="s">
-        <v>424</v>
+      <c r="A5" s="236"/>
+      <c r="B5" s="237"/>
+      <c r="C5" s="234" t="s">
+        <v>430</v>
       </c>
       <c r="D5" s="207" t="s">
         <v>423</v>
       </c>
-      <c r="E5" s="245" t="s">
+      <c r="E5" s="234" t="s">
         <v>422</v>
       </c>
       <c r="F5" s="192" t="s">
@@ -47100,13 +47097,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="244" t="s">
+      <c r="A6" s="238" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="241">
+      <c r="C6" s="231">
         <v>1.7929999999999999</v>
       </c>
       <c r="D6" s="38"/>
@@ -47116,19 +47113,19 @@
       <c r="F6" s="67"/>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="244"/>
+      <c r="A7" s="238"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="221"/>
+      <c r="D7" s="220"/>
       <c r="E7" s="8"/>
       <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="244"/>
+      <c r="A8" s="238"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -47136,7 +47133,7 @@
         <v>208</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>134</v>
@@ -47144,11 +47141,11 @@
       <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="244"/>
+      <c r="A9" s="238"/>
       <c r="B9" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="C9" s="242">
+      <c r="C9" s="232">
         <v>1.804</v>
       </c>
       <c r="D9" s="39"/>
@@ -47156,7 +47153,7 @@
       <c r="F9" s="71"/>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="244"/>
+      <c r="A10" s="238"/>
       <c r="B10" s="14" t="s">
         <v>152</v>
       </c>
@@ -47164,7 +47161,7 @@
         <v>153</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="243">
+      <c r="E10" s="233">
         <v>13.5</v>
       </c>
       <c r="F10" s="68"/>
@@ -48083,10 +48080,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -48117,10 +48114,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="232"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="15" t="s">
         <v>79</v>
       </c>
@@ -48135,10 +48132,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="232" t="s">
+      <c r="A4" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="9" t="s">
         <v>200</v>
       </c>
@@ -48153,8 +48150,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="273" x14ac:dyDescent="0.25">
-      <c r="A5" s="233"/>
-      <c r="B5" s="234"/>
+      <c r="A5" s="236"/>
+      <c r="B5" s="237"/>
       <c r="C5" s="37" t="s">
         <v>204</v>
       </c>
@@ -48169,7 +48166,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="235" t="s">
+      <c r="A6" s="239" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48187,7 +48184,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="235"/>
+      <c r="A7" s="239"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48203,7 +48200,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="235"/>
+      <c r="A8" s="239"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -48221,7 +48218,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="235"/>
+      <c r="A9" s="239"/>
       <c r="B9" s="12" t="s">
         <v>151</v>
       </c>
@@ -48237,7 +48234,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="235"/>
+      <c r="A10" s="239"/>
       <c r="B10" s="14" t="s">
         <v>152</v>
       </c>
@@ -48998,7 +48995,7 @@
   <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49010,17 +49007,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="235" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="235"/>
       <c r="C1" s="104" t="s">
         <v>211</v>
       </c>
       <c r="D1" s="117" t="s">
         <v>408</v>
       </c>
-      <c r="E1" s="229" t="s">
+      <c r="E1" s="228" t="s">
         <v>212</v>
       </c>
       <c r="F1" s="129" t="s">
@@ -49042,10 +49039,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="235" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="232"/>
+      <c r="B3" s="235"/>
       <c r="C3" s="103" t="s">
         <v>20</v>
       </c>
@@ -49060,10 +49057,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="232" t="s">
+      <c r="A4" s="235" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="235"/>
       <c r="C4" s="104" t="s">
         <v>211</v>
       </c>
@@ -49078,8 +49075,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="233"/>
-      <c r="B5" s="234"/>
+      <c r="A5" s="236"/>
+      <c r="B5" s="237"/>
       <c r="C5" s="210" t="s">
         <v>214</v>
       </c>
@@ -49089,12 +49086,12 @@
       <c r="E5" s="210" t="s">
         <v>406</v>
       </c>
-      <c r="F5" s="222" t="s">
+      <c r="F5" s="221" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="235" t="s">
+      <c r="A6" s="239" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -49108,7 +49105,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="235"/>
+      <c r="A7" s="239"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -49118,7 +49115,7 @@
       <c r="F7" s="131"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="235"/>
+      <c r="A8" s="239"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -49136,7 +49133,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="235"/>
+      <c r="A9" s="239"/>
       <c r="B9" s="12" t="s">
         <v>151</v>
       </c>
@@ -49148,7 +49145,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="235"/>
+      <c r="A10" s="239"/>
       <c r="B10" s="14" t="s">
         <v>152</v>
       </c>
@@ -50068,10 +50065,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="236" t="s">
+      <c r="A1" s="240" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="236"/>
+      <c r="B1" s="240"/>
       <c r="C1" s="17" t="s">
         <v>220</v>
       </c>
@@ -50238,10 +50235,10 @@
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="240" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="236"/>
+      <c r="B3" s="240"/>
       <c r="C3" s="185" t="s">
         <v>20</v>
       </c>
@@ -50325,10 +50322,10 @@
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="236" t="s">
+      <c r="A4" s="240" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="236"/>
+      <c r="B4" s="240"/>
       <c r="C4" s="65" t="s">
         <v>19</v>
       </c>
@@ -50412,18 +50409,18 @@
       </c>
     </row>
     <row r="5" spans="1:29" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="237"/>
-      <c r="B5" s="237"/>
-      <c r="C5" s="225" t="s">
+      <c r="A5" s="241"/>
+      <c r="B5" s="241"/>
+      <c r="C5" s="224" t="s">
         <v>232</v>
       </c>
-      <c r="D5" s="225" t="s">
+      <c r="D5" s="224" t="s">
         <v>233</v>
       </c>
-      <c r="E5" s="225" t="s">
+      <c r="E5" s="224" t="s">
         <v>234</v>
       </c>
-      <c r="F5" s="225" t="s">
+      <c r="F5" s="224" t="s">
         <v>235</v>
       </c>
       <c r="G5" s="186" t="s">
@@ -50447,19 +50444,19 @@
       <c r="M5" s="186" t="s">
         <v>50</v>
       </c>
-      <c r="N5" s="225" t="s">
+      <c r="N5" s="224" t="s">
         <v>242</v>
       </c>
-      <c r="O5" s="225" t="s">
+      <c r="O5" s="224" t="s">
         <v>243</v>
       </c>
-      <c r="P5" s="225" t="s">
+      <c r="P5" s="224" t="s">
         <v>244</v>
       </c>
-      <c r="Q5" s="225" t="s">
+      <c r="Q5" s="224" t="s">
         <v>245</v>
       </c>
-      <c r="R5" s="225" t="s">
+      <c r="R5" s="224" t="s">
         <v>246</v>
       </c>
       <c r="S5" s="191" t="s">
@@ -50492,12 +50489,12 @@
       <c r="AB5" s="192" t="s">
         <v>256</v>
       </c>
-      <c r="AC5" s="225" t="s">
+      <c r="AC5" s="224" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="238" t="s">
+      <c r="A6" s="242" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -50576,7 +50573,7 @@
       <c r="AC6" s="67"/>
     </row>
     <row r="7" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="238"/>
+      <c r="A7" s="242"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -50611,7 +50608,7 @@
       <c r="AC7" s="68"/>
     </row>
     <row r="8" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="238"/>
+      <c r="A8" s="242"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -50664,7 +50661,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="238"/>
+      <c r="A9" s="242"/>
       <c r="B9" s="62" t="s">
         <v>151</v>
       </c>
@@ -50743,7 +50740,7 @@
       <c r="AC9" s="71"/>
     </row>
     <row r="10" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="238"/>
+      <c r="A10" s="242"/>
       <c r="B10" s="60" t="s">
         <v>152</v>
       </c>
@@ -54285,10 +54282,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="236" t="s">
+      <c r="A1" s="240" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="236"/>
+      <c r="B1" s="240"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -54383,10 +54380,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="240" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="236"/>
+      <c r="B3" s="240"/>
       <c r="C3" s="15" t="s">
         <v>99</v>
       </c>
@@ -54434,10 +54431,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="236" t="s">
+      <c r="A4" s="240" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="236"/>
+      <c r="B4" s="240"/>
       <c r="C4" s="65" t="s">
         <v>276</v>
       </c>
@@ -54485,19 +54482,19 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="239"/>
-      <c r="B5" s="240"/>
-      <c r="C5" s="223" t="s">
+      <c r="A5" s="243"/>
+      <c r="B5" s="244"/>
+      <c r="C5" s="222" t="s">
         <v>291</v>
       </c>
-      <c r="D5" s="224" t="s">
+      <c r="D5" s="223" t="s">
         <v>292</v>
       </c>
       <c r="E5" s="206" t="s">
         <v>293</v>
       </c>
-      <c r="F5" s="231" t="s">
-        <v>429</v>
+      <c r="F5" s="230" t="s">
+        <v>428</v>
       </c>
       <c r="G5" s="206" t="s">
         <v>294</v>
@@ -54515,7 +54512,7 @@
         <v>298</v>
       </c>
       <c r="L5" s="206" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M5" s="205" t="s">
         <v>299</v>
@@ -54534,7 +54531,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="238" t="s">
+      <c r="A6" s="242" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -54557,7 +54554,7 @@
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="238"/>
+      <c r="A7" s="242"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -54578,7 +54575,7 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="238"/>
+      <c r="A8" s="242"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -54623,7 +54620,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="238"/>
+      <c r="A9" s="242"/>
       <c r="B9" s="62" t="s">
         <v>151</v>
       </c>
@@ -54648,7 +54645,7 @@
       <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="238"/>
+      <c r="A10" s="242"/>
       <c r="B10" s="60" t="s">
         <v>152</v>
       </c>
@@ -56819,10 +56816,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="236" t="s">
+      <c r="A1" s="240" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="236"/>
+      <c r="B1" s="240"/>
       <c r="C1" s="65" t="s">
         <v>64</v>
       </c>
@@ -56893,10 +56890,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="236" t="s">
+      <c r="A3" s="240" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="236"/>
+      <c r="B3" s="240"/>
       <c r="C3" s="64" t="s">
         <v>65</v>
       </c>
@@ -56932,10 +56929,10 @@
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A4" s="236" t="s">
+      <c r="A4" s="240" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="236"/>
+      <c r="B4" s="240"/>
       <c r="C4" s="65" t="s">
         <v>64</v>
       </c>
@@ -56971,10 +56968,10 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="239"/>
-      <c r="B5" s="239"/>
+      <c r="A5" s="243"/>
+      <c r="B5" s="243"/>
       <c r="C5" s="211" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D5" s="37" t="s">
         <v>415</v>
@@ -56997,16 +56994,16 @@
       <c r="J5" s="56" t="s">
         <v>336</v>
       </c>
-      <c r="K5" s="230" t="s">
-        <v>428</v>
-      </c>
-      <c r="L5" s="230" t="s">
+      <c r="K5" s="229" t="s">
         <v>427</v>
       </c>
+      <c r="L5" s="229" t="s">
+        <v>426</v>
+      </c>
       <c r="M5" s="56"/>
     </row>
     <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="238" t="s">
+      <c r="A6" s="242" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -57025,7 +57022,7 @@
       <c r="M6" s="67"/>
     </row>
     <row r="7" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="238"/>
+      <c r="A7" s="242"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -57042,7 +57039,7 @@
       <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="238"/>
+      <c r="A8" s="242"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -57079,7 +57076,7 @@
       <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="238"/>
+      <c r="A9" s="242"/>
       <c r="B9" s="62" t="s">
         <v>151</v>
       </c>
@@ -57096,7 +57093,7 @@
       <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="238"/>
+      <c r="A10" s="242"/>
       <c r="B10" s="60" t="s">
         <v>152</v>
       </c>
@@ -58815,7 +58812,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="228" t="s">
+      <c r="A2" s="227" t="s">
         <v>402</v>
       </c>
       <c r="B2" s="177" t="s">

</xml_diff>

<commit_message>
Remove some non necessary files, AZ_comp, reference and trimming now are working
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6308DB7A-7C35-4C55-A070-E8722ACD6C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC43E845-9275-41A0-B9E9-BE4DEF3319F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38076,97 +38076,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Run__DAC-PA TDM_768_IN
-ForceTDM__-6_1000
-Measure__THD__OUTP__OUTN
-Measure__flatness__OUTP__OUTN
-Measure__PSRR__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-ForceTDM__-60__1000
-Measure__noise__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run__DAC-PA ANALOG_IN_DC_COUPLED
-ForceANA__-6_1000
-Measure__THD__OUTP__OUTN
-Measure__flatness__OUTP__OUTN
-Measure__PSRR__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-ForceANA__-60__1000
-Measure__noise__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run__DAC-PA ANALOG_IN_AC_COUPLED
-ForceANA__-6_1000
-Measure__THD__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-ForceANA__-60__1000
-Measure__noise__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-</t>
-  </si>
-  <si>
-    <t>Run__DAC-PA PDM_3MHz_IN
-ForcePDM__-6_1000
-Measure__THD__OUTP__OUTN
-Measure__flatness__OUTP__OUTN
-Measure__PSRR__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-ForcePDM__-60__1000
-Measure__noise__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT</t>
-  </si>
-  <si>
-    <t>Run__DAC-PA PDM_6MHz_IN
-ForcePDM__-6_1000
-Measure__THD__OUTP__OUTN
-Measure__flatness__OUTP__OUTN
-Measure__PSRR__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-ForcePDM__-60__1000
-Measure__noise__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT</t>
-  </si>
-  <si>
-    <t>Run__DAC-PA PDM_12MHz_IN
-ForcePDM__-6_1000
-Measure__THD__OUTP__OUTN
-Measure__flatness__OUTP__OUTN
-Measure__PSRR__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-ForcePDM__-60__1000
-Measure__noise__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="16"/>
@@ -42235,99 +42144,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Run__DAC-PA TDM_768_IN_and_Path_generator
-Measure__THD__OUTP__OUTN
-Measure__flatness__OUTP__OUTN
-Measure__PSRR__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "in test page"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1E_0xF8</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "set enable and gain = -61dB (Gains from-1dB to -61dB step -6) anf freq=1kHz (available freq: 1-2-4-8-16kHz)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="16"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="16"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "in base page"</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="16"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Measure__noise__OUTP__OUTN
-Measure__current__VDDIO
-Measure__current__VDD
-Measure__current__VBAT
-</t>
-    </r>
-  </si>
-  <si>
     <t>0.542</t>
   </si>
   <si>
@@ -43673,15 +43489,6 @@
       <t>0x1A_0x00
 0x19_0x00</t>
     </r>
-  </si>
-  <si>
-    <t>13M</t>
-  </si>
-  <si>
-    <t>12.5M</t>
-  </si>
-  <si>
-    <t>13.5M</t>
   </si>
   <si>
     <t xml:space="preserve">Run__Startup
@@ -43710,9 +43517,193 @@
 </t>
   </si>
   <si>
+    <t>Run__DAC-PA_PDM_12MHz_IN
+ForcePDM__-6_1000
+Measure__THD__OUTP__OUTN
+Measure__flatness__OUTP__OUTN
+Measure__PSRR__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+ForcePDM__-60__1000
+Measure__noise__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT</t>
+  </si>
+  <si>
+    <t>Run__DAC-PA_PDM_6MHz_IN
+ForcePDM__-6_1000
+Measure__THD__OUTP__OUTN
+Measure__flatness__OUTP__OUTN
+Measure__PSRR__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+ForcePDM__-60__1000
+Measure__noise__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT</t>
+  </si>
+  <si>
+    <t>Run__DAC-PA_PDM_3MHz_IN
+ForcePDM__-6_1000
+Measure__THD__OUTP__OUTN
+Measure__flatness__OUTP__OUTN
+Measure__PSRR__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+ForcePDM__-60__1000
+Measure__noise__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run__DAC-PA_ANALOG_IN_AC_COUPLED
+ForceANA__-6_1000
+Measure__THD__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+ForceANA__-60__1000
+Measure__noise__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run__DAC-PA_ANALOG_IN_DC_COUPLED
+ForceANA__-6_1000
+Measure__THD__OUTP__OUTN
+Measure__flatness__OUTP__OUTN
+Measure__PSRR__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+ForceANA__-60__1000
+Measure__noise__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run__DAC-PA_TDM_768_IN
+ForceTDM__-6_1000
+Measure__THD__OUTP__OUTN
+Measure__flatness__OUTP__OUTN
+Measure__PSRR__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+ForceTDM__-60__1000
+Measure__noise__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run__DAC-PA_TDM_768_IN_and_Path_generator
+Measure__THD__OUTP__OUTN
+Measure__flatness__OUTP__OUTN
+Measure__PSRR__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "in test page"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1E_0xF8</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "set enable and gain = -61dB (Gains from-1dB to -61dB step -6) anf freq=1kHz (available freq: 1-2-4-8-16kHz)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "in base page"</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Measure__noise__OUTP__OUTN
+Measure__current__VDDIO
+Measure__current__VDD
+Measure__current__VBAT
+</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Run__Startup
 0xFE_0x00 "Select page 0"
-0x00_0x01
+0x00_0x0F "Select 812.5 kHz"
 0xFE_0x01 "Select page 1"
 0x03_0x04 "Enable digital test FSYN"
 0x04_0x20 "Enable digital test ana_ref_fro_clk_13m"
@@ -43724,6 +43715,15 @@
 Calculate__MinError
 0xFE_0x00 "Select page 0"
 </t>
+  </si>
+  <si>
+    <t>812.5k</t>
+  </si>
+  <si>
+    <t>800k</t>
+  </si>
+  <si>
+    <t>825k</t>
   </si>
 </sst>
 </file>
@@ -45927,177 +45927,177 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="K6" s="58" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="58" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="23" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -46993,8 +46993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A58BE6-10B8-478E-A3FE-3CA6A691AC11}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47007,7 +47007,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="235" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="B1" s="235"/>
       <c r="C1" s="9" t="s">
@@ -47079,16 +47079,16 @@
       <c r="A5" s="236"/>
       <c r="B5" s="237"/>
       <c r="C5" s="207" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="D5" s="207" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="E5" s="207" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F5" s="192" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
@@ -47103,7 +47103,7 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="F6" s="67"/>
     </row>
@@ -47128,10 +47128,10 @@
         <v>208</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="F8" s="69"/>
     </row>
@@ -47157,7 +47157,7 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="233" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="F10" s="68"/>
     </row>
@@ -49010,7 +49010,7 @@
         <v>211</v>
       </c>
       <c r="D1" s="117" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E1" s="228" t="s">
         <v>212</v>
@@ -49060,7 +49060,7 @@
         <v>211</v>
       </c>
       <c r="D4" s="117" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E4" s="104" t="s">
         <v>212</v>
@@ -49076,10 +49076,10 @@
         <v>214</v>
       </c>
       <c r="D5" s="219" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E5" s="210" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="F5" s="221" t="s">
         <v>215</v>
@@ -49115,7 +49115,7 @@
         <v>149</v>
       </c>
       <c r="C8" s="107" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="D8" s="120" t="s">
         <v>216</v>
@@ -50422,16 +50422,16 @@
         <v>236</v>
       </c>
       <c r="H5" s="191" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="I5" s="191" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="J5" s="191" t="s">
         <v>237</v>
       </c>
       <c r="K5" s="191" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="L5" s="224" t="s">
         <v>238</v>
@@ -54256,8 +54256,8 @@
   </sheetPr>
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54486,43 +54486,43 @@
         <v>289</v>
       </c>
       <c r="E5" s="206" t="s">
+        <v>428</v>
+      </c>
+      <c r="F5" s="230" t="s">
+        <v>429</v>
+      </c>
+      <c r="G5" s="206" t="s">
+        <v>427</v>
+      </c>
+      <c r="H5" s="206" t="s">
+        <v>426</v>
+      </c>
+      <c r="I5" s="206" t="s">
+        <v>425</v>
+      </c>
+      <c r="J5" s="206" t="s">
+        <v>424</v>
+      </c>
+      <c r="K5" s="206" t="s">
+        <v>423</v>
+      </c>
+      <c r="L5" s="206" t="s">
+        <v>414</v>
+      </c>
+      <c r="M5" s="205" t="s">
         <v>290</v>
       </c>
-      <c r="F5" s="230" t="s">
-        <v>423</v>
-      </c>
-      <c r="G5" s="206" t="s">
+      <c r="N5" s="205" t="s">
         <v>291</v>
       </c>
-      <c r="H5" s="206" t="s">
+      <c r="O5" s="205" t="s">
         <v>292</v>
       </c>
-      <c r="I5" s="206" t="s">
+      <c r="P5" s="205" t="s">
         <v>293</v>
       </c>
-      <c r="J5" s="206" t="s">
+      <c r="Q5" s="205" t="s">
         <v>294</v>
-      </c>
-      <c r="K5" s="206" t="s">
-        <v>295</v>
-      </c>
-      <c r="L5" s="206" t="s">
-        <v>420</v>
-      </c>
-      <c r="M5" s="205" t="s">
-        <v>296</v>
-      </c>
-      <c r="N5" s="205" t="s">
-        <v>297</v>
-      </c>
-      <c r="O5" s="205" t="s">
-        <v>298</v>
-      </c>
-      <c r="P5" s="205" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q5" s="205" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -54577,41 +54577,41 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="N8" s="11" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="O8" s="11" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="Q8" s="11" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -54623,7 +54623,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E9" s="71"/>
       <c r="F9" s="71"/>
@@ -54666,47 +54666,47 @@
         <v>154</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5" t="s">
         <v>262</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>155</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -55026,13 +55026,13 @@
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="50" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F20" s="50" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="G20" s="89"/>
       <c r="I20" s="76"/>
@@ -55053,29 +55053,29 @@
         <v>184</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D21" s="50" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E21" s="50" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="50" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="H21" s="50" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="I21" s="76" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="J21" s="76" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="K21" s="76" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="L21" s="76"/>
       <c r="M21" s="50"/>
@@ -55092,31 +55092,31 @@
         <v>186</v>
       </c>
       <c r="C22" s="50" t="s">
+        <v>308</v>
+      </c>
+      <c r="D22" s="50" t="s">
         <v>314</v>
       </c>
-      <c r="D22" s="50" t="s">
+      <c r="E22" s="50" t="s">
+        <v>315</v>
+      </c>
+      <c r="F22" s="50" t="s">
+        <v>315</v>
+      </c>
+      <c r="G22" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="H22" s="50" t="s">
+        <v>317</v>
+      </c>
+      <c r="I22" s="76" t="s">
+        <v>318</v>
+      </c>
+      <c r="J22" s="76" t="s">
+        <v>319</v>
+      </c>
+      <c r="K22" s="76" t="s">
         <v>320</v>
-      </c>
-      <c r="E22" s="50" t="s">
-        <v>321</v>
-      </c>
-      <c r="F22" s="50" t="s">
-        <v>321</v>
-      </c>
-      <c r="G22" s="50" t="s">
-        <v>322</v>
-      </c>
-      <c r="H22" s="50" t="s">
-        <v>323</v>
-      </c>
-      <c r="I22" s="76" t="s">
-        <v>324</v>
-      </c>
-      <c r="J22" s="76" t="s">
-        <v>325</v>
-      </c>
-      <c r="K22" s="76" t="s">
-        <v>326</v>
       </c>
       <c r="L22" s="76"/>
       <c r="M22" s="50"/>
@@ -55202,31 +55202,31 @@
         <v>195</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D26" s="50" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="F26" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="G26" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="I26" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="J26" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="K26" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="L26" s="50"/>
       <c r="M26" s="50"/>
@@ -55243,31 +55243,31 @@
         <v>197</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D27" s="50" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E27" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="F27" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="G27" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="I27" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="J27" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="K27" s="50" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="L27" s="50"/>
       <c r="M27" s="50"/>
@@ -56819,16 +56819,16 @@
         <v>64</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="G1" s="65" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>114</v>
@@ -56837,16 +56837,16 @@
         <v>118</v>
       </c>
       <c r="J1" s="65" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="K1" s="65" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="L1" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M1" s="95" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
@@ -56920,7 +56920,7 @@
         <v>36</v>
       </c>
       <c r="M3" s="64" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
@@ -56932,16 +56932,16 @@
         <v>64</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="E4" s="65" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="F4" s="65" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>114</v>
@@ -56950,50 +56950,50 @@
         <v>118</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="K4" s="65" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="L4" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M4" s="95" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="243"/>
       <c r="B5" s="243"/>
       <c r="C5" s="211" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="G5" s="37" t="s">
+        <v>409</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="J5" s="56" t="s">
+        <v>327</v>
+      </c>
+      <c r="K5" s="229" t="s">
+        <v>416</v>
+      </c>
+      <c r="L5" s="229" t="s">
         <v>415</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>416</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>417</v>
-      </c>
-      <c r="J5" s="56" t="s">
-        <v>333</v>
-      </c>
-      <c r="K5" s="229" t="s">
-        <v>422</v>
-      </c>
-      <c r="L5" s="229" t="s">
-        <v>421</v>
       </c>
       <c r="M5" s="56"/>
     </row>
@@ -57042,13 +57042,13 @@
         <v>257</v>
       </c>
       <c r="D8" s="69" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="E8" s="69" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>20</v>
@@ -57060,10 +57060,10 @@
         <v>75</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>75</v>
@@ -58767,84 +58767,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="D1" s="57" t="s">
+        <v>332</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="F1" s="57" t="s">
+        <v>334</v>
+      </c>
+      <c r="G1" s="57" t="s">
+        <v>335</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="I1" s="57" t="s">
+        <v>337</v>
+      </c>
+      <c r="J1" s="57" t="s">
         <v>338</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>339</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="L1" s="57" t="s">
         <v>340</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="M1" s="57" t="s">
         <v>341</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>342</v>
-      </c>
-      <c r="I1" s="57" t="s">
-        <v>343</v>
-      </c>
-      <c r="J1" s="57" t="s">
-        <v>344</v>
-      </c>
-      <c r="K1" s="57" t="s">
-        <v>345</v>
-      </c>
-      <c r="L1" s="57" t="s">
-        <v>346</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="227" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="B2" s="177" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="C2" s="177" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D2" s="83" t="s">
+        <v>342</v>
+      </c>
+      <c r="E2" s="83" t="s">
+        <v>343</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>344</v>
+      </c>
+      <c r="G2" s="83" t="s">
+        <v>345</v>
+      </c>
+      <c r="H2" s="83" t="s">
+        <v>346</v>
+      </c>
+      <c r="I2" s="83" t="s">
+        <v>347</v>
+      </c>
+      <c r="J2" s="83" t="s">
         <v>348</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="K2" s="83" t="s">
         <v>349</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="L2" s="83" t="s">
         <v>350</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="M2" s="83" t="s">
         <v>351</v>
-      </c>
-      <c r="H2" s="83" t="s">
-        <v>352</v>
-      </c>
-      <c r="I2" s="83" t="s">
-        <v>353</v>
-      </c>
-      <c r="J2" s="83" t="s">
-        <v>354</v>
-      </c>
-      <c r="K2" s="83" t="s">
-        <v>355</v>
-      </c>
-      <c r="L2" s="83" t="s">
-        <v>356</v>
-      </c>
-      <c r="M2" s="83" t="s">
-        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -58854,15 +58854,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
@@ -58871,6 +58862,15 @@
     <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59091,20 +59091,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
     <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added control for SDWN and cleaned some files. Trimming, reference, AZ_comp are working now
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC43E845-9275-41A0-B9E9-BE4DEF3319F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EE1F2B-3E8E-4C3A-9175-29F69F7C0F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43494,19 +43494,6 @@
     <t xml:space="preserve">Run__Startup
 Run__Enable_Ana_Testpoint
 0xFE_0x01 "Select page 1"
-0x1A_0x01 "Bandgap"
-0xB0_0x0E
-"Loop__trim:"
-Trim__0xB0[7:4] "Select code which sets ATEST voltage as close as possible to target"
-Measure__Voltage__SDWN
-Calculate__MinError
-0xFE_0x00 "Select page 0"
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run__Startup
-Run__Enable_Ana_Testpoint
-0xFE_0x01 "Select page 1"
 0x1A_0x04 "TSDN"
 0xB0_0x0E
 "Loop__trim:"
@@ -43724,6 +43711,19 @@
   </si>
   <si>
     <t>825k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run__Startup
+Run__Enable_Ana_Testpoint
+0xFE_0x01 "Select page 1"
+0xB0_0x0E
+0x1A_0x01 "Bandgap"
+"Loop__trim:"
+Trim__0xB0[7:4] "Select code which sets ATEST voltage as close as possible to target"
+Measure__Voltage__SDWN
+Calculate__MinError
+0xFE_0x00 "Select page 0"
+</t>
   </si>
 </sst>
 </file>
@@ -46993,8 +46993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A58BE6-10B8-478E-A3FE-3CA6A691AC11}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47079,13 +47079,13 @@
       <c r="A5" s="236"/>
       <c r="B5" s="237"/>
       <c r="C5" s="207" t="s">
+        <v>433</v>
+      </c>
+      <c r="D5" s="207" t="s">
         <v>421</v>
       </c>
-      <c r="D5" s="207" t="s">
-        <v>422</v>
-      </c>
       <c r="E5" s="207" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F5" s="192" t="s">
         <v>412</v>
@@ -47103,7 +47103,7 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F6" s="67"/>
     </row>
@@ -47131,7 +47131,7 @@
         <v>417</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F8" s="69"/>
     </row>
@@ -47157,7 +47157,7 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="233" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F10" s="68"/>
     </row>
@@ -48056,6 +48056,7 @@
     <mergeCell ref="A6:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -54486,25 +54487,25 @@
         <v>289</v>
       </c>
       <c r="E5" s="206" t="s">
+        <v>427</v>
+      </c>
+      <c r="F5" s="230" t="s">
         <v>428</v>
       </c>
-      <c r="F5" s="230" t="s">
-        <v>429</v>
-      </c>
       <c r="G5" s="206" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H5" s="206" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I5" s="206" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J5" s="206" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K5" s="206" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L5" s="206" t="s">
         <v>414</v>
@@ -58854,6 +58855,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
@@ -58862,15 +58872,6 @@
     <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59091,20 +59092,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
     <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added on the boost_class the procedure for the right boost power up  with the forcing of VBIAS and VBSO through the matrix
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF0EFE6-AAA8-4EAF-8293-A4979EC83D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613A7D38-0920-4209-AF37-23A68DE7820C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32777,1152 +32777,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Run__startup
-Run__Boost_test_default
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Force__VBSO_3.6V</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Force__VPAP_OUT__ 0V </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"PA positive output"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Force__VPAN_OUT__0V</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "PA negative output"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1[7]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "env_err en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst general en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x03_0x04</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "FSYN en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x04_0x09</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "FSYN=bst_env_err"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Power Force en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x15[4]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force bst general en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x15[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "force env_err"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst_test en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Voltage__FSYN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "it should be 0 since the ref is higher than the PA OUTPUT"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Force__VPAP_OUT__3.6V</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "PA positive output"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Voltage__FSYN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "now it should be 1 since the PA output should be higher than the ref"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19_0x00
-0x03_0x00
-0x04_0x00</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Run__startup
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Run__Boost_test_default</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Force__VBIAS__5V
-Force__VBSO__3.6V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 1 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 2 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB3[4:3]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 3 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x18[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Enable Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Bootstrap en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ls_sel on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB4[2:0]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "hsa_hsb_byp off"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x17[6]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x16[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force Bootstrap"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ocp en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst general en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xC0[2:0]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"ocp threshold set to 200 mA"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x03_0x04</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "FSYN en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x04_0x18</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "FSYN=ana_bst_ocp_1"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Power Force en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x15[4]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force bst general en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0x15[2]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "force ocp"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst_test en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Voltage__FSYN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "it should be 0 "
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Force__Current__SW__300mA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"inject"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Voltage__FSYN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "it should be 1 since the current flowing is higher than the selected threshold (200mA)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19_0x00
-0x03_0x00
-0x04_0x01</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF3399"/>
@@ -39156,305 +38010,6 @@
       </rPr>
       <t xml:space="preserve">Run_startup
 Run_Boost_test_default
-Force__VBIAS__5V
-Force__VBSO__3.6V
-Force__SW__3.6V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 1 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 2 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB3[4:3]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 3 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run_Enable_Ana_Testpoint
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1A_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "TSW_Mirr test"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x18[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Enable Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x17[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force Mirr"
-Force__SDWN__0.6V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst_test_en 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Current__SDWN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "tswitch mirr measure"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x00
-0x19_0x00
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run_startup
-Run_Boost_test_default
 Run_Enable_Ana_Testpoint
 Force__VBIAS__5V
 Force__VBSO__3.6V
@@ -44223,6 +42778,1523 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run__startup
+Run__Boost_test_default
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Force__VBSO_3.6V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Force__OUTP__ 0V </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"PA positive output"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Force__OUTN__0V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "PA negative output"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1[7]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "env_err en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB0[0]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "bst general en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x03_0x04</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "FSYN en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x04_0x09</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "FSYN=bst_env_err"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[0]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Power Force en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x15[4]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force bst general en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x15[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "force env_err"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "bst_test en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Voltage__FSYN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "it should be 0 since the ref is higher than the PA OUTPUT"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Force__OUTP__3.6V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "PA positive output"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Voltage__FSYN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "now it should be 1 since the PA output should be higher than the ref"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19_0x00
+0x03_0x00
+0x04_0x00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Run__startup
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Run__Boost_test_default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Force__VBIAS__5V
+Force__VBSO__3.6V
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB0_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 1 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 2 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB3[4:3]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 3 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x18[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Enable Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Bootstrap en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "ls_sel on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB4[2:0]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "hsa_hsb_byp off"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x17[6]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x16[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force Bootstrap"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB0[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "ocp en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB0[0]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "bst general en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xC0[2:0]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"ocp threshold set to 200 mA"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x03_0x04</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "FSYN en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x04_0x18</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "FSYN=ana_bst_ocp_1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[0]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Power Force en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x15[4]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force bst general en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0x15[2]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "force ocp"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "bst_test en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Voltage__FSYN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "it should be 0 "
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Force__Current__SW__300mA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"inject"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Voltage__FSYN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "it should be 1 since the current flowing is higher than the selected threshold (200mA)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19_0x00
+0x03_0x00
+0x04_0x01</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run_startup
+Run_Boost_test_default
+Run_Enable_Ana_Testpoint
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB0_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 1 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 2 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB3[4:3]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 3 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1A_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "TSW_Mirr test"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x18[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Enable Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x17[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Force__SDWN__0.6V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "bst_test_en 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Current__SDWN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "tswitch mirr measure"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x00
+0x19_0x00
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
@@ -44239,7 +44311,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="117" x14ac:knownFonts="1">
+  <fonts count="118" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44985,6 +45057,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -45377,7 +45458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="243">
+  <cellXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -45993,6 +46074,12 @@
     <xf numFmtId="3" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="117" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -46407,177 +46494,177 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23" t="s">
+        <v>350</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>352</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="H6" s="24" t="s">
         <v>353</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="J6" s="25" t="s">
         <v>354</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="K6" s="58" t="s">
         <v>355</v>
-      </c>
-      <c r="J6" s="25" t="s">
-        <v>356</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="58" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="23" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="G8" s="23" t="s">
         <v>360</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>361</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>362</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>363</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -47473,8 +47560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A58BE6-10B8-478E-A3FE-3CA6A691AC11}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47487,7 +47574,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="233" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B1" s="233"/>
       <c r="C1" s="9" t="s">
@@ -47559,16 +47646,16 @@
       <c r="A5" s="234"/>
       <c r="B5" s="235"/>
       <c r="C5" s="206" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D5" s="206" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E5" s="206" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F5" s="191" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
@@ -47583,7 +47670,7 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F6" s="67"/>
     </row>
@@ -47608,10 +47695,10 @@
         <v>208</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F8" s="69"/>
     </row>
@@ -47637,7 +47724,7 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="231" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F10" s="68"/>
     </row>
@@ -49491,7 +49578,7 @@
         <v>211</v>
       </c>
       <c r="D1" s="116" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E1" s="227" t="s">
         <v>212</v>
@@ -49541,7 +49628,7 @@
         <v>211</v>
       </c>
       <c r="D4" s="116" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E4" s="103" t="s">
         <v>212</v>
@@ -49557,10 +49644,10 @@
         <v>214</v>
       </c>
       <c r="D5" s="218" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E5" s="209" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F5" s="220" t="s">
         <v>215</v>
@@ -49596,7 +49683,7 @@
         <v>149</v>
       </c>
       <c r="C8" s="106" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D8" s="119" t="s">
         <v>216</v>
@@ -50523,8 +50610,8 @@
   <dimension ref="A1:AC104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X5" sqref="X5"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50593,14 +50680,14 @@
       <c r="R1" s="151" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="138" t="s">
-        <v>102</v>
-      </c>
-      <c r="T1" s="162" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" s="65" t="s">
-        <v>59</v>
+      <c r="S1" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="U1" s="243" t="s">
+        <v>138</v>
       </c>
       <c r="V1" s="65" t="s">
         <v>51</v>
@@ -50888,40 +50975,40 @@
       <c r="A5" s="239"/>
       <c r="B5" s="239"/>
       <c r="C5" s="223" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="D5" s="223" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E5" s="223" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="F5" s="223" t="s">
         <v>231</v>
       </c>
       <c r="G5" s="185" t="s">
+        <v>423</v>
+      </c>
+      <c r="H5" s="191" t="s">
+        <v>424</v>
+      </c>
+      <c r="I5" s="190" t="s">
+        <v>425</v>
+      </c>
+      <c r="J5" s="190" t="s">
         <v>426</v>
       </c>
-      <c r="H5" s="191" t="s">
+      <c r="K5" s="190" t="s">
         <v>427</v>
       </c>
-      <c r="I5" s="190" t="s">
+      <c r="L5" s="223" t="s">
         <v>428</v>
       </c>
-      <c r="J5" s="190" t="s">
+      <c r="M5" s="223" t="s">
         <v>429</v>
       </c>
-      <c r="K5" s="190" t="s">
+      <c r="N5" s="223" t="s">
         <v>430</v>
-      </c>
-      <c r="L5" s="223" t="s">
-        <v>431</v>
-      </c>
-      <c r="M5" s="223" t="s">
-        <v>432</v>
-      </c>
-      <c r="N5" s="223" t="s">
-        <v>433</v>
       </c>
       <c r="O5" s="223" t="s">
         <v>232</v>
@@ -50960,13 +51047,13 @@
         <v>243</v>
       </c>
       <c r="AA5" s="191" t="s">
+        <v>431</v>
+      </c>
+      <c r="AB5" s="191" t="s">
+        <v>432</v>
+      </c>
+      <c r="AC5" s="244" t="s">
         <v>244</v>
-      </c>
-      <c r="AB5" s="191" t="s">
-        <v>245</v>
-      </c>
-      <c r="AC5" s="223" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -51089,36 +51176,36 @@
         <v>149</v>
       </c>
       <c r="C8" s="69" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D8" s="69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E8" s="69" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="69"/>
       <c r="G8" s="69" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H8" s="69" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I8" s="69" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K8" s="69" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L8" s="69"/>
       <c r="M8" s="69"/>
       <c r="N8" s="69"/>
       <c r="O8" s="69"/>
       <c r="P8" s="69" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="Q8" s="69"/>
       <c r="R8" s="153"/>
@@ -51133,7 +51220,7 @@
       <c r="AA8" s="69"/>
       <c r="AB8" s="69"/>
       <c r="AC8" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -51150,19 +51237,19 @@
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H9" s="71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I9" s="71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J9" s="71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K9" s="71" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="L9" s="71">
         <v>3</v>
@@ -51177,7 +51264,7 @@
         <v>4</v>
       </c>
       <c r="P9" s="71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="Q9" s="70">
         <v>1.64</v>
@@ -51187,16 +51274,16 @@
       </c>
       <c r="S9" s="142"/>
       <c r="T9" s="166" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="U9" s="71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="V9" s="71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="W9" s="71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="X9" s="198">
         <v>20.074999999999999</v>
@@ -51205,13 +51292,13 @@
         <v>24.2</v>
       </c>
       <c r="Z9" s="71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AA9" s="39" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AB9" s="39" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AC9" s="71"/>
     </row>
@@ -51259,10 +51346,10 @@
         <v>218</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E11" s="72" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F11" s="72"/>
       <c r="G11" s="72" t="s">
@@ -51330,7 +51417,7 @@
         <v>155</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -51468,10 +51555,10 @@
         <v>163</v>
       </c>
       <c r="D14" s="86" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E14" s="86" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F14" s="85" t="s">
         <v>163</v>
@@ -51534,7 +51621,7 @@
         <v>163</v>
       </c>
       <c r="AB14" s="84" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AC14" s="85" t="s">
         <v>163</v>
@@ -51884,7 +51971,7 @@
       <c r="N20" s="85"/>
       <c r="O20" s="85"/>
       <c r="P20" s="85" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="Q20" s="85"/>
       <c r="R20" s="155"/>
@@ -52003,7 +52090,7 @@
         <v>191</v>
       </c>
       <c r="F23" s="98" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G23" s="84" t="s">
         <v>163</v>
@@ -52045,7 +52132,7 @@
         <v>163</v>
       </c>
       <c r="T23" s="170" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="U23" s="84" t="s">
         <v>163</v>
@@ -52132,10 +52219,10 @@
         <v>191</v>
       </c>
       <c r="T24" s="168" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="U24" s="85" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="V24" s="85" t="s">
         <v>191</v>
@@ -52227,11 +52314,11 @@
       <c r="Y26" s="85"/>
       <c r="Z26" s="85"/>
       <c r="AA26" s="84" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AB26" s="84"/>
       <c r="AC26" s="84" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:29" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -52266,7 +52353,7 @@
       <c r="Y27" s="85"/>
       <c r="Z27" s="85"/>
       <c r="AA27" s="84" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AB27" s="85"/>
       <c r="AC27" s="85"/>
@@ -54912,98 +54999,98 @@
       </c>
       <c r="B4" s="238"/>
       <c r="C4" s="65" t="s">
+        <v>262</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="G4" s="65" t="s">
         <v>266</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="I4" s="90" t="s">
         <v>268</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="J4" s="90" t="s">
         <v>269</v>
       </c>
-      <c r="I4" s="90" t="s">
+      <c r="K4" s="90" t="s">
         <v>270</v>
       </c>
-      <c r="J4" s="90" t="s">
+      <c r="L4" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="K4" s="90" t="s">
+      <c r="M4" s="93" t="s">
         <v>272</v>
       </c>
-      <c r="L4" s="93" t="s">
+      <c r="N4" s="93" t="s">
         <v>273</v>
       </c>
-      <c r="M4" s="93" t="s">
+      <c r="O4" s="93" t="s">
         <v>274</v>
       </c>
-      <c r="N4" s="93" t="s">
+      <c r="P4" s="93" t="s">
         <v>275</v>
       </c>
-      <c r="O4" s="93" t="s">
+      <c r="Q4" s="93" t="s">
         <v>276</v>
-      </c>
-      <c r="P4" s="93" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q4" s="93" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="241"/>
       <c r="B5" s="242"/>
       <c r="C5" s="221" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" s="222" t="s">
+        <v>278</v>
+      </c>
+      <c r="E5" s="205" t="s">
+        <v>413</v>
+      </c>
+      <c r="F5" s="205" t="s">
+        <v>420</v>
+      </c>
+      <c r="G5" s="205" t="s">
+        <v>412</v>
+      </c>
+      <c r="H5" s="205" t="s">
+        <v>411</v>
+      </c>
+      <c r="I5" s="205" t="s">
+        <v>410</v>
+      </c>
+      <c r="J5" s="205" t="s">
+        <v>409</v>
+      </c>
+      <c r="K5" s="205" t="s">
+        <v>408</v>
+      </c>
+      <c r="L5" s="205" t="s">
+        <v>403</v>
+      </c>
+      <c r="M5" s="204" t="s">
         <v>279</v>
       </c>
-      <c r="D5" s="222" t="s">
+      <c r="N5" s="204" t="s">
         <v>280</v>
       </c>
-      <c r="E5" s="205" t="s">
-        <v>415</v>
-      </c>
-      <c r="F5" s="205" t="s">
-        <v>422</v>
-      </c>
-      <c r="G5" s="205" t="s">
-        <v>414</v>
-      </c>
-      <c r="H5" s="205" t="s">
-        <v>413</v>
-      </c>
-      <c r="I5" s="205" t="s">
-        <v>412</v>
-      </c>
-      <c r="J5" s="205" t="s">
-        <v>411</v>
-      </c>
-      <c r="K5" s="205" t="s">
-        <v>410</v>
-      </c>
-      <c r="L5" s="205" t="s">
-        <v>405</v>
-      </c>
-      <c r="M5" s="204" t="s">
+      <c r="O5" s="204" t="s">
         <v>281</v>
       </c>
-      <c r="N5" s="204" t="s">
+      <c r="P5" s="204" t="s">
         <v>282</v>
       </c>
-      <c r="O5" s="204" t="s">
+      <c r="Q5" s="204" t="s">
         <v>283</v>
-      </c>
-      <c r="P5" s="204" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q5" s="204" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -55058,41 +55145,41 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="O8" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>289</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="Q8" s="11" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -55104,7 +55191,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E9" s="71"/>
       <c r="F9" s="71"/>
@@ -55147,47 +55234,47 @@
         <v>154</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>155</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -55507,13 +55594,13 @@
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="50" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F20" s="50" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G20" s="89"/>
       <c r="I20" s="76"/>
@@ -55534,29 +55621,29 @@
         <v>184</v>
       </c>
       <c r="C21" s="50" t="s">
+        <v>297</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>298</v>
+      </c>
+      <c r="E21" s="50" t="s">
         <v>299</v>
-      </c>
-      <c r="D21" s="50" t="s">
-        <v>300</v>
-      </c>
-      <c r="E21" s="50" t="s">
-        <v>301</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="50" t="s">
+        <v>300</v>
+      </c>
+      <c r="H21" s="50" t="s">
+        <v>301</v>
+      </c>
+      <c r="I21" s="76" t="s">
         <v>302</v>
       </c>
-      <c r="H21" s="50" t="s">
-        <v>303</v>
-      </c>
-      <c r="I21" s="76" t="s">
-        <v>304</v>
-      </c>
       <c r="J21" s="76" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K21" s="76" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L21" s="76"/>
       <c r="M21" s="50"/>
@@ -55573,31 +55660,31 @@
         <v>186</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D22" s="50" t="s">
+        <v>303</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>304</v>
+      </c>
+      <c r="F22" s="50" t="s">
+        <v>304</v>
+      </c>
+      <c r="G22" s="50" t="s">
         <v>305</v>
       </c>
-      <c r="E22" s="50" t="s">
+      <c r="H22" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="F22" s="50" t="s">
-        <v>306</v>
-      </c>
-      <c r="G22" s="50" t="s">
+      <c r="I22" s="76" t="s">
         <v>307</v>
       </c>
-      <c r="H22" s="50" t="s">
+      <c r="J22" s="76" t="s">
         <v>308</v>
       </c>
-      <c r="I22" s="76" t="s">
+      <c r="K22" s="76" t="s">
         <v>309</v>
-      </c>
-      <c r="J22" s="76" t="s">
-        <v>310</v>
-      </c>
-      <c r="K22" s="76" t="s">
-        <v>311</v>
       </c>
       <c r="L22" s="76"/>
       <c r="M22" s="50"/>
@@ -55683,31 +55770,31 @@
         <v>195</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D26" s="50" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F26" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G26" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I26" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J26" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K26" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L26" s="50"/>
       <c r="M26" s="50"/>
@@ -55724,31 +55811,31 @@
         <v>197</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D27" s="50" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E27" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F27" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G27" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I27" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J27" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K27" s="50" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L27" s="50"/>
       <c r="M27" s="50"/>
@@ -57300,16 +57387,16 @@
         <v>64</v>
       </c>
       <c r="D1" s="65" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>390</v>
+      </c>
+      <c r="F1" s="65" t="s">
+        <v>392</v>
+      </c>
+      <c r="G1" s="65" t="s">
         <v>391</v>
-      </c>
-      <c r="E1" s="65" t="s">
-        <v>392</v>
-      </c>
-      <c r="F1" s="65" t="s">
-        <v>394</v>
-      </c>
-      <c r="G1" s="65" t="s">
-        <v>393</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>114</v>
@@ -57318,16 +57405,16 @@
         <v>118</v>
       </c>
       <c r="J1" s="65" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K1" s="65" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="L1" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M1" s="95" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
@@ -57401,7 +57488,7 @@
         <v>36</v>
       </c>
       <c r="M3" s="64" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
@@ -57413,16 +57500,16 @@
         <v>64</v>
       </c>
       <c r="D4" s="65" t="s">
+        <v>389</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>390</v>
+      </c>
+      <c r="F4" s="65" t="s">
+        <v>392</v>
+      </c>
+      <c r="G4" s="65" t="s">
         <v>391</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>392</v>
-      </c>
-      <c r="F4" s="65" t="s">
-        <v>394</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>393</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>114</v>
@@ -57431,50 +57518,50 @@
         <v>118</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K4" s="65" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="L4" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M4" s="95" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="241"/>
       <c r="B5" s="241"/>
       <c r="C5" s="210" t="s">
+        <v>402</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>395</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>396</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>397</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>398</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>399</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>400</v>
+      </c>
+      <c r="J5" s="56" t="s">
+        <v>316</v>
+      </c>
+      <c r="K5" s="228" t="s">
+        <v>405</v>
+      </c>
+      <c r="L5" s="228" t="s">
         <v>404</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>397</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>398</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>399</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>400</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>401</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>402</v>
-      </c>
-      <c r="J5" s="56" t="s">
-        <v>318</v>
-      </c>
-      <c r="K5" s="228" t="s">
-        <v>407</v>
-      </c>
-      <c r="L5" s="228" t="s">
-        <v>406</v>
       </c>
       <c r="M5" s="56"/>
     </row>
@@ -57520,16 +57607,16 @@
         <v>149</v>
       </c>
       <c r="C8" s="69" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D8" s="69" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E8" s="69" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F8" s="69" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>20</v>
@@ -57541,10 +57628,10 @@
         <v>75</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>75</v>
@@ -59231,7 +59318,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59248,84 +59335,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D1" s="57" t="s">
+        <v>321</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>322</v>
+      </c>
+      <c r="F1" s="57" t="s">
         <v>323</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="G1" s="57" t="s">
         <v>324</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="H1" s="57" t="s">
         <v>325</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="I1" s="57" t="s">
         <v>326</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="J1" s="57" t="s">
         <v>327</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="L1" s="57" t="s">
         <v>329</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="M1" s="57" t="s">
         <v>330</v>
-      </c>
-      <c r="L1" s="57" t="s">
-        <v>331</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="226" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B2" s="176" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C2" s="176" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D2" s="83" t="s">
+        <v>331</v>
+      </c>
+      <c r="E2" s="226" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="83" t="s">
         <v>333</v>
       </c>
-      <c r="E2" s="226" t="s">
+      <c r="G2" s="83" t="s">
         <v>334</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="H2" s="83" t="s">
         <v>335</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="I2" s="83" t="s">
         <v>336</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="J2" s="83" t="s">
         <v>337</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="K2" s="83" t="s">
         <v>338</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="L2" s="83" t="s">
         <v>339</v>
       </c>
-      <c r="K2" s="83" t="s">
+      <c r="M2" s="83" t="s">
         <v>340</v>
-      </c>
-      <c r="L2" s="83" t="s">
-        <v>341</v>
-      </c>
-      <c r="M2" s="83" t="s">
-        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -59335,6 +59422,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -59551,27 +59658,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -59588,23 +59694,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1st test of boost working
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613A7D38-0920-4209-AF37-23A68DE7820C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844A086E-2E1A-4926-AD00-442410A89978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44002,6 +44002,7 @@
         <sz val="11"/>
         <color rgb="FFFF3399"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Run_startup
@@ -44014,16 +44015,18 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>0xFE_0x00</t>
@@ -44033,6 +44036,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "Select page 0"
@@ -44043,6 +44047,7 @@
         <sz val="11"/>
         <color rgb="FF4472C4"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>0xB0_0x00</t>
@@ -44052,6 +44057,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "en 1 bst low"
@@ -44062,6 +44068,7 @@
         <sz val="11"/>
         <color rgb="FF4472C4"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>0xB1_0x00</t>
@@ -44071,6 +44078,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "en 2 bst low"
@@ -44081,6 +44089,7 @@
         <sz val="11"/>
         <color rgb="FF4472C4"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>0xB3[4:3]_0x00</t>
@@ -44090,6 +44099,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "en 3 bst low"
@@ -44100,16 +44110,18 @@
         <sz val="11"/>
         <color rgb="FFFF3399"/>
         <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -44120,6 +44132,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "Select page 1"
@@ -44130,6 +44143,7 @@
         <sz val="11"/>
         <color rgb="FF4472C4"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>0x1A_0x00</t>
@@ -44139,6 +44153,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "TSW_Mirr test"
@@ -44149,6 +44164,7 @@
         <sz val="11"/>
         <color rgb="FF4472C4"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>0x18[6]_0x01</t>
@@ -44158,6 +44174,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "Enable Mirr"
@@ -44168,6 +44185,7 @@
         <sz val="11"/>
         <color rgb="FF4472C4"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>0x17[6]_0x01</t>
@@ -44177,6 +44195,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "Force Mirr"
@@ -44197,6 +44216,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -44207,6 +44227,7 @@
         <sz val="11"/>
         <color rgb="FF7030A0"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Wait__delay__0.1ms
@@ -44217,16 +44238,18 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>0x19[1]_0x01</t>
@@ -44236,6 +44259,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "bst_test_en 1"
@@ -44246,6 +44270,7 @@
         <sz val="11"/>
         <color rgb="FF7030A0"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Wait__delay__0.1ms
@@ -44256,6 +44281,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -44266,6 +44292,7 @@
         <sz val="11"/>
         <color rgb="FF70AD47"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Measure__Current__SDWN</t>
@@ -44275,6 +44302,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "tswitch mirr measure"
@@ -44285,6 +44313,7 @@
         <sz val="11"/>
         <color rgb="FF4472C4"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">0x1A_0x00
@@ -44296,6 +44325,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -46044,6 +46074,9 @@
     <xf numFmtId="3" fontId="116" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="117" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -46073,9 +46106,6 @@
     </xf>
     <xf numFmtId="3" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="117" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -46399,7 +46429,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46677,7 +46707,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
@@ -47560,8 +47590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A58BE6-10B8-478E-A3FE-3CA6A691AC11}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47573,10 +47603,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>384</v>
       </c>
-      <c r="B1" s="233"/>
+      <c r="B1" s="234"/>
       <c r="C1" s="9" t="s">
         <v>142</v>
       </c>
@@ -47607,10 +47637,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="233" t="s">
+      <c r="A3" s="234" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="233"/>
+      <c r="B3" s="234"/>
       <c r="C3" s="15" t="s">
         <v>60</v>
       </c>
@@ -47625,10 +47655,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="233" t="s">
+      <c r="A4" s="234" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="233"/>
+      <c r="B4" s="234"/>
       <c r="C4" s="9" t="s">
         <v>142</v>
       </c>
@@ -47643,8 +47673,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="234"/>
-      <c r="B5" s="235"/>
+      <c r="A5" s="235"/>
+      <c r="B5" s="236"/>
       <c r="C5" s="206" t="s">
         <v>418</v>
       </c>
@@ -47659,7 +47689,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -47675,7 +47705,7 @@
       <c r="F6" s="67"/>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="236"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -47687,7 +47717,7 @@
       <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="236"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -47703,7 +47733,7 @@
       <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="236"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="12" t="s">
         <v>151</v>
       </c>
@@ -47715,7 +47745,7 @@
       <c r="F9" s="71"/>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="236"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="14" t="s">
         <v>152</v>
       </c>
@@ -48643,10 +48673,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="233"/>
+      <c r="B1" s="234"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -48677,10 +48707,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="233" t="s">
+      <c r="A3" s="234" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="233"/>
+      <c r="B3" s="234"/>
       <c r="C3" s="15" t="s">
         <v>79</v>
       </c>
@@ -48695,10 +48725,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="233" t="s">
+      <c r="A4" s="234" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="233"/>
+      <c r="B4" s="234"/>
       <c r="C4" s="9" t="s">
         <v>200</v>
       </c>
@@ -48713,8 +48743,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="273" x14ac:dyDescent="0.25">
-      <c r="A5" s="234"/>
-      <c r="B5" s="235"/>
+      <c r="A5" s="235"/>
+      <c r="B5" s="236"/>
       <c r="C5" s="37" t="s">
         <v>204</v>
       </c>
@@ -48729,7 +48759,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="238" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48747,7 +48777,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="237"/>
+      <c r="A7" s="238"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48763,7 +48793,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="237"/>
+      <c r="A8" s="238"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -48781,7 +48811,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="237"/>
+      <c r="A9" s="238"/>
       <c r="B9" s="12" t="s">
         <v>151</v>
       </c>
@@ -48797,7 +48827,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="237"/>
+      <c r="A10" s="238"/>
       <c r="B10" s="14" t="s">
         <v>152</v>
       </c>
@@ -49570,10 +49600,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="233" t="s">
+      <c r="A1" s="234" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="233"/>
+      <c r="B1" s="234"/>
       <c r="C1" s="103" t="s">
         <v>211</v>
       </c>
@@ -49602,10 +49632,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="233" t="s">
+      <c r="A3" s="234" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="233"/>
+      <c r="B3" s="234"/>
       <c r="C3" s="102" t="s">
         <v>20</v>
       </c>
@@ -49620,10 +49650,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="233" t="s">
+      <c r="A4" s="234" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="233"/>
+      <c r="B4" s="234"/>
       <c r="C4" s="103" t="s">
         <v>211</v>
       </c>
@@ -49638,8 +49668,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="234"/>
-      <c r="B5" s="235"/>
+      <c r="A5" s="235"/>
+      <c r="B5" s="236"/>
       <c r="C5" s="209" t="s">
         <v>214</v>
       </c>
@@ -49654,7 +49684,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="238" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -49668,7 +49698,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="237"/>
+      <c r="A7" s="238"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -49678,7 +49708,7 @@
       <c r="F7" s="130"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="237"/>
+      <c r="A8" s="238"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -49696,7 +49726,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="237"/>
+      <c r="A9" s="238"/>
       <c r="B9" s="12" t="s">
         <v>151</v>
       </c>
@@ -49708,7 +49738,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="237"/>
+      <c r="A10" s="238"/>
       <c r="B10" s="14" t="s">
         <v>152</v>
       </c>
@@ -50609,9 +50639,9 @@
   </sheetPr>
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D5" sqref="D5"/>
+      <selection pane="topRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50628,10 +50658,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="239" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="238"/>
+      <c r="B1" s="239"/>
       <c r="C1" s="65" t="s">
         <v>19</v>
       </c>
@@ -50686,7 +50716,7 @@
       <c r="T1" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="U1" s="243" t="s">
+      <c r="U1" s="233" t="s">
         <v>138</v>
       </c>
       <c r="V1" s="65" t="s">
@@ -50798,10 +50828,10 @@
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="239" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="238"/>
+      <c r="B3" s="239"/>
       <c r="C3" s="184" t="s">
         <v>20</v>
       </c>
@@ -50885,10 +50915,10 @@
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="238" t="s">
+      <c r="A4" s="239" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="238"/>
+      <c r="B4" s="239"/>
       <c r="C4" s="65" t="s">
         <v>19</v>
       </c>
@@ -50972,9 +51002,9 @@
       </c>
     </row>
     <row r="5" spans="1:29" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="239"/>
-      <c r="B5" s="239"/>
-      <c r="C5" s="223" t="s">
+      <c r="A5" s="240"/>
+      <c r="B5" s="240"/>
+      <c r="C5" s="244" t="s">
         <v>433</v>
       </c>
       <c r="D5" s="223" t="s">
@@ -51052,12 +51082,12 @@
       <c r="AB5" s="191" t="s">
         <v>432</v>
       </c>
-      <c r="AC5" s="244" t="s">
+      <c r="AC5" s="185" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="240" t="s">
+      <c r="A6" s="241" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -51136,7 +51166,7 @@
       <c r="AC6" s="67"/>
     </row>
     <row r="7" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="240"/>
+      <c r="A7" s="241"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -51171,7 +51201,7 @@
       <c r="AC7" s="68"/>
     </row>
     <row r="8" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="240"/>
+      <c r="A8" s="241"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -51224,7 +51254,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="240"/>
+      <c r="A9" s="241"/>
       <c r="B9" s="62" t="s">
         <v>151</v>
       </c>
@@ -51303,7 +51333,7 @@
       <c r="AC9" s="71"/>
     </row>
     <row r="10" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="240"/>
+      <c r="A10" s="241"/>
       <c r="B10" s="60" t="s">
         <v>152</v>
       </c>
@@ -54845,10 +54875,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="239" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="238"/>
+      <c r="B1" s="239"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -54943,10 +54973,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="239" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="238"/>
+      <c r="B3" s="239"/>
       <c r="C3" s="15" t="s">
         <v>99</v>
       </c>
@@ -54994,10 +55024,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="238" t="s">
+      <c r="A4" s="239" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="238"/>
+      <c r="B4" s="239"/>
       <c r="C4" s="65" t="s">
         <v>262</v>
       </c>
@@ -55045,8 +55075,8 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="241"/>
-      <c r="B5" s="242"/>
+      <c r="A5" s="242"/>
+      <c r="B5" s="243"/>
       <c r="C5" s="221" t="s">
         <v>277</v>
       </c>
@@ -55094,7 +55124,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="240" t="s">
+      <c r="A6" s="241" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -55117,7 +55147,7 @@
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="240"/>
+      <c r="A7" s="241"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -55138,7 +55168,7 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="240"/>
+      <c r="A8" s="241"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -55183,7 +55213,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="240"/>
+      <c r="A9" s="241"/>
       <c r="B9" s="62" t="s">
         <v>151</v>
       </c>
@@ -55208,7 +55238,7 @@
       <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="240"/>
+      <c r="A10" s="241"/>
       <c r="B10" s="60" t="s">
         <v>152</v>
       </c>
@@ -57379,10 +57409,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="239" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="238"/>
+      <c r="B1" s="239"/>
       <c r="C1" s="65" t="s">
         <v>64</v>
       </c>
@@ -57453,10 +57483,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="238" t="s">
+      <c r="A3" s="239" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="238"/>
+      <c r="B3" s="239"/>
       <c r="C3" s="64" t="s">
         <v>65</v>
       </c>
@@ -57492,10 +57522,10 @@
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A4" s="238" t="s">
+      <c r="A4" s="239" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="238"/>
+      <c r="B4" s="239"/>
       <c r="C4" s="65" t="s">
         <v>64</v>
       </c>
@@ -57531,8 +57561,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="241"/>
-      <c r="B5" s="241"/>
+      <c r="A5" s="242"/>
+      <c r="B5" s="242"/>
       <c r="C5" s="210" t="s">
         <v>402</v>
       </c>
@@ -57566,7 +57596,7 @@
       <c r="M5" s="56"/>
     </row>
     <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="240" t="s">
+      <c r="A6" s="241" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -57585,7 +57615,7 @@
       <c r="M6" s="67"/>
     </row>
     <row r="7" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="240"/>
+      <c r="A7" s="241"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -57602,7 +57632,7 @@
       <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="240"/>
+      <c r="A8" s="241"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -57639,7 +57669,7 @@
       <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="240"/>
+      <c r="A9" s="241"/>
       <c r="B9" s="62" t="s">
         <v>151</v>
       </c>
@@ -57656,7 +57686,7 @@
       <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="240"/>
+      <c r="A10" s="241"/>
       <c r="B10" s="60" t="s">
         <v>152</v>
       </c>
@@ -59318,7 +59348,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59422,26 +59452,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -59658,10 +59668,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -59678,20 +59719,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Problems with the boost tests, checking tomorrow how can going on
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844A086E-2E1A-4926-AD00-442410A89978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496287A2-1AB0-4B6B-85E1-0FE59EDEB345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="3" r:id="rId1"/>
@@ -34657,238 +34657,6 @@
     <t>Procedura per consentire la misura dell'offset in ANALOG_IN, visto che i DAC non sono abilitati di default  per applicare la parola di correzione</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Force__VBIAS__5V
-Force__VBSO__3.6V
-Force__SW__3.6V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 1 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 2 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB3[4:3]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 3 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x18[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Enable Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Bootstrap en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[1]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ls_sel off"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB4[2:0]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "hsa_hsb_byp off"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x17[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x16[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force Bootstrap"</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Run__Startup
 0xFE_0x00 "in base page"
 0x13[4]_1b1 "seq_auto_cal_dis=1 disable authomatic calibration"
@@ -35293,60 +35061,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F_0x88
-0x10_0x08
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">FORCE__SDWN__OPEN
-0x19_0x81 "Enable reference analog test"
-0x1A_0x00
-</t>
-    </r>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -37768,19 +37482,6 @@
   </si>
   <si>
     <t>0.542</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run__Startup
-Run__Enable_Ana_Testpoint
-0xFE_0x01 "Select page 1"
-0x1A_0x04 "TSDN"
-0xB0_0x0E
-"Loop__trim:"
-Trim__ 0xB3[7:5] "Select code which sets ATEST voltage as close as possible to target"
-Measure__Voltage__SDWN
-Calculate__MinError
-0xFE_0x00 "Select page 0"
-</t>
   </si>
   <si>
     <t>Run__DAC-PA_PDM_12MHz_IN
@@ -37899,19 +37600,6 @@
     <t>825k</t>
   </si>
   <si>
-    <t xml:space="preserve">Run__Startup
-Run__Enable_Ana_Testpoint
-0xFE_0x01 "Select page 1"
-0xB0_0x0E
-0x1A_0x01 "Bandgap"
-"Loop__trim:"
-Trim__0xB0[7:4] "Select code which sets ATEST voltage as close as possible to target"
-Measure__Voltage__SDWN
-Calculate__MinError
-0xFE_0x00 "Select page 0"
-</t>
-  </si>
-  <si>
     <t>400n</t>
   </si>
   <si>
@@ -37997,543 +37685,6 @@
 Measure__current__VDDIO
 Measure__current__VDD
 Measure__current__VBAT
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run_startup
-Run_Boost_test_default
-Run_Enable_Ana_Testpoint
-Force__VBIAS__5V
-Force__VBSO__3.6V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 1 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 2 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB3[4:3]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 3 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x18[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Enable Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Bootstrap en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[1]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ls_sel off"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB4[2:0]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "hsa_hsb_byp off"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x17[6]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x16[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force Bootstrap"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1A_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "TSwitch SW"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ls_sel on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Power Force en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst_test en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Force_Current__SW__400mA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>chiedere comando corrente</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__SDWN
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1A_0x02</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "TSwitch PGND"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__SDWN
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__parameter__diff__TSwitch SW__TSwitch PGND
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x00
-0x19_0x00
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
 </t>
     </r>
   </si>
@@ -44002,31 +43153,269 @@
         <sz val="11"/>
         <color rgb="FFFF3399"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Run_startup
 Run_Boost_test_default
 Run_Enable_Ana_Testpoint
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+Force__VBIAS__5V
+Force__VBSO__3.6V
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB0_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 1 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 2 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB3[4:3]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 3 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x18[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Enable Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Bootstrap en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[1]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "ls_sel off"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB4[2:0]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "hsa_hsb_byp off"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x17[6]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x16[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force Bootstrap"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1A_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "TSwitch SW"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t>0xFE_0x00</t>
@@ -44036,7 +43425,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> "Select page 0"
@@ -44047,62 +43435,95 @@
         <sz val="11"/>
         <color rgb="FF4472C4"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 1 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 2 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB3[4:3]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 3 bst low"
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "ls_sel on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[0]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Power Force en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "bst_test en"
 </t>
     </r>
     <r>
@@ -44110,116 +43531,36 @@
         <sz val="11"/>
         <color rgb="FFFF3399"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1A_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "TSW_Mirr test"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x18[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Enable Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x17[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Force__SDWN__0.6V</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+        <scheme val="minor"/>
+      </rPr>
+      <t>Force_Current__SW__400mA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>chiedere comando corrente</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"
 </t>
     </r>
     <r>
@@ -44227,7 +43568,6 @@
         <sz val="11"/>
         <color rgb="FF7030A0"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Wait__delay__0.1ms
@@ -44238,50 +43578,6 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst_test_en 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
@@ -44292,28 +43588,75 @@
         <sz val="11"/>
         <color rgb="FF70AD47"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Current__SDWN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "tswitch mirr measure"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__SDWN
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1A_0x02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "TSwitch PGND"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__SDWN
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__parameter__diff__TSwitch SW__TSwitch PGND
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">0x1A_0x00
@@ -44325,12 +43668,648 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
+      <t xml:space="preserve">Run_startup
+Run_Boost_test_default
+Run_Enable_Ana_Testpoint
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB0_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 1 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 2 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB3[4:3]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 3 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1A_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "TSW_Mirr test"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x18[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Enable Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x17[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Force__SDWN__0.6V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "bst_test_en 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Current__SDWN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "tswitch mirr measure"
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F_0x88
+0x10_0x08
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">FORCE__SDWN__OPEN
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19_0x80</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Force__VBIAS__5V
+Force__VBSO__3.6V
+Force__SW__3.6V
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB0_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 1 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 2 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB3[4:3]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 3 bst low"
+0xFE_0x01 "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x18[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Enable Mirr"
+0xFE_0x00 "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Bootstrap en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[1]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "ls_sel off"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB4[2:0]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "hsa_hsb_byp off"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x17[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x16[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force Bootstrap"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Run__Startup
+Run__Enable_Ana_Testpoint
+0xFE_0x01 "Select page 1"
+0xB0_0x0E
+0x19_0x81
+0x1A_0x01 "Bandgap"
+"Loop__trim:"
+Trim__0xB0[7:4] "Select code which sets ATEST voltage as close as possible to target"
+Measure__Voltage__SDWN
+Calculate__MinError
+0xFE_0x00 "Select page 0"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run__Startup
+Run__Enable_Ana_Testpoint
+0xFE_0x01 "Select page 1"
+0xB0_0x0E
+0x19_0x81
+0x1A_0x04 "TSDN"
+"Loop__trim:"
+Trim__ 0xB3[7:5] "Select code which sets ATEST voltage as close as possible to target"
+Measure__Voltage__SDWN
+Calculate__MinError
+0xFE_0x00 "Select page 0"
+</t>
   </si>
 </sst>
 </file>
@@ -44341,7 +44320,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="118" x14ac:knownFonts="1">
+  <fonts count="119" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45096,6 +45075,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -45488,7 +45474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="245">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -46110,6 +46096,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -46524,177 +46513,177 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>341</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
+        <v>342</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>343</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>350</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="G6" s="23" t="s">
         <v>351</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="24" t="s">
         <v>352</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="J6" s="25" t="s">
         <v>353</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="K6" s="58" t="s">
         <v>354</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="58" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="23" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>360</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>361</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="J9" s="25" t="s">
         <v>362</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="J10" s="25" t="s">
         <v>364</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="J11" s="25" t="s">
         <v>366</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>368</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
+        <v>369</v>
+      </c>
+      <c r="J13" s="25" t="s">
         <v>370</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="J14" s="25" t="s">
         <v>372</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="J15" s="25" t="s">
         <v>374</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="J16" s="25" t="s">
         <v>376</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="J17" s="25" t="s">
         <v>378</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="J18" s="25" t="s">
         <v>380</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -47590,7 +47579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A58BE6-10B8-478E-A3FE-3CA6A691AC11}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -47604,7 +47593,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="234" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B1" s="234"/>
       <c r="C1" s="9" t="s">
@@ -47676,16 +47665,16 @@
       <c r="A5" s="235"/>
       <c r="B5" s="236"/>
       <c r="C5" s="206" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="D5" s="206" t="s">
-        <v>407</v>
+        <v>433</v>
       </c>
       <c r="E5" s="206" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F5" s="191" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
@@ -47700,7 +47689,7 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F6" s="67"/>
     </row>
@@ -47725,10 +47714,10 @@
         <v>208</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="F8" s="69"/>
     </row>
@@ -47754,7 +47743,7 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="231" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F10" s="68"/>
     </row>
@@ -49608,7 +49597,7 @@
         <v>211</v>
       </c>
       <c r="D1" s="116" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E1" s="227" t="s">
         <v>212</v>
@@ -49658,7 +49647,7 @@
         <v>211</v>
       </c>
       <c r="D4" s="116" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E4" s="103" t="s">
         <v>212</v>
@@ -49674,10 +49663,10 @@
         <v>214</v>
       </c>
       <c r="D5" s="218" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E5" s="209" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F5" s="220" t="s">
         <v>215</v>
@@ -49713,7 +49702,7 @@
         <v>149</v>
       </c>
       <c r="C8" s="106" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D8" s="119" t="s">
         <v>216</v>
@@ -50639,7 +50628,7 @@
   </sheetPr>
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C5" sqref="C5"/>
     </sheetView>
@@ -51005,40 +50994,40 @@
       <c r="A5" s="240"/>
       <c r="B5" s="240"/>
       <c r="C5" s="244" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D5" s="223" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="E5" s="223" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="F5" s="223" t="s">
         <v>231</v>
       </c>
       <c r="G5" s="185" t="s">
+        <v>418</v>
+      </c>
+      <c r="H5" s="191" t="s">
+        <v>419</v>
+      </c>
+      <c r="I5" s="190" t="s">
+        <v>420</v>
+      </c>
+      <c r="J5" s="190" t="s">
+        <v>421</v>
+      </c>
+      <c r="K5" s="190" t="s">
+        <v>422</v>
+      </c>
+      <c r="L5" s="223" t="s">
         <v>423</v>
       </c>
-      <c r="H5" s="191" t="s">
+      <c r="M5" s="223" t="s">
         <v>424</v>
       </c>
-      <c r="I5" s="190" t="s">
+      <c r="N5" s="223" t="s">
         <v>425</v>
-      </c>
-      <c r="J5" s="190" t="s">
-        <v>426</v>
-      </c>
-      <c r="K5" s="190" t="s">
-        <v>427</v>
-      </c>
-      <c r="L5" s="223" t="s">
-        <v>428</v>
-      </c>
-      <c r="M5" s="223" t="s">
-        <v>429</v>
-      </c>
-      <c r="N5" s="223" t="s">
-        <v>430</v>
       </c>
       <c r="O5" s="223" t="s">
         <v>232</v>
@@ -51077,10 +51066,10 @@
         <v>243</v>
       </c>
       <c r="AA5" s="191" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="AB5" s="191" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="AC5" s="185" t="s">
         <v>244</v>
@@ -51206,7 +51195,7 @@
         <v>149</v>
       </c>
       <c r="C8" s="69" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D8" s="69" t="s">
         <v>245</v>
@@ -55084,28 +55073,28 @@
         <v>278</v>
       </c>
       <c r="E5" s="205" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F5" s="205" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="G5" s="205" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H5" s="205" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="I5" s="205" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="J5" s="205" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="K5" s="205" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="L5" s="205" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="M5" s="204" t="s">
         <v>279</v>
@@ -57417,16 +57406,16 @@
         <v>64</v>
       </c>
       <c r="D1" s="65" t="s">
+        <v>387</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>388</v>
+      </c>
+      <c r="F1" s="65" t="s">
+        <v>390</v>
+      </c>
+      <c r="G1" s="65" t="s">
         <v>389</v>
-      </c>
-      <c r="E1" s="65" t="s">
-        <v>390</v>
-      </c>
-      <c r="F1" s="65" t="s">
-        <v>392</v>
-      </c>
-      <c r="G1" s="65" t="s">
-        <v>391</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>114</v>
@@ -57530,16 +57519,16 @@
         <v>64</v>
       </c>
       <c r="D4" s="65" t="s">
+        <v>387</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>388</v>
+      </c>
+      <c r="F4" s="65" t="s">
+        <v>390</v>
+      </c>
+      <c r="G4" s="65" t="s">
         <v>389</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>390</v>
-      </c>
-      <c r="F4" s="65" t="s">
-        <v>392</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>391</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>114</v>
@@ -57564,34 +57553,34 @@
       <c r="A5" s="242"/>
       <c r="B5" s="242"/>
       <c r="C5" s="210" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D5" s="37" t="s">
+        <v>393</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>394</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>395</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="G5" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="H5" s="37" t="s">
         <v>397</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="I5" s="37" t="s">
         <v>398</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>399</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>400</v>
       </c>
       <c r="J5" s="56" t="s">
         <v>316</v>
       </c>
       <c r="K5" s="228" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L5" s="228" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="M5" s="56"/>
     </row>
@@ -59348,7 +59337,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59371,7 +59360,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D1" s="57" t="s">
         <v>321</v>
@@ -59406,43 +59395,43 @@
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="226" t="s">
-        <v>382</v>
-      </c>
-      <c r="B2" s="176" t="s">
-        <v>383</v>
+        <v>381</v>
+      </c>
+      <c r="B2" s="245" t="s">
+        <v>430</v>
       </c>
       <c r="C2" s="176" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D2" s="83" t="s">
         <v>331</v>
       </c>
       <c r="E2" s="226" t="s">
+        <v>431</v>
+      </c>
+      <c r="F2" s="83" t="s">
         <v>332</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="G2" s="83" t="s">
         <v>333</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="H2" s="83" t="s">
         <v>334</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="I2" s="83" t="s">
         <v>335</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="J2" s="83" t="s">
         <v>336</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="K2" s="83" t="s">
         <v>337</v>
       </c>
-      <c r="K2" s="83" t="s">
+      <c r="L2" s="83" t="s">
         <v>338</v>
       </c>
-      <c r="L2" s="83" t="s">
+      <c r="M2" s="83" t="s">
         <v>339</v>
-      </c>
-      <c r="M2" s="83" t="s">
-        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -59452,6 +59441,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -59668,27 +59677,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -59705,23 +59713,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update boost classe, added a function for the calculation of RON
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A0218E-AA6E-479E-BC72-6A53D55AC79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AEAAAF-F6FF-4994-AB26-40B28902F2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,6 +25,7 @@
     <sheet name="Keywords" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42614,533 +42615,6 @@
         <sz val="11"/>
         <color rgb="FFFF3399"/>
         <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Run_startup
-Run_Boost_test_default
-Run_Enable_Ana_Testpoint
-Force__VBIAS__5V
-Force__VBSO__3.6V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 1 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 2 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB3[4:3]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 3 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x18[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Enable Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Bootstrap en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[1]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ls_sel off"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB4[2:0]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "hsa_hsb_byp off"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x17[6]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x16[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force Bootstrap"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1A_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "TSwitch SW"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ls_sel on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Power Force en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst_test en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Force_Current__SW__400mA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>chiedere comando corrente</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__SDWN
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1A_0x02</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "TSwitch PGND"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__SDWN
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__parameter__diff__TSwitch SW__TSwitch PGND
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x1A_0x00
-0x19_0x00
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -44072,7 +43546,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> "Force Mirr"
+      <t xml:space="preserve"> "Force Mirr" 
 </t>
     </r>
     <r>
@@ -44345,12 +43819,22 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculate__TSswitch2__VBSO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FF70AD47"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Measure__parameter__diff__TSwitch SW__VBSO
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -44364,6 +43848,564 @@
       <t xml:space="preserve">
 0x1A_0x00
 0x19_0x00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run_startup
+Run_Boost_test_default
+Run_Enable_Ana_Testpoint
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB0_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 1 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 2 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB3[4:3]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "en 3 bst low"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x18[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Enable Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB1[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Bootstrap en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[1]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "ls_sel off"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB4[2:0]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "hsa_hsb_byp off"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x17[6]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force Mirr"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x16[6]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force Bootstrap"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1A_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "TSwitch SW"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "ls_sel on"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[0]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Power Force en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "bst_test en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Force__SW__400mA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>chiedere comando corrente</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__SDWN
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1A_0x02</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "TSwitch PGND"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__SDWN
+Calculate__TSwitchSW1__TSwitchPGND
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x1A_0x00
+0x19_0x00
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
     </r>
   </si>
 </sst>
@@ -44375,7 +44417,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="121" x14ac:knownFonts="1">
+  <fonts count="122" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45147,6 +45189,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -47744,10 +47793,10 @@
       <c r="A5" s="237"/>
       <c r="B5" s="238"/>
       <c r="C5" s="206" t="s">
+        <v>430</v>
+      </c>
+      <c r="D5" s="206" t="s">
         <v>431</v>
-      </c>
-      <c r="D5" s="206" t="s">
-        <v>432</v>
       </c>
       <c r="E5" s="206" t="s">
         <v>411</v>
@@ -50709,7 +50758,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E5" sqref="E5"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51073,13 +51122,13 @@
       <c r="A5" s="242"/>
       <c r="B5" s="242"/>
       <c r="C5" s="185" t="s">
-        <v>428</v>
-      </c>
-      <c r="D5" s="223" t="s">
         <v>427</v>
       </c>
-      <c r="E5" s="246" t="s">
+      <c r="D5" s="246" t="s">
         <v>433</v>
+      </c>
+      <c r="E5" s="185" t="s">
+        <v>432</v>
       </c>
       <c r="F5" s="223" t="s">
         <v>231</v>
@@ -51150,7 +51199,7 @@
       <c r="AB5" s="191" t="s">
         <v>426</v>
       </c>
-      <c r="AC5" s="185" t="s">
+      <c r="AC5" s="223" t="s">
         <v>244</v>
       </c>
     </row>
@@ -54922,8 +54971,8 @@
   </sheetPr>
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57457,8 +57506,8 @@
   </sheetPr>
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59415,7 +59464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853352DE-922C-4F00-B110-569410679C0C}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -59477,7 +59526,7 @@
         <v>381</v>
       </c>
       <c r="B2" s="234" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C2" s="176" t="s">
         <v>392</v>
@@ -59486,7 +59535,7 @@
         <v>331</v>
       </c>
       <c r="E2" s="226" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F2" s="83" t="s">
         <v>332</v>
@@ -59520,26 +59569,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -59756,10 +59785,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -59776,20 +59836,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added function on dft_syntaaxparser, extract_calculation_instruction
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AEAAAF-F6FF-4994-AB26-40B28902F2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047F5664-940B-47AC-87D4-1CD386F1DA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,6 @@
     <sheet name="Keywords" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50758,7 +50757,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D5" sqref="D5"/>
+      <selection pane="topRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51124,10 +51123,10 @@
       <c r="C5" s="185" t="s">
         <v>427</v>
       </c>
-      <c r="D5" s="246" t="s">
+      <c r="D5" s="185" t="s">
         <v>433</v>
       </c>
-      <c r="E5" s="185" t="s">
+      <c r="E5" s="246" t="s">
         <v>432</v>
       </c>
       <c r="F5" s="223" t="s">
@@ -59569,6 +59568,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -59785,27 +59804,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -59822,23 +59840,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated the boost class, ron ls and hs working
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047F5664-940B-47AC-87D4-1CD386F1DA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6823F606-17BA-4B4D-845B-FECBE737CD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="434">
   <si>
     <t>Revision</t>
   </si>
@@ -26376,490 +26376,6 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Run_startup
-Force__VBIAS__5V
-Force__SW__3.6V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 1 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 2 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB3[4:3]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "en 3 bst low"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x18[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Enable Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB1[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Bootstrap en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[1]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ls_sel off"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB4[2:0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "hsa_hsb off byp on"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x17[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force Mirr"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x16[6]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force Bootstrap"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Power Force en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst_test en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Force_Current__VBSO__-100mA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sink</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__VBSO
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1A_0x00
-0x19_0x00</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">Run__startup
 Run__Boost_test_default
 Run__Enable_Ana_Testpoint
@@ -43251,6 +42767,542 @@
         <sz val="11"/>
         <color rgb="FFFF3399"/>
         <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Run_startup
+Force__VBIAS__5V
+Force__SW__3.6V
+Force__VBAT__5V
+Force__VDDIO__1.8V
+Force__VDD__1.8V
+Force__VBIAS__6V
+Force__VBSO__4.3V
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 0"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xB0_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"en 1 bst low"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xB1_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"en 2 bst low"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xB3[4:3]_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"en 3 bst low"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0x18[6]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Enable Mirr"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 0"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xB1[6]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Bootstrap en"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xB2[1]_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"ls_sel off"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xB4[2:0]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"hsa_hsb off byp on"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0x17[6]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Force Mirr"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0x16[6]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Force Bootstrap"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF8D77F9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wait__delay__0.1ms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF8D77F9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 0"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xB2[0]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Power Force en"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Select page 1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wait__delay__0.1ms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0x19[1]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"bst_test en"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wait__delay__0.1ms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF6699"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Force_Current__VBSO__-100mA "sink"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Wait__delay__0.1ms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF6699"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__VBSO
+Measure__Voltage__VBAT
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculate__diff__VBAT__VBSO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"RON_BYP divided by 100mA"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0x1A_0x00
+0x19_0x00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -43727,7 +43779,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Force_Current_SW_-100mA</t>
+      <t>Force__SW__-100mA</t>
     </r>
     <r>
       <rPr>
@@ -43774,56 +43826,35 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF70AD47"/>
+        <color rgb="FF92D050"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Measure__Voltage__SDWN
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__VBSO
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Calculate__TSswitch2__VBSO</t>
+Measure__Voltage__VBSO
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Calculate__diff__TSswitchHS__VBSO</t>
     </r>
     <r>
       <rPr>
@@ -44369,7 +44400,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Measure__Voltage__SDWN
-Calculate__TSwitchSW1__TSwitchPGND
+Calculate__diff__TSwitchLS__TSwitchPGND
 </t>
     </r>
     <r>
@@ -44416,7 +44447,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="122" x14ac:knownFonts="1">
+  <fonts count="124" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45194,7 +45225,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <color rgb="FF8D77F9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF6699"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46235,15 +46280,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00CC00"/>
+      <color rgb="FFFF6699"/>
+      <color rgb="FF8D77F9"/>
       <color rgb="FFFF3399"/>
       <color rgb="FFFF66FF"/>
       <color rgb="FFFF33CC"/>
       <color rgb="FF28CF75"/>
-      <color rgb="FF8D77F9"/>
       <color rgb="FF00D0C6"/>
       <color rgb="FF2DFFF5"/>
       <color rgb="FF00C2BA"/>
-      <color rgb="FFFDFDFD"/>
     </mruColors>
   </colors>
   <extLst>
@@ -46640,177 +46686,177 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>340</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>342</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>349</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="G6" s="23" t="s">
         <v>350</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="24" t="s">
         <v>351</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="J6" s="25" t="s">
         <v>352</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="K6" s="58" t="s">
         <v>353</v>
-      </c>
-      <c r="K6" s="58" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="58" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>359</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>360</v>
       </c>
       <c r="J8" s="25"/>
       <c r="K8" s="58"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="J9" s="25" t="s">
         <v>361</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="J10" s="25" t="s">
         <v>363</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="J11" s="25" t="s">
         <v>365</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>367</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="J13" s="25" t="s">
         <v>369</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="J14" s="25" t="s">
         <v>371</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="J15" s="25" t="s">
         <v>373</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="J16" s="25" t="s">
         <v>375</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="J17" s="25" t="s">
         <v>377</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="J18" s="25" t="s">
         <v>379</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -47720,7 +47766,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="236" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B1" s="236"/>
       <c r="C1" s="9" t="s">
@@ -47792,16 +47838,16 @@
       <c r="A5" s="237"/>
       <c r="B5" s="238"/>
       <c r="C5" s="206" t="s">
+        <v>429</v>
+      </c>
+      <c r="D5" s="206" t="s">
         <v>430</v>
       </c>
-      <c r="D5" s="206" t="s">
-        <v>431</v>
-      </c>
       <c r="E5" s="206" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F5" s="191" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
@@ -47816,7 +47862,7 @@
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F6" s="67"/>
     </row>
@@ -47841,10 +47887,10 @@
         <v>208</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F8" s="69"/>
     </row>
@@ -47870,7 +47916,7 @@
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="231" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F10" s="68"/>
     </row>
@@ -49704,7 +49750,7 @@
   <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49724,7 +49770,7 @@
         <v>211</v>
       </c>
       <c r="D1" s="116" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E1" s="227" t="s">
         <v>212</v>
@@ -49774,7 +49820,7 @@
         <v>211</v>
       </c>
       <c r="D4" s="116" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E4" s="103" t="s">
         <v>212</v>
@@ -49790,10 +49836,10 @@
         <v>214</v>
       </c>
       <c r="D5" s="218" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E5" s="209" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F5" s="220" t="s">
         <v>215</v>
@@ -49829,7 +49875,7 @@
         <v>149</v>
       </c>
       <c r="C8" s="106" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D8" s="119" t="s">
         <v>216</v>
@@ -50755,9 +50801,9 @@
   </sheetPr>
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51121,85 +51167,85 @@
       <c r="A5" s="242"/>
       <c r="B5" s="242"/>
       <c r="C5" s="185" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D5" s="185" t="s">
         <v>433</v>
       </c>
-      <c r="E5" s="246" t="s">
+      <c r="E5" s="185" t="s">
         <v>432</v>
       </c>
       <c r="F5" s="223" t="s">
+        <v>431</v>
+      </c>
+      <c r="G5" s="246" t="s">
+        <v>416</v>
+      </c>
+      <c r="H5" s="191" t="s">
+        <v>417</v>
+      </c>
+      <c r="I5" s="190" t="s">
+        <v>418</v>
+      </c>
+      <c r="J5" s="190" t="s">
+        <v>419</v>
+      </c>
+      <c r="K5" s="190" t="s">
+        <v>420</v>
+      </c>
+      <c r="L5" s="223" t="s">
+        <v>421</v>
+      </c>
+      <c r="M5" s="223" t="s">
+        <v>422</v>
+      </c>
+      <c r="N5" s="223" t="s">
+        <v>423</v>
+      </c>
+      <c r="O5" s="223" t="s">
         <v>231</v>
       </c>
-      <c r="G5" s="185" t="s">
-        <v>417</v>
-      </c>
-      <c r="H5" s="191" t="s">
-        <v>418</v>
-      </c>
-      <c r="I5" s="190" t="s">
-        <v>419</v>
-      </c>
-      <c r="J5" s="190" t="s">
-        <v>420</v>
-      </c>
-      <c r="K5" s="190" t="s">
-        <v>421</v>
-      </c>
-      <c r="L5" s="223" t="s">
-        <v>422</v>
-      </c>
-      <c r="M5" s="223" t="s">
-        <v>423</v>
-      </c>
-      <c r="N5" s="223" t="s">
+      <c r="P5" s="223" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q5" s="223" t="s">
+        <v>233</v>
+      </c>
+      <c r="R5" s="223" t="s">
+        <v>234</v>
+      </c>
+      <c r="S5" s="190" t="s">
+        <v>235</v>
+      </c>
+      <c r="T5" s="191" t="s">
+        <v>236</v>
+      </c>
+      <c r="U5" s="191" t="s">
+        <v>237</v>
+      </c>
+      <c r="V5" s="191" t="s">
+        <v>238</v>
+      </c>
+      <c r="W5" s="192" t="s">
+        <v>239</v>
+      </c>
+      <c r="X5" s="192" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y5" s="192" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z5" s="192" t="s">
+        <v>242</v>
+      </c>
+      <c r="AA5" s="191" t="s">
         <v>424</v>
       </c>
-      <c r="O5" s="223" t="s">
-        <v>232</v>
-      </c>
-      <c r="P5" s="223" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q5" s="223" t="s">
-        <v>234</v>
-      </c>
-      <c r="R5" s="223" t="s">
-        <v>235</v>
-      </c>
-      <c r="S5" s="190" t="s">
-        <v>236</v>
-      </c>
-      <c r="T5" s="191" t="s">
-        <v>237</v>
-      </c>
-      <c r="U5" s="191" t="s">
-        <v>238</v>
-      </c>
-      <c r="V5" s="191" t="s">
-        <v>239</v>
-      </c>
-      <c r="W5" s="192" t="s">
-        <v>240</v>
-      </c>
-      <c r="X5" s="192" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y5" s="192" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z5" s="192" t="s">
+      <c r="AB5" s="191" t="s">
+        <v>425</v>
+      </c>
+      <c r="AC5" s="223" t="s">
         <v>243</v>
-      </c>
-      <c r="AA5" s="191" t="s">
-        <v>425</v>
-      </c>
-      <c r="AB5" s="191" t="s">
-        <v>426</v>
-      </c>
-      <c r="AC5" s="223" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -51322,36 +51368,38 @@
         <v>149</v>
       </c>
       <c r="C8" s="69" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D8" s="69" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E8" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="69"/>
+      <c r="F8" s="69" t="s">
+        <v>44</v>
+      </c>
       <c r="G8" s="69" t="s">
+        <v>245</v>
+      </c>
+      <c r="H8" s="69" t="s">
+        <v>245</v>
+      </c>
+      <c r="I8" s="69" t="s">
+        <v>245</v>
+      </c>
+      <c r="J8" s="69" t="s">
+        <v>245</v>
+      </c>
+      <c r="K8" s="69" t="s">
         <v>246</v>
-      </c>
-      <c r="H8" s="69" t="s">
-        <v>246</v>
-      </c>
-      <c r="I8" s="69" t="s">
-        <v>246</v>
-      </c>
-      <c r="J8" s="69" t="s">
-        <v>246</v>
-      </c>
-      <c r="K8" s="69" t="s">
-        <v>247</v>
       </c>
       <c r="L8" s="69"/>
       <c r="M8" s="69"/>
       <c r="N8" s="69"/>
       <c r="O8" s="69"/>
       <c r="P8" s="69" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q8" s="69"/>
       <c r="R8" s="153"/>
@@ -51366,7 +51414,7 @@
       <c r="AA8" s="69"/>
       <c r="AB8" s="69"/>
       <c r="AC8" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -51383,19 +51431,19 @@
       </c>
       <c r="F9" s="71"/>
       <c r="G9" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H9" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I9" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J9" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K9" s="71" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L9" s="71">
         <v>3</v>
@@ -51410,7 +51458,7 @@
         <v>4</v>
       </c>
       <c r="P9" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="Q9" s="70">
         <v>1.64</v>
@@ -51420,16 +51468,16 @@
       </c>
       <c r="S9" s="142"/>
       <c r="T9" s="166" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="U9" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="V9" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="W9" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="X9" s="198">
         <v>20.074999999999999</v>
@@ -51438,13 +51486,13 @@
         <v>24.2</v>
       </c>
       <c r="Z9" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AA9" s="39" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AB9" s="39" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AC9" s="71"/>
     </row>
@@ -51492,10 +51540,10 @@
         <v>218</v>
       </c>
       <c r="D11" s="72" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E11" s="72" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F11" s="72"/>
       <c r="G11" s="72" t="s">
@@ -51563,7 +51611,7 @@
         <v>155</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -51701,10 +51749,10 @@
         <v>163</v>
       </c>
       <c r="D14" s="86" t="s">
+        <v>251</v>
+      </c>
+      <c r="E14" s="86" t="s">
         <v>252</v>
-      </c>
-      <c r="E14" s="86" t="s">
-        <v>253</v>
       </c>
       <c r="F14" s="85" t="s">
         <v>163</v>
@@ -51767,7 +51815,7 @@
         <v>163</v>
       </c>
       <c r="AB14" s="84" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AC14" s="85" t="s">
         <v>163</v>
@@ -52117,7 +52165,7 @@
       <c r="N20" s="85"/>
       <c r="O20" s="85"/>
       <c r="P20" s="85" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q20" s="85"/>
       <c r="R20" s="155"/>
@@ -52236,7 +52284,7 @@
         <v>191</v>
       </c>
       <c r="F23" s="98" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G23" s="84" t="s">
         <v>163</v>
@@ -52278,7 +52326,7 @@
         <v>163</v>
       </c>
       <c r="T23" s="170" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="U23" s="84" t="s">
         <v>163</v>
@@ -52365,10 +52413,10 @@
         <v>191</v>
       </c>
       <c r="T24" s="168" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U24" s="85" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="V24" s="85" t="s">
         <v>191</v>
@@ -52460,11 +52508,11 @@
       <c r="Y26" s="85"/>
       <c r="Z26" s="85"/>
       <c r="AA26" s="84" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AB26" s="84"/>
       <c r="AC26" s="84" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:29" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -52499,7 +52547,7 @@
       <c r="Y27" s="85"/>
       <c r="Z27" s="85"/>
       <c r="AA27" s="84" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AB27" s="85"/>
       <c r="AC27" s="85"/>
@@ -55145,98 +55193,98 @@
       </c>
       <c r="B4" s="241"/>
       <c r="C4" s="65" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="65" t="s">
         <v>265</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="H4" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="90" t="s">
         <v>267</v>
       </c>
-      <c r="I4" s="90" t="s">
+      <c r="J4" s="90" t="s">
         <v>268</v>
       </c>
-      <c r="J4" s="90" t="s">
+      <c r="K4" s="90" t="s">
         <v>269</v>
       </c>
-      <c r="K4" s="90" t="s">
+      <c r="L4" s="93" t="s">
         <v>270</v>
       </c>
-      <c r="L4" s="93" t="s">
+      <c r="M4" s="93" t="s">
         <v>271</v>
       </c>
-      <c r="M4" s="93" t="s">
+      <c r="N4" s="93" t="s">
         <v>272</v>
       </c>
-      <c r="N4" s="93" t="s">
+      <c r="O4" s="93" t="s">
         <v>273</v>
       </c>
-      <c r="O4" s="93" t="s">
+      <c r="P4" s="93" t="s">
         <v>274</v>
       </c>
-      <c r="P4" s="93" t="s">
+      <c r="Q4" s="93" t="s">
         <v>275</v>
-      </c>
-      <c r="Q4" s="93" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="244"/>
       <c r="B5" s="245"/>
       <c r="C5" s="221" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" s="222" t="s">
         <v>277</v>
       </c>
-      <c r="D5" s="222" t="s">
+      <c r="E5" s="205" t="s">
+        <v>409</v>
+      </c>
+      <c r="F5" s="205" t="s">
+        <v>415</v>
+      </c>
+      <c r="G5" s="205" t="s">
+        <v>408</v>
+      </c>
+      <c r="H5" s="205" t="s">
+        <v>407</v>
+      </c>
+      <c r="I5" s="205" t="s">
+        <v>406</v>
+      </c>
+      <c r="J5" s="205" t="s">
+        <v>405</v>
+      </c>
+      <c r="K5" s="205" t="s">
+        <v>404</v>
+      </c>
+      <c r="L5" s="205" t="s">
+        <v>400</v>
+      </c>
+      <c r="M5" s="204" t="s">
         <v>278</v>
       </c>
-      <c r="E5" s="205" t="s">
-        <v>410</v>
-      </c>
-      <c r="F5" s="205" t="s">
-        <v>416</v>
-      </c>
-      <c r="G5" s="205" t="s">
-        <v>409</v>
-      </c>
-      <c r="H5" s="205" t="s">
-        <v>408</v>
-      </c>
-      <c r="I5" s="205" t="s">
-        <v>407</v>
-      </c>
-      <c r="J5" s="205" t="s">
-        <v>406</v>
-      </c>
-      <c r="K5" s="205" t="s">
-        <v>405</v>
-      </c>
-      <c r="L5" s="205" t="s">
-        <v>401</v>
-      </c>
-      <c r="M5" s="204" t="s">
+      <c r="N5" s="204" t="s">
         <v>279</v>
       </c>
-      <c r="N5" s="204" t="s">
+      <c r="O5" s="204" t="s">
         <v>280</v>
       </c>
-      <c r="O5" s="204" t="s">
+      <c r="P5" s="204" t="s">
         <v>281</v>
       </c>
-      <c r="P5" s="204" t="s">
+      <c r="Q5" s="204" t="s">
         <v>282</v>
-      </c>
-      <c r="Q5" s="204" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -55291,41 +55339,41 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="N8" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="O8" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>288</v>
-      </c>
-      <c r="Q8" s="11" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -55337,7 +55385,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E9" s="71"/>
       <c r="F9" s="71"/>
@@ -55380,47 +55428,47 @@
         <v>154</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>292</v>
-      </c>
       <c r="G11" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P11" s="5" t="s">
         <v>155</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -55740,13 +55788,13 @@
       </c>
       <c r="C20" s="50"/>
       <c r="D20" s="50" t="s">
+        <v>294</v>
+      </c>
+      <c r="E20" s="50" t="s">
         <v>295</v>
       </c>
-      <c r="E20" s="50" t="s">
-        <v>296</v>
-      </c>
       <c r="F20" s="50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G20" s="89"/>
       <c r="I20" s="76"/>
@@ -55767,29 +55815,29 @@
         <v>184</v>
       </c>
       <c r="C21" s="50" t="s">
+        <v>296</v>
+      </c>
+      <c r="D21" s="50" t="s">
         <v>297</v>
       </c>
-      <c r="D21" s="50" t="s">
+      <c r="E21" s="50" t="s">
         <v>298</v>
-      </c>
-      <c r="E21" s="50" t="s">
-        <v>299</v>
       </c>
       <c r="F21" s="50"/>
       <c r="G21" s="50" t="s">
+        <v>299</v>
+      </c>
+      <c r="H21" s="50" t="s">
         <v>300</v>
       </c>
-      <c r="H21" s="50" t="s">
+      <c r="I21" s="76" t="s">
         <v>301</v>
       </c>
-      <c r="I21" s="76" t="s">
-        <v>302</v>
-      </c>
       <c r="J21" s="76" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K21" s="76" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L21" s="76"/>
       <c r="M21" s="50"/>
@@ -55806,31 +55854,31 @@
         <v>186</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D22" s="50" t="s">
+        <v>302</v>
+      </c>
+      <c r="E22" s="50" t="s">
         <v>303</v>
       </c>
-      <c r="E22" s="50" t="s">
+      <c r="F22" s="50" t="s">
+        <v>303</v>
+      </c>
+      <c r="G22" s="50" t="s">
         <v>304</v>
       </c>
-      <c r="F22" s="50" t="s">
-        <v>304</v>
-      </c>
-      <c r="G22" s="50" t="s">
+      <c r="H22" s="50" t="s">
         <v>305</v>
       </c>
-      <c r="H22" s="50" t="s">
+      <c r="I22" s="76" t="s">
         <v>306</v>
       </c>
-      <c r="I22" s="76" t="s">
+      <c r="J22" s="76" t="s">
         <v>307</v>
       </c>
-      <c r="J22" s="76" t="s">
+      <c r="K22" s="76" t="s">
         <v>308</v>
-      </c>
-      <c r="K22" s="76" t="s">
-        <v>309</v>
       </c>
       <c r="L22" s="76"/>
       <c r="M22" s="50"/>
@@ -55916,31 +55964,31 @@
         <v>195</v>
       </c>
       <c r="C26" s="50" t="s">
+        <v>309</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>309</v>
+      </c>
+      <c r="E26" s="50" t="s">
         <v>310</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="F26" s="50" t="s">
         <v>310</v>
       </c>
-      <c r="E26" s="50" t="s">
-        <v>311</v>
-      </c>
-      <c r="F26" s="50" t="s">
-        <v>311</v>
-      </c>
       <c r="G26" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H26" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I26" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J26" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K26" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L26" s="50"/>
       <c r="M26" s="50"/>
@@ -55957,31 +56005,31 @@
         <v>197</v>
       </c>
       <c r="C27" s="50" t="s">
+        <v>309</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>309</v>
+      </c>
+      <c r="E27" s="50" t="s">
         <v>310</v>
       </c>
-      <c r="D27" s="50" t="s">
+      <c r="F27" s="50" t="s">
         <v>310</v>
       </c>
-      <c r="E27" s="50" t="s">
-        <v>311</v>
-      </c>
-      <c r="F27" s="50" t="s">
-        <v>311</v>
-      </c>
       <c r="G27" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H27" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I27" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J27" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K27" s="50" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L27" s="50"/>
       <c r="M27" s="50"/>
@@ -57533,16 +57581,16 @@
         <v>64</v>
       </c>
       <c r="D1" s="65" t="s">
+        <v>386</v>
+      </c>
+      <c r="E1" s="65" t="s">
         <v>387</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="F1" s="65" t="s">
+        <v>389</v>
+      </c>
+      <c r="G1" s="65" t="s">
         <v>388</v>
-      </c>
-      <c r="F1" s="65" t="s">
-        <v>390</v>
-      </c>
-      <c r="G1" s="65" t="s">
-        <v>389</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>114</v>
@@ -57551,16 +57599,16 @@
         <v>118</v>
       </c>
       <c r="J1" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="K1" s="65" t="s">
         <v>313</v>
-      </c>
-      <c r="K1" s="65" t="s">
-        <v>314</v>
       </c>
       <c r="L1" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M1" s="95" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.35">
@@ -57634,7 +57682,7 @@
         <v>36</v>
       </c>
       <c r="M3" s="64" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
@@ -57646,16 +57694,16 @@
         <v>64</v>
       </c>
       <c r="D4" s="65" t="s">
+        <v>386</v>
+      </c>
+      <c r="E4" s="65" t="s">
         <v>387</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="F4" s="65" t="s">
+        <v>389</v>
+      </c>
+      <c r="G4" s="65" t="s">
         <v>388</v>
-      </c>
-      <c r="F4" s="65" t="s">
-        <v>390</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>389</v>
       </c>
       <c r="H4" s="65" t="s">
         <v>114</v>
@@ -57664,50 +57712,50 @@
         <v>118</v>
       </c>
       <c r="J4" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="K4" s="65" t="s">
         <v>313</v>
-      </c>
-      <c r="K4" s="65" t="s">
-        <v>314</v>
       </c>
       <c r="L4" s="65" t="s">
         <v>122</v>
       </c>
       <c r="M4" s="95" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="244"/>
       <c r="B5" s="244"/>
       <c r="C5" s="210" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D5" s="37" t="s">
+        <v>392</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>393</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="F5" s="37" t="s">
         <v>394</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="G5" s="37" t="s">
         <v>395</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="H5" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="I5" s="37" t="s">
         <v>397</v>
       </c>
-      <c r="I5" s="37" t="s">
-        <v>398</v>
-      </c>
       <c r="J5" s="56" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K5" s="228" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L5" s="228" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M5" s="56"/>
     </row>
@@ -57753,16 +57801,16 @@
         <v>149</v>
       </c>
       <c r="C8" s="69" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D8" s="69" t="s">
+        <v>316</v>
+      </c>
+      <c r="E8" s="69" t="s">
         <v>317</v>
       </c>
-      <c r="E8" s="69" t="s">
-        <v>318</v>
-      </c>
       <c r="F8" s="69" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>20</v>
@@ -57774,10 +57822,10 @@
         <v>75</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L8" s="11" t="s">
         <v>75</v>
@@ -59481,84 +59529,84 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="57" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B1" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D1" s="57" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1" s="57" t="s">
         <v>321</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="F1" s="57" t="s">
         <v>322</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="G1" s="57" t="s">
         <v>323</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="H1" s="57" t="s">
         <v>324</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="I1" s="57" t="s">
         <v>325</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="J1" s="57" t="s">
         <v>326</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>327</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="L1" s="57" t="s">
         <v>328</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="M1" s="57" t="s">
         <v>329</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="91" customFormat="1" ht="408.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="226" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B2" s="234" t="s">
+        <v>427</v>
+      </c>
+      <c r="C2" s="176" t="s">
+        <v>391</v>
+      </c>
+      <c r="D2" s="83" t="s">
+        <v>330</v>
+      </c>
+      <c r="E2" s="226" t="s">
         <v>428</v>
       </c>
-      <c r="C2" s="176" t="s">
-        <v>392</v>
-      </c>
-      <c r="D2" s="83" t="s">
+      <c r="F2" s="83" t="s">
         <v>331</v>
       </c>
-      <c r="E2" s="226" t="s">
-        <v>429</v>
-      </c>
-      <c r="F2" s="83" t="s">
+      <c r="G2" s="83" t="s">
         <v>332</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="H2" s="83" t="s">
         <v>333</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="I2" s="83" t="s">
         <v>334</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="J2" s="83" t="s">
         <v>335</v>
       </c>
-      <c r="J2" s="83" t="s">
+      <c r="K2" s="83" t="s">
         <v>336</v>
       </c>
-      <c r="K2" s="83" t="s">
+      <c r="L2" s="83" t="s">
         <v>337</v>
       </c>
-      <c r="L2" s="83" t="s">
+      <c r="M2" s="83" t="s">
         <v>338</v>
-      </c>
-      <c r="M2" s="83" t="s">
-        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added vbso to the matrix due to the rson_byp, now this test is working
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6823F606-17BA-4B4D-845B-FECBE737CD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDE4167-C2E0-44E6-94C7-8A5B54C308F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43264,7 +43264,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Calculate__diff__VBAT__VBSO</t>
+      <t>Calculate__diff__RONBYP</t>
     </r>
     <r>
       <rPr>
@@ -43854,7 +43854,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Calculate__diff__TSswitchHS__VBSO</t>
+      <t>Calculate__diff__RONHS</t>
     </r>
     <r>
       <rPr>
@@ -44400,7 +44400,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Measure__Voltage__SDWN
-Calculate__diff__TSwitchLS__TSwitchPGND
+Calculate__diff__RONLS
 </t>
     </r>
     <r>
@@ -50802,8 +50802,8 @@
   <dimension ref="A1:AC104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D5" sqref="D5"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51172,13 +51172,13 @@
       <c r="D5" s="185" t="s">
         <v>433</v>
       </c>
-      <c r="E5" s="185" t="s">
+      <c r="E5" s="246" t="s">
         <v>432</v>
       </c>
       <c r="F5" s="223" t="s">
         <v>431</v>
       </c>
-      <c r="G5" s="246" t="s">
+      <c r="G5" s="185" t="s">
         <v>416</v>
       </c>
       <c r="H5" s="191" t="s">
@@ -59616,26 +59616,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -59852,10 +59832,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -59872,20 +59883,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
The first fout tests are working fort he boost class
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDE4167-C2E0-44E6-94C7-8A5B54C308F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6EB5CD-77CE-4CCB-9F68-86FFD8C1D36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45642,7 +45642,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="119" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="247">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -46267,9 +46267,6 @@
     <xf numFmtId="3" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -50803,7 +50800,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E5" sqref="E5"/>
+      <selection pane="topRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51172,7 +51169,7 @@
       <c r="D5" s="185" t="s">
         <v>433</v>
       </c>
-      <c r="E5" s="246" t="s">
+      <c r="E5" s="185" t="s">
         <v>432</v>
       </c>
       <c r="F5" s="223" t="s">
@@ -59616,6 +59613,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -59832,27 +59849,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -59869,23 +59885,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
problems with the debugger, updated oscilloscpe library and updated BST_LS_DRIVE
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2C2FC7-2DF9-42D5-A457-9F339DA6223E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02871E0-746B-4945-B5DE-4B41D30E44DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="435">
   <si>
     <t>Revision</t>
   </si>
@@ -44437,6 +44437,9 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t>1.8</t>
   </si>
 </sst>
 </file>
@@ -50799,7 +50802,7 @@
   <dimension ref="A1:AC104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -51377,16 +51380,16 @@
         <v>44</v>
       </c>
       <c r="G8" s="69" t="s">
-        <v>245</v>
+        <v>434</v>
       </c>
       <c r="H8" s="69" t="s">
-        <v>245</v>
+        <v>434</v>
       </c>
       <c r="I8" s="69" t="s">
-        <v>245</v>
+        <v>434</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>245</v>
+        <v>434</v>
       </c>
       <c r="K8" s="69" t="s">
         <v>246</v>
@@ -51427,17 +51430,17 @@
         <v>6</v>
       </c>
       <c r="F9" s="71"/>
-      <c r="G9" s="71" t="s">
-        <v>245</v>
-      </c>
-      <c r="H9" s="71" t="s">
-        <v>245</v>
-      </c>
-      <c r="I9" s="71" t="s">
-        <v>245</v>
-      </c>
-      <c r="J9" s="71" t="s">
-        <v>245</v>
+      <c r="G9" s="71">
+        <v>1.8</v>
+      </c>
+      <c r="H9" s="71">
+        <v>1.8</v>
+      </c>
+      <c r="I9" s="71">
+        <v>1.8</v>
+      </c>
+      <c r="J9" s="71">
+        <v>1.8</v>
       </c>
       <c r="K9" s="71" t="s">
         <v>248</v>

</xml_diff>

<commit_message>
procedures bst_byp doesn't work, when enables the bypass fsyn remained to 1.8 sdi remanined to 0
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02871E0-746B-4945-B5DE-4B41D30E44DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098C3543-23A5-46C3-8CE4-46AF73F77891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50801,9 +50801,9 @@
   </sheetPr>
   <dimension ref="A1:AC104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G5" sqref="G5"/>
+      <selection pane="topRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59616,6 +59616,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -59832,27 +59852,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -59869,23 +59888,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CBF6B91-9305-4674-87E0-A56D6B941238}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add waiting time function
</commit_message>
<xml_diff>
--- a/IVM6311_Testing_scripts.xlsx
+++ b/IVM6311_Testing_scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\invlab\Documents\IVM6311ATE\IVM6311ATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4D1759-1666-4A0F-A8D1-5DFC090D1277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C02E442-669E-43D0-A8A6-A25CE6B16830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="693" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42936,6 +42936,690 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Run_startup
+Run_Boost_test_default
+Run_Enable_Ana_Testpoint
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x11_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "VREF basso così l'uscita del comparatore è 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB3[4]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "clamp bias en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xB1[5]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"err amp bias en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xB1[3]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"comp bias en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xB0[0]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"bst general en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x0F[5]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force bst bias"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x03_0x05 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"FSYN and SDI TMUX"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x04_0x11 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig test EN FSYN=db SDI=b"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x15[4]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force bst general en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[0]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Power Force en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x16[5]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force err amp bias"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x16[3]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "force comp bias"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x17[5]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"force clamp bias"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "bst_test en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Force__VBIAS__10V
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__FSYN
+Measure__Voltage_SDI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"db and b, FSYN should be 0 and SDI 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x04_0x0B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "dig test EN FSYN=outcomp"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__FSYN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"out_comp, it should be 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x11_0x0A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"VREF high so comparator output should be 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Measure__Voltage__FSYN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"out_comp, it should be 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x04_0x11 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"dig test EN FSYN=db SDI=b"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Voltage__FSYN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Voltage__SDI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"FSYN should be 0 and SDI 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Force__VBIAS__5V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x03_0x00 
+0x04_0x00
+0x19_0x00</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Run__startup
 Run__Boost_test_default
 Run__Enable_Ana_Testpoint
@@ -42978,124 +43662,126 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0xB1[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "OVP_BIAS_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[3:2]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ovp ref bias sel set to threshold +0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xB0[0]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"bst general en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x11_0x06</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "correspond to a VREF BIAS of 9.36V"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x1A_0x0D</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "TSW to VREF_OVP_BIAS"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x03_0x04</t>
-    </r>
-    <r>
-      <rPr>
+      <t>0xB1[0]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "OVP_BSO_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[5:4]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "ovp ref bso sel set to 9V"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xCA_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "correspond to a VREF BSO of 0V"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB0[0]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "bst general en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1A_0x0C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "TSW to VREF_OVP_BSO"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x03_0x07</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF3399"/>
         <rFont val="Calibri"/>
@@ -43105,18 +43791,19 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"FSYN en"
-</t>
-    </r>
-    <r>
-      <rPr>
         <b/>
         <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"FSYN en, BCLK en, SDI en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
         <color rgb="FF4472C4"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
@@ -43131,7 +43818,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> "SDI=ovp_bias"
+      <t xml:space="preserve"> "SDI=ovp_bso"
 </t>
     </r>
     <r>
@@ -43209,16 +43896,190 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">0x15[4]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force bst general en"
+      <t>0x15[4]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Force bst general en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x16[0]_0x01  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force ovp bso"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19[1]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"bst_test en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__SDWN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"threshold measure vref_ovp, it should be corresponding to the 9V threshold (0.66V)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Voltage__FSYN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "OVP_BSO output, it should be 0 since BSO 3.6V&lt;9V"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0xFE_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x13_0x80 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"clamp disable"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0x14_0x00
+0x18_0x10
+0x19_0x10
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Force__VBIAS__12V
 </t>
     </r>
     <r>
@@ -43228,7 +44089,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">Force__VBSO__11V
 </t>
     </r>
     <r>
@@ -43244,189 +44105,58 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x16[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  "Force ovp bias"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19[1]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"bst_test en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Measure__Voltage__FSYN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "OVP_BSO output, it should be 1, since we force the VBSO the discharge should be on but never dischargin VBSO"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF33CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Force__VBSO__3.6V
+Force VBIAS_5V
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF0070C0"/>
         <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19[7]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ana_tst_mode_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__SDWN </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"threshold measure vref_bias, it should be corresponding to the 9,36V"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Voltage__FSYN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "OVP_BIAS output, it should be 0 since Bias 6V&lt;9V"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Force__VBIAS__11V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Measure__Voltage__FSYN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "OVP_BIAS output, it should be 1, since we force the VBIAS the discharge should be on but never dischargin VBIAS"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Force__VBIAS__5V</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x13_0x00
+0x14_0x00
+0x18_0x00
+0x19_0x00
 </t>
     </r>
     <r>
@@ -43444,690 +44174,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Run_startup
-Run_Boost_test_default
-Run_Enable_Ana_Testpoint
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x11_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "VREF basso così l'uscita del comparatore è 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x00 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB3[4]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "clamp bias en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xB1[5]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"err amp bias en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xB1[3]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"comp bias en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xB0[0]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"bst general en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x0F[5]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force bst bias"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x03_0x05 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"FSYN and SDI TMUX"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x04_0x11 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig test EN FSYN=db SDI=b"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x15[4]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force bst general en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Power Force en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0xFE_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x16[5]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force err amp bias"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x16[3]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "force comp bias"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x17[5]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"force clamp bias"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x19[1]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst_test en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Force__VBIAS__10V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__FSYN
-Measure__Voltage_SDI </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"db and b, FSYN should be 0 and SDI 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x04_0x0B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "dig test EN FSYN=outcomp"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Measure__Voltage__FSYN </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"out_comp, it should be 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x11_0x0A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"VREF high so comparator output should be 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Measure__Voltage__FSYN </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"out_comp, it should be 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x04_0x11 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"dig test EN FSYN=db SDI=b"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Voltage__FSYN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Voltage__SDI</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"FSYN should be 0 and SDI 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Force__VBIAS__5V</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x03_0x00 
-0x04_0x00
-0x19_0x00</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Run__startup
 Run__Boost_test_default
 Run__Enable_Ana_Testpoint
@@ -44170,73 +44216,209 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0xB1[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "OVP_BSO_en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[5:4]_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "ovp ref bso sel set to 9V"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xCA_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "correspond to a VREF BSO of 0V"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB0[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "bst general en"
+      <t>0xB1[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "OVP_BIAS_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[3:2]_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "ovp ref bias sel set to threshold +0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xB0[0]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"bst general en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0xFE_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Select page 1"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x11_0x06</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "correspond to a VREF BIAS of 9.36V"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x1A_0x0D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "TSW to VREF_OVP_BIAS"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x03_0x04</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"FSYN en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x04_0x1C</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "SDI=ovp_bias"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xFE_0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Select page 0"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0xB2[0]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Power Force en"
 </t>
     </r>
     <r>
@@ -44265,68 +44447,164 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t>0x1A_0x0C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "TSW to VREF_OVP_BSO"
+      <t xml:space="preserve">0x15[4]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Force bst general en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF3399"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x16[1]_0x01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  "Force ovp bias"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x19[1]_0x01 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"bst_test en"
 </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x03_0x07</t>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x19[7]_0x01</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "ana_tst_mode_en"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Wait__delay__0.1ms
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Measure__Voltage__SDWN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"threshold measure vref_bias, it should be corresponding to the 9,36V"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF70AD47"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Measure__Voltage__FSYN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "OVP_BIAS output, it should be 0 since Bias 6V&lt;9V"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color rgb="FFFF3399"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"FSYN en, BCLK en, SDI en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x04_0x1B</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "SDI=ovp_bso"
+      <t xml:space="preserve">Force__VBIAS__11V
 </t>
     </r>
     <r>
@@ -44336,146 +44614,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 0"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xB2[0]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Power Force en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x15[4]_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Force bst general en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x16[0]_0x01  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"Force ovp bso"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x19[1]_0x01 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"bst_test en"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Wait__delay__0.1ms
+      <t xml:space="preserve">Wait__delay__0.1ms
 </t>
     </r>
     <r>
@@ -44485,99 +44624,17 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Measure__Voltage__SDWN </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"threshold measure vref_ovp, it should be corresponding to the 9V threshold (0.66V)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Measure__Voltage__FSYN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "OVP_BSO output, it should be 0 since BSO 3.6V&lt;9V"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0xFE_0x01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "Select page 1"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x13_0x80 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"clamp disable"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0x14_0x00
-0x18_0x10
-0x19_0x10
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t xml:space="preserve">
+Measure__Voltage__FSYN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "OVP_BIAS output, it should be 1, since we force the VBIAS the discharge should be on but never dischargin VBIAS"
 </t>
     </r>
     <r>
@@ -44585,9 +44642,19 @@
         <sz val="11"/>
         <color rgb="FFFF33CC"/>
         <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Force__VBIAS__12V
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Force__VBIAS__5V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -44597,74 +44664,7 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Force__VBSO__11V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wait__delay__0.1ms
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF70AD47"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Measure__Voltage__FSYN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "OVP_BSO output, it should be 1, since we force the VBSO the discharge should be on but never dischargin VBSO"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF33CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Force__VBSO__3.6V
-Force VBIAS_5V
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3399"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x13_0x00
-0x14_0x00
-0x18_0x00
-0x19_0x00
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -45875,7 +45875,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="118" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -46458,6 +46458,9 @@
     <xf numFmtId="49" fontId="118" fillId="14" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="27" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -46487,12 +46490,6 @@
     </xf>
     <xf numFmtId="3" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -47989,10 +47986,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="233" t="s">
         <v>377</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="233"/>
       <c r="C1" s="9" t="s">
         <v>142</v>
       </c>
@@ -48023,10 +48020,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="233" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="232"/>
+      <c r="B3" s="233"/>
       <c r="C3" s="15" t="s">
         <v>60</v>
       </c>
@@ -48041,10 +48038,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="232" t="s">
+      <c r="A4" s="233" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="233"/>
       <c r="C4" s="9" t="s">
         <v>142</v>
       </c>
@@ -48059,8 +48056,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="233"/>
-      <c r="B5" s="234"/>
+      <c r="A5" s="234"/>
+      <c r="B5" s="235"/>
       <c r="C5" s="204" t="s">
         <v>420</v>
       </c>
@@ -48075,7 +48072,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="235" t="s">
+      <c r="A6" s="236" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -48091,7 +48088,7 @@
       <c r="F6" s="67"/>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="235"/>
+      <c r="A7" s="236"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -48103,7 +48100,7 @@
       <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="235"/>
+      <c r="A8" s="236"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -48119,7 +48116,7 @@
       <c r="F8" s="69"/>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="235"/>
+      <c r="A9" s="236"/>
       <c r="B9" s="12" t="s">
         <v>151</v>
       </c>
@@ -48131,7 +48128,7 @@
       <c r="F9" s="71"/>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="235"/>
+      <c r="A10" s="236"/>
       <c r="B10" s="14" t="s">
         <v>152</v>
       </c>
@@ -49059,10 +49056,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="233" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="233"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -49093,10 +49090,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="233" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="232"/>
+      <c r="B3" s="233"/>
       <c r="C3" s="15" t="s">
         <v>79</v>
       </c>
@@ -49111,10 +49108,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="232" t="s">
+      <c r="A4" s="233" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="233"/>
       <c r="C4" s="9" t="s">
         <v>200</v>
       </c>
@@ -49129,8 +49126,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="273" x14ac:dyDescent="0.25">
-      <c r="A5" s="233"/>
-      <c r="B5" s="234"/>
+      <c r="A5" s="234"/>
+      <c r="B5" s="235"/>
       <c r="C5" s="37" t="s">
         <v>204</v>
       </c>
@@ -49145,7 +49142,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -49163,7 +49160,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="236"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -49179,7 +49176,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="236"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -49197,7 +49194,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="236"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="12" t="s">
         <v>151</v>
       </c>
@@ -49213,7 +49210,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="236"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="14" t="s">
         <v>152</v>
       </c>
@@ -49986,10 +49983,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="233" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="232"/>
+      <c r="B1" s="233"/>
       <c r="C1" s="103" t="s">
         <v>211</v>
       </c>
@@ -50018,10 +50015,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="233" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="232"/>
+      <c r="B3" s="233"/>
       <c r="C3" s="102" t="s">
         <v>20</v>
       </c>
@@ -50036,10 +50033,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="232" t="s">
+      <c r="A4" s="233" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="233"/>
       <c r="C4" s="103" t="s">
         <v>211</v>
       </c>
@@ -50054,8 +50051,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="233"/>
-      <c r="B5" s="234"/>
+      <c r="A5" s="234"/>
+      <c r="B5" s="235"/>
       <c r="C5" s="207" t="s">
         <v>214</v>
       </c>
@@ -50070,7 +50067,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="237" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -50084,7 +50081,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="236"/>
+      <c r="A7" s="237"/>
       <c r="B7" s="14" t="s">
         <v>147</v>
       </c>
@@ -50094,7 +50091,7 @@
       <c r="F7" s="130"/>
     </row>
     <row r="8" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="236"/>
+      <c r="A8" s="237"/>
       <c r="B8" s="10" t="s">
         <v>149</v>
       </c>
@@ -50112,7 +50109,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="236"/>
+      <c r="A9" s="237"/>
       <c r="B9" s="12" t="s">
         <v>151</v>
       </c>
@@ -50124,7 +50121,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="236"/>
+      <c r="A10" s="237"/>
       <c r="B10" s="14" t="s">
         <v>152</v>
       </c>
@@ -51026,8 +51023,8 @@
   <dimension ref="A1:AC104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U4" sqref="U4"/>
+      <pane xSplit="2" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51044,10 +51041,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="237" t="s">
+      <c r="A1" s="238" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="237"/>
+      <c r="B1" s="238"/>
       <c r="C1" s="65" t="s">
         <v>19</v>
       </c>
@@ -51099,11 +51096,11 @@
       <c r="S1" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="T1" s="116" t="s">
-        <v>55</v>
-      </c>
-      <c r="U1" s="65" t="s">
-        <v>59</v>
+      <c r="T1" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="V1" s="65" t="s">
         <v>51</v>
@@ -51214,10 +51211,10 @@
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="237" t="s">
+      <c r="A3" s="238" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="237"/>
+      <c r="B3" s="238"/>
       <c r="C3" s="182" t="s">
         <v>20</v>
       </c>
@@ -51301,10 +51298,10 @@
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="237" t="s">
+      <c r="A4" s="238" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="237"/>
+      <c r="B4" s="238"/>
       <c r="C4" s="65" t="s">
         <v>19</v>
       </c>
@@ -51388,8 +51385,8 @@
       </c>
     </row>
     <row r="5" spans="1:29" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="238"/>
-      <c r="B5" s="238"/>
+      <c r="A5" s="239"/>
+      <c r="B5" s="239"/>
       <c r="C5" s="183" t="s">
         <v>418</v>
       </c>
@@ -51412,7 +51409,7 @@
         <v>413</v>
       </c>
       <c r="J5" s="189" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K5" s="189" t="s">
         <v>430</v>
@@ -51426,7 +51423,7 @@
       <c r="N5" s="183" t="s">
         <v>428</v>
       </c>
-      <c r="O5" s="242" t="s">
+      <c r="O5" s="183" t="s">
         <v>231</v>
       </c>
       <c r="P5" s="221" t="s">
@@ -51442,10 +51439,10 @@
         <v>234</v>
       </c>
       <c r="T5" s="189" t="s">
+        <v>434</v>
+      </c>
+      <c r="U5" s="189" t="s">
         <v>435</v>
-      </c>
-      <c r="U5" s="189" t="s">
-        <v>433</v>
       </c>
       <c r="V5" s="189" t="s">
         <v>235</v>
@@ -51473,7 +51470,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="239" t="s">
+      <c r="A6" s="240" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -51552,7 +51549,7 @@
       <c r="AC6" s="67"/>
     </row>
     <row r="7" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="239"/>
+      <c r="A7" s="240"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -51587,7 +51584,7 @@
       <c r="AC7" s="68"/>
     </row>
     <row r="8" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="239"/>
+      <c r="A8" s="240"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -51643,7 +51640,9 @@
       <c r="T8" s="119" t="s">
         <v>425</v>
       </c>
-      <c r="U8" s="69"/>
+      <c r="U8" s="69" t="s">
+        <v>425</v>
+      </c>
       <c r="V8" s="69"/>
       <c r="W8" s="69"/>
       <c r="X8" s="69"/>
@@ -51656,7 +51655,7 @@
       </c>
     </row>
     <row r="9" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="239"/>
+      <c r="A9" s="240"/>
       <c r="B9" s="62" t="s">
         <v>151</v>
       </c>
@@ -51705,10 +51704,8 @@
         <v>0.9</v>
       </c>
       <c r="S9" s="142"/>
-      <c r="T9" s="243"/>
-      <c r="U9" s="71" t="s">
-        <v>242</v>
-      </c>
+      <c r="T9" s="232"/>
+      <c r="U9" s="71"/>
       <c r="V9" s="71" t="s">
         <v>242</v>
       </c>
@@ -51733,7 +51730,7 @@
       <c r="AC9" s="71"/>
     </row>
     <row r="10" spans="1:29" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="239"/>
+      <c r="A10" s="240"/>
       <c r="B10" s="60" t="s">
         <v>152</v>
       </c>
@@ -55275,10 +55272,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="237" t="s">
+      <c r="A1" s="238" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="237"/>
+      <c r="B1" s="238"/>
       <c r="C1" s="17" t="s">
         <v>138</v>
       </c>
@@ -55373,10 +55370,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="237" t="s">
+      <c r="A3" s="238" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="237"/>
+      <c r="B3" s="238"/>
       <c r="C3" s="15" t="s">
         <v>99</v>
       </c>
@@ -55424,10 +55421,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="237" t="s">
+      <c r="A4" s="238" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="237"/>
+      <c r="B4" s="238"/>
       <c r="C4" s="65" t="s">
         <v>258</v>
       </c>
@@ -55475,8 +55472,8 @@
       </c>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="240"/>
-      <c r="B5" s="241"/>
+      <c r="A5" s="241"/>
+      <c r="B5" s="242"/>
       <c r="C5" s="219" t="s">
         <v>273</v>
       </c>
@@ -55524,7 +55521,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="239" t="s">
+      <c r="A6" s="240" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -55547,7 +55544,7 @@
       <c r="Q6" s="38"/>
     </row>
     <row r="7" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="239"/>
+      <c r="A7" s="240"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -55568,7 +55565,7 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="239"/>
+      <c r="A8" s="240"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -55613,7 +55610,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="239"/>
+      <c r="A9" s="240"/>
       <c r="B9" s="62" t="s">
         <v>151</v>
       </c>
@@ -55638,7 +55635,7 @@
       <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="239"/>
+      <c r="A10" s="240"/>
       <c r="B10" s="60" t="s">
         <v>152</v>
       </c>
@@ -57809,10 +57806,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="237" t="s">
+      <c r="A1" s="238" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="237"/>
+      <c r="B1" s="238"/>
       <c r="C1" s="231" t="s">
         <v>64</v>
       </c>
@@ -57883,10 +57880,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="237" t="s">
+      <c r="A3" s="238" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="237"/>
+      <c r="B3" s="238"/>
       <c r="C3" s="64" t="s">
         <v>65</v>
       </c>
@@ -57922,10 +57919,10 @@
       </c>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="74.45" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A4" s="237" t="s">
+      <c r="A4" s="238" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="237"/>
+      <c r="B4" s="238"/>
       <c r="C4" s="65" t="s">
         <v>64</v>
       </c>
@@ -57961,8 +57958,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="240"/>
-      <c r="B5" s="240"/>
+      <c r="A5" s="241"/>
+      <c r="B5" s="241"/>
       <c r="C5" s="208" t="s">
         <v>395</v>
       </c>
@@ -57996,7 +57993,7 @@
       <c r="M5" s="56"/>
     </row>
     <row r="6" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="239" t="s">
+      <c r="A6" s="240" t="s">
         <v>145</v>
       </c>
       <c r="B6" s="59" t="s">
@@ -58015,7 +58012,7 @@
       <c r="M6" s="67"/>
     </row>
     <row r="7" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="239"/>
+      <c r="A7" s="240"/>
       <c r="B7" s="60" t="s">
         <v>147</v>
       </c>
@@ -58032,7 +58029,7 @@
       <c r="M7" s="68"/>
     </row>
     <row r="8" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="239"/>
+      <c r="A8" s="240"/>
       <c r="B8" s="61" t="s">
         <v>149</v>
       </c>
@@ -58069,7 +58066,7 @@
       <c r="M8" s="69"/>
     </row>
     <row r="9" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="239"/>
+      <c r="A9" s="240"/>
       <c r="B9" s="62" t="s">
         <v>151</v>
       </c>
@@ -58086,7 +58083,7 @@
       <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="239"/>
+      <c r="A10" s="240"/>
       <c r="B10" s="60" t="s">
         <v>152</v>
       </c>
@@ -59747,8 +59744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853352DE-922C-4F00-B110-569410679C0C}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59852,26 +59849,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C9B53A5B1F235B4EBDF9F22062DFC34D" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ad5b12d537450e73edf2af95672e184c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e658002f-fdfe-4e4b-94aa-0526ee42a8ac" xmlns:ns3="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac16958afaf1bb0d1dccad67078e8e2c" ns2:_="" ns3:_="">
     <xsd:import namespace="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
@@ -60088,10 +60065,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e658002f-fdfe-4e4b-94aa-0526ee42a8ac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
+    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -60108,20 +60116,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D0029D-E8A7-4DC9-B140-19D450DFB7E0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA99F9FA-472B-49CB-8CD8-32BE0FD0DC5E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e658002f-fdfe-4e4b-94aa-0526ee42a8ac"/>
-    <ds:schemaRef ds:uri="4ad8f8a2-17e7-49a9-8390-22f3c8f42b39"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>